<commit_message>
update snapshot 20250910; add support WLFI
</commit_message>
<xml_diff>
--- a/snapshot/huobi_por.xlsx
+++ b/snapshot/huobi_por.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiangliqiang/Repo/Tool-Node.js-VerifyAddress/snapshot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB77BD51-B1D2-0B4D-8861-26E5B17D0F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4BFD7D70-5CE1-F041-8578-C891867E606C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{CC46D7D1-6889-8648-A26E-EA8F1C64F6A4}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{61F6E2F5-AE0B-B040-B17F-BAD31E87A5D9}"/>
   </bookViews>
   <sheets>
     <sheet name="huobi_por" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="131">
   <si>
     <t>coin</t>
   </si>
@@ -67,16 +67,13 @@
     <t>HTX(ALL)</t>
   </si>
   <si>
-    <t>282051619467149.00</t>
-  </si>
-  <si>
     <t>HTX-ERC20</t>
   </si>
   <si>
     <t>HTX-TRC20</t>
   </si>
   <si>
-    <t>281401688846504.00</t>
+    <t>281357035978733.00</t>
   </si>
   <si>
     <t>SOL(All)</t>
@@ -115,6 +112,12 @@
     <t>USDT-aEthUSDT</t>
   </si>
   <si>
+    <t>WLFI(All)</t>
+  </si>
+  <si>
+    <t>WLFI</t>
+  </si>
+  <si>
     <t>XRP(All)</t>
   </si>
   <si>
@@ -151,123 +154,114 @@
     <t>IDxEvxbNOXY2KeARpazYGHu4ZPPx+/LJpG+dItGV1GFNZoR5+sVekMFAf2ICYE0CwULl9PDejDl8aM6fnGheCFM=</t>
   </si>
   <si>
-    <t>12AxQ3mM2rwY2mwLa5qNVY65uHoQGfvSVF</t>
-  </si>
-  <si>
-    <t>1AQLXAB6aXSVbRMjbhSBudLf1kcsbWSEjg</t>
+    <t>3EpyhpDRu2wz5LtS4sPAmXaGozuxYWdRkN</t>
+  </si>
+  <si>
+    <t>TDToUxX8sH4z6moQpK3ZLAN24eupu2ivA4</t>
+  </si>
+  <si>
+    <t>8fa14929f7d46128d4b0b89fde15396ff1f322f516b10677c523d1e9b9b52a027f85234f880aacb806631d6f2102e5947408415f2d5531d81924215964c78c8c01</t>
+  </si>
+  <si>
+    <t>TK86Qm97uM848dMk8G7xNbJB7zG1uW3h1n</t>
+  </si>
+  <si>
+    <t>0x18709e89bd403f470088abdacebe86cc60dda12e</t>
+  </si>
+  <si>
+    <t>0x68a79a40adfb16777e49206d60f9cd11de0fbaf3acad5be1e30dd955182475f43255dfec5fede4dc97fcf1fbce1583dd05ee419bf3939ca95919aff931eec41d01</t>
+  </si>
+  <si>
+    <t>TYh6mgoMNZTCsgpYHBz7gttEfrQmDMABub</t>
+  </si>
+  <si>
+    <t>24d160af1f9f0c4ff530f85f6ed0850927727a7a4a576918d1d502c2af3eb4227417b1527e5eb5aae09529935d0662b5775d5f67db06d46ac34ee7e127c1582901</t>
+  </si>
+  <si>
+    <t>TKgD8Qnx9Zw3DNvG6o83PkufnMbtEXis4T</t>
+  </si>
+  <si>
+    <t>1acfc19531231fd17c1f28d0f3534a00afcbca453773d8840cd75a3d0ef51ee66a995f4149c4ddc5f713e13511ca2c242da9826b4d83c3730364d866f406e0cd01</t>
+  </si>
+  <si>
+    <t>TGn1uvntAVntT1pG8o7qoKkbViiYfeg6Gj</t>
+  </si>
+  <si>
+    <t>1d67ec16daee2603e595999693e2d4cec89207ba16fae4cf9d373edbcd362d5260468b7e57ac8205a9b6bf4cfca6cbd820173d4a4001422e3ce519ca2ced8cbf01</t>
+  </si>
+  <si>
+    <t>TAuUCiH4JVNBZmDnEDZkXEUXDARdGpXTmX</t>
+  </si>
+  <si>
+    <t>5982075dacfacbb88888b6e3cb44eb32f3d1f149a5d8587452f101964d588d58011f38d05d13fda5cedeccc8f4a7d1b7f31c4564bf6838da6d87163bd8a2bc9400</t>
+  </si>
+  <si>
+    <t>TF2fmSbg5HAD34KPUH7WtWCxxvgXHohzYM</t>
+  </si>
+  <si>
+    <t>72617d480d203e93a54d38a27361d96a761b12fa4ebf9bca61e34e720c232b3b27a6cddfca0e4fc92d5b51e9ef61d3d5a90abe39b693bb3ae5174d3a5b13e9c900</t>
+  </si>
+  <si>
+    <t>THZovMcKoZaV9zzFTWteQYd2f3NEvnzxAM</t>
+  </si>
+  <si>
+    <t>b23b3b34780d5d0a3fb62667aef5d598030660f22f508980bcb4f2fdc192f9d92307d7b73edd52c31fb057ebdb29ea18e304aac94a55c5dcd747946bfe5acc4d01</t>
+  </si>
+  <si>
+    <t>TZ1SsapyhKNWaVLca6P2qgVzkHTdk6nkXa</t>
+  </si>
+  <si>
+    <t>6a8a95f0830edb75eff19aac342c74554f9d027a925c55961cd073c7380dc7802eb1451d4041971397e3f1c330e6d412a8c51ca38e9fe10c21b3fd6c1227a21a01</t>
+  </si>
+  <si>
+    <t>TRSXRWudzfzY4jH7AaMowdMNUXDkHisbcd</t>
+  </si>
+  <si>
+    <t>2583d69f88055b1cab1905ea4f30845edd6b7bd5be58b3e9117ec1b13bfc501052872139bdb95749aa3132530757f589928f45106d7566555767952825e77ef600</t>
+  </si>
+  <si>
+    <t>TCiRCBNFrL6bFKWL94yWQi5hNMGNp1Nu27</t>
+  </si>
+  <si>
+    <t>51fbb14497b6f5265b44931dac48e23822b645598d7a9c5fee183c9a517db9491594b82a03e1dfea9072e3e95a29d5716610f5aefdbd934fab8b67d73f148d6900</t>
+  </si>
+  <si>
+    <t>0x4fb312915b779b1339388e14b6d079741ca83128</t>
+  </si>
+  <si>
+    <t>0xef72CC0Bb3EE2236b3B875C66a8A5D06b53Adb99</t>
+  </si>
+  <si>
+    <t>htx</t>
+  </si>
+  <si>
+    <t>0xc91377206d5903eff7c725d0ab54ed1a652110581e449c5ccc7f4f5bb991af80228ae4a95f448bb18a6ac78e850334daa495930b85375f3d6ab606ac0146d8b61b</t>
+  </si>
+  <si>
+    <t>0x406ea8F3C6464171f3dEccF6Ba99748D9487CD52</t>
+  </si>
+  <si>
+    <t>0x3ba1542404430b5818a403ab451e4ee2299a0b9e8c2d71f178edf0e2c4df222a77ac3dd16011369cc395063da048e975620ddc6e511f762ad639640ca8d4fac31c</t>
+  </si>
+  <si>
+    <t>0x3f95d25BfB08e6cF5bA3e159e477D28852BA3F04</t>
+  </si>
+  <si>
+    <t>0xc766bb36b671096e668bd902515eecef9939bcd99226bb668768f7d3a2cc5387339c98d0d8f21a3f3ec27024ccfeb5034d617a4d6021cab5538f061f198808d31b</t>
+  </si>
+  <si>
+    <t>0x9EC19cE75a7557d52c32774779158F5A466e0080</t>
+  </si>
+  <si>
+    <t>0x0d929c70239b715b65f891088a5143e21449c36cab4243f71e5ce84317454c6605013fad579dc198c43798e2a9e7d575a9c39fc67689a2b4e38635e2e934ef661c</t>
+  </si>
+  <si>
+    <t>0xa03400e098f4421b34a3a44a1b4e571419517687</t>
   </si>
   <si>
     <t>King will be back!</t>
   </si>
   <si>
-    <t>H1JDQp1uGjVNXcXdpUUUnbiRS1YyttPeo8btOTuA86tXLEIWrVeoNlZsjufIBkfR/f5wqxklyHg1wnNY3cHqIrw=</t>
-  </si>
-  <si>
-    <t>3EpyhpDRu2wz5LtS4sPAmXaGozuxYWdRkN</t>
-  </si>
-  <si>
-    <t>TDToUxX8sH4z6moQpK3ZLAN24eupu2ivA4</t>
-  </si>
-  <si>
-    <t>8fa14929f7d46128d4b0b89fde15396ff1f322f516b10677c523d1e9b9b52a027f85234f880aacb806631d6f2102e5947408415f2d5531d81924215964c78c8c01</t>
-  </si>
-  <si>
-    <t>TK86Qm97uM848dMk8G7xNbJB7zG1uW3h1n</t>
-  </si>
-  <si>
-    <t>0x18709e89bd403f470088abdacebe86cc60dda12e</t>
-  </si>
-  <si>
-    <t>0x68a79a40adfb16777e49206d60f9cd11de0fbaf3acad5be1e30dd955182475f43255dfec5fede4dc97fcf1fbce1583dd05ee419bf3939ca95919aff931eec41d01</t>
-  </si>
-  <si>
-    <t>TYh6mgoMNZTCsgpYHBz7gttEfrQmDMABub</t>
-  </si>
-  <si>
-    <t>24d160af1f9f0c4ff530f85f6ed0850927727a7a4a576918d1d502c2af3eb4227417b1527e5eb5aae09529935d0662b5775d5f67db06d46ac34ee7e127c1582901</t>
-  </si>
-  <si>
-    <t>TKgD8Qnx9Zw3DNvG6o83PkufnMbtEXis4T</t>
-  </si>
-  <si>
-    <t>1acfc19531231fd17c1f28d0f3534a00afcbca453773d8840cd75a3d0ef51ee66a995f4149c4ddc5f713e13511ca2c242da9826b4d83c3730364d866f406e0cd01</t>
-  </si>
-  <si>
-    <t>TGn1uvntAVntT1pG8o7qoKkbViiYfeg6Gj</t>
-  </si>
-  <si>
-    <t>1d67ec16daee2603e595999693e2d4cec89207ba16fae4cf9d373edbcd362d5260468b7e57ac8205a9b6bf4cfca6cbd820173d4a4001422e3ce519ca2ced8cbf01</t>
-  </si>
-  <si>
-    <t>TAuUCiH4JVNBZmDnEDZkXEUXDARdGpXTmX</t>
-  </si>
-  <si>
-    <t>5982075dacfacbb88888b6e3cb44eb32f3d1f149a5d8587452f101964d588d58011f38d05d13fda5cedeccc8f4a7d1b7f31c4564bf6838da6d87163bd8a2bc9400</t>
-  </si>
-  <si>
-    <t>TF2fmSbg5HAD34KPUH7WtWCxxvgXHohzYM</t>
-  </si>
-  <si>
-    <t>72617d480d203e93a54d38a27361d96a761b12fa4ebf9bca61e34e720c232b3b27a6cddfca0e4fc92d5b51e9ef61d3d5a90abe39b693bb3ae5174d3a5b13e9c900</t>
-  </si>
-  <si>
-    <t>THZovMcKoZaV9zzFTWteQYd2f3NEvnzxAM</t>
-  </si>
-  <si>
-    <t>b23b3b34780d5d0a3fb62667aef5d598030660f22f508980bcb4f2fdc192f9d92307d7b73edd52c31fb057ebdb29ea18e304aac94a55c5dcd747946bfe5acc4d01</t>
-  </si>
-  <si>
-    <t>TZ1SsapyhKNWaVLca6P2qgVzkHTdk6nkXa</t>
-  </si>
-  <si>
-    <t>6a8a95f0830edb75eff19aac342c74554f9d027a925c55961cd073c7380dc7802eb1451d4041971397e3f1c330e6d412a8c51ca38e9fe10c21b3fd6c1227a21a01</t>
-  </si>
-  <si>
-    <t>TRSXRWudzfzY4jH7AaMowdMNUXDkHisbcd</t>
-  </si>
-  <si>
-    <t>2583d69f88055b1cab1905ea4f30845edd6b7bd5be58b3e9117ec1b13bfc501052872139bdb95749aa3132530757f589928f45106d7566555767952825e77ef600</t>
-  </si>
-  <si>
-    <t>TCiRCBNFrL6bFKWL94yWQi5hNMGNp1Nu27</t>
-  </si>
-  <si>
-    <t>51fbb14497b6f5265b44931dac48e23822b645598d7a9c5fee183c9a517db9491594b82a03e1dfea9072e3e95a29d5716610f5aefdbd934fab8b67d73f148d6900</t>
-  </si>
-  <si>
-    <t>0x4fb312915b779b1339388e14b6d079741ca83128</t>
-  </si>
-  <si>
-    <t>0xef72CC0Bb3EE2236b3B875C66a8A5D06b53Adb99</t>
-  </si>
-  <si>
-    <t>htx</t>
-  </si>
-  <si>
-    <t>0xc91377206d5903eff7c725d0ab54ed1a652110581e449c5ccc7f4f5bb991af80228ae4a95f448bb18a6ac78e850334daa495930b85375f3d6ab606ac0146d8b61b</t>
-  </si>
-  <si>
-    <t>0x406ea8F3C6464171f3dEccF6Ba99748D9487CD52</t>
-  </si>
-  <si>
-    <t>0x3ba1542404430b5818a403ab451e4ee2299a0b9e8c2d71f178edf0e2c4df222a77ac3dd16011369cc395063da048e975620ddc6e511f762ad639640ca8d4fac31c</t>
-  </si>
-  <si>
-    <t>0x3f95d25BfB08e6cF5bA3e159e477D28852BA3F04</t>
-  </si>
-  <si>
-    <t>0xc766bb36b671096e668bd902515eecef9939bcd99226bb668768f7d3a2cc5387339c98d0d8f21a3f3ec27024ccfeb5034d617a4d6021cab5538f061f198808d31b</t>
-  </si>
-  <si>
-    <t>0x9EC19cE75a7557d52c32774779158F5A466e0080</t>
-  </si>
-  <si>
-    <t>0x0d929c70239b715b65f891088a5143e21449c36cab4243f71e5ce84317454c6605013fad579dc198c43798e2a9e7d575a9c39fc67689a2b4e38635e2e934ef661c</t>
-  </si>
-  <si>
-    <t>0xa03400e098f4421b34a3a44a1b4e571419517687</t>
-  </si>
-  <si>
     <t>0xc24e6ba40bb68f98b4bfcf653e3557f7accde2c539937f2f865eda96c9d48688481d49e38bc31d0450d164eac66cb3c5e0bfd9e472684bfb3d9bc3ea3a3bc82a01</t>
   </si>
   <si>
@@ -331,15 +325,9 @@
     <t>rneMKXXdKMD1R9WZ4Yqv1bfst6bjpaD5tP</t>
   </si>
   <si>
-    <t>9ztZpRN3v9xv5JhAT7MTtmy4DfyMEAG8YU</t>
-  </si>
-  <si>
     <t>DRRU8L7fF4k9w7SF3Z6ei8onPCsh9hjGX1</t>
   </si>
   <si>
-    <t>DJX3kCZfcDuREturnUNKEBQELi1PFaLkJC</t>
-  </si>
-  <si>
     <t>DHaGhSzL2HTzyHyYxLXNKzGRKmQjWRbot3</t>
   </si>
   <si>
@@ -379,34 +367,52 @@
     <t>DSqzssxy31fpuGFJfZjoM6TqP38oNPAPiN</t>
   </si>
   <si>
-    <t>DKs2WBbiaAEe9RGzQTmtJj1o9bqsKTUTtC</t>
+    <t>DLzCvKskasu4Adj3XgbyNitKBukBSa5JPP</t>
   </si>
   <si>
     <t>DB5KWytcxHyphHPn9iC92Y9JqPRL1Fq21p</t>
   </si>
   <si>
-    <t>A4vGxy18SuYts12xuj9NH7Xt6HfcqJjdpL</t>
-  </si>
-  <si>
-    <t>AEreBtLaqQWvJTcGYaXpdguh1Rhfv64MDR</t>
-  </si>
-  <si>
-    <t>A1cEKcmS2GzY7HAupW9AfHpsP8G9vXJJFD</t>
-  </si>
-  <si>
-    <t>A4v3NQryewiyYDk9G6vsFHrmVjD2pMLa95</t>
-  </si>
-  <si>
-    <t>9vaTpzdYTCFUd1vwr62vzvtPa1rquPYqVA</t>
-  </si>
-  <si>
-    <t>A77Ur7Xkx2ZVXiyZ1mUZNUJvfmK86iBW9g</t>
-  </si>
-  <si>
-    <t>9v7nQJPSgLkDh5vYGFG96vy4pbvhzHLJcX</t>
-  </si>
-  <si>
-    <t>A4JZEjPDBZxhwmM89zk7NrUWjxMVreeM3K</t>
+    <t>A7rh9YzPJvkHvmJ4CxZGLMH6za55GhHchC</t>
+  </si>
+  <si>
+    <t>A9nQnT5Q77vLVYhcMTgCTjsPuzx1B7fqxo</t>
+  </si>
+  <si>
+    <t>9zfbkebu6Cv4Jd853BXAGKnppnKqzEa8QN</t>
+  </si>
+  <si>
+    <t>9rvn4wnK25vwXECpnaZWzLPWe4i7EQVULq</t>
+  </si>
+  <si>
+    <t>9vruGagGajRTC1kFcmfeEK9z4yEYvLHUXd</t>
+  </si>
+  <si>
+    <t>9yoTs1Y8iDL3gdhmCHYeUbxBUbAfpd8UKf</t>
+  </si>
+  <si>
+    <t>AAyT52Ni4MGsYCGsAMUHQ5QNKiCkZzSaY7</t>
+  </si>
+  <si>
+    <t>A3DwCPWCEH5E2GBZ8nfiVeWPBRgvZpEHXz</t>
+  </si>
+  <si>
+    <t>A5iDSrbhUjo6jaian3FAafceyjnM5mYniK</t>
+  </si>
+  <si>
+    <t>A9VTrFUAZX2m5HNEM1BVoXh5A4ZjNgahYT</t>
+  </si>
+  <si>
+    <t>A4AB5tNJDoxaJZepa6ukvuHvwB7odp1wcV</t>
+  </si>
+  <si>
+    <t>A55jHGWNwfNChbH5Psz97xNwXSgbruwmJw</t>
+  </si>
+  <si>
+    <t>9y5Civ2PpDz84j4Lr5Vcna43ZTxUnER9f1</t>
+  </si>
+  <si>
+    <t>9uLxcGj4CZpDarfoozN6BrRo5aLv1YJuPS</t>
   </si>
 </sst>
 </file>
@@ -1410,21 +1416,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECA46CB9-41E0-0046-AEFE-2938847FA626}">
-  <dimension ref="A1:F117"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A29CAB09-E350-9A47-A01D-958BA1FF6BE9}">
+  <dimension ref="A1:F124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:F30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="24.1640625" customWidth="1"/>
-    <col min="2" max="2" width="52" customWidth="1"/>
-    <col min="3" max="3" width="20.5" customWidth="1"/>
-    <col min="4" max="4" width="21.83203125" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
-    <col min="6" max="6" width="141" customWidth="1"/>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
+    <col min="2" max="2" width="51.83203125" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" customWidth="1"/>
+    <col min="4" max="4" width="19.1640625" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="135.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1446,7 +1452,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="1">
-        <v>20181.43</v>
+        <v>20089.828020000001</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1454,10 +1460,10 @@
         <v>5</v>
       </c>
       <c r="B3" s="1">
-        <v>912570</v>
+        <v>913920</v>
       </c>
       <c r="C3" s="1">
-        <v>9543.7800000000007</v>
+        <v>9451.18</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1465,10 +1471,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="1">
-        <v>75332174</v>
+        <v>75591302</v>
       </c>
       <c r="C4" s="1">
-        <v>10225.93</v>
+        <v>10226.93</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1490,7 +1496,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="1">
-        <v>431612714.89999998</v>
+        <v>412767143.30000001</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1498,10 +1504,10 @@
         <v>9</v>
       </c>
       <c r="B7" s="1">
-        <v>5857586</v>
+        <v>55869896</v>
       </c>
       <c r="C7" s="1">
-        <v>431612714.89999998</v>
+        <v>412767143.30000001</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1512,7 +1518,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="1">
-        <v>107081.96</v>
+        <v>110282.13189999999</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1520,10 +1526,10 @@
         <v>11</v>
       </c>
       <c r="B9" s="1">
-        <v>23262182</v>
+        <v>23326594</v>
       </c>
       <c r="C9" s="1">
-        <v>6470.02</v>
+        <v>9608.7000000000007</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1531,10 +1537,10 @@
         <v>12</v>
       </c>
       <c r="B10" s="1">
-        <v>23262182</v>
+        <v>23326594</v>
       </c>
       <c r="C10" s="1">
-        <v>26344.65</v>
+        <v>26357.42</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1542,10 +1548,10 @@
         <v>13</v>
       </c>
       <c r="B11" s="1">
-        <v>23262182</v>
+        <v>23326594</v>
       </c>
       <c r="C11" s="1">
-        <v>74267.289999999994</v>
+        <v>74316.009999999995</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1555,79 +1561,79 @@
       <c r="B12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>15</v>
+      <c r="C12" s="1">
+        <v>282019861205662</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="1">
-        <v>23262182</v>
+        <v>23326594</v>
       </c>
       <c r="C13" s="1">
-        <v>649930620646.09998</v>
+        <v>662825226929.5</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1">
+        <v>75591302</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B14" s="1">
-        <v>75332174</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="1">
-        <v>293341.21999999997</v>
+        <v>284213.9877</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" s="1">
-        <v>363760458</v>
+        <v>365711359</v>
       </c>
       <c r="C16" s="1">
-        <v>293341.21999999997</v>
+        <v>284213.99</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="1">
-        <v>11113166321.92</v>
+        <v>11047203296</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" s="1">
-        <v>75332174</v>
+        <v>75591302</v>
       </c>
       <c r="C18" s="1">
-        <v>10190692515.969999</v>
+        <v>10124729489.639999</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" s="1">
         <v>75332174</v>
@@ -1638,161 +1644,143 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C20" s="1">
-        <v>1160825136.26</v>
+        <v>1404148839</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" s="1">
-        <v>75332174</v>
+        <v>75591302</v>
       </c>
       <c r="C21" s="1">
-        <v>38633584.850000001</v>
+        <v>38662662.909999996</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" s="1">
-        <v>67943213</v>
+        <v>68482953</v>
       </c>
       <c r="C22" s="1">
-        <v>476754.81</v>
+        <v>541764.97</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B23" s="1">
-        <v>23262182</v>
+        <v>23326594</v>
       </c>
       <c r="C23" s="1">
-        <v>19796237.859999999</v>
+        <v>30524528.559999999</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B24" s="1">
-        <v>75332174</v>
+        <v>75591302</v>
       </c>
       <c r="C24" s="1">
-        <v>53833783.369999997</v>
+        <v>96190257.760000005</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B25" s="1">
-        <v>75332174</v>
+        <v>75591302</v>
       </c>
       <c r="C25" s="1">
-        <v>21575194.140000001</v>
+        <v>96071462.310000002</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B26" s="1">
-        <v>23262182</v>
+        <v>23326594</v>
       </c>
       <c r="C26" s="1">
-        <v>1026509581.23</v>
+        <v>1142158162.01</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C27" s="1">
-        <v>33330018.059999999</v>
+        <v>87832784.959999993</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="1">
+        <v>23326594</v>
+      </c>
+      <c r="C28" s="1">
+        <v>87832784.959999993</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="1">
-        <v>98537381</v>
-      </c>
-      <c r="C28" s="1">
-        <v>33330018.059999999</v>
+      <c r="B29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="1">
+        <v>32624562.699999999</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="1">
+        <v>98738024</v>
+      </c>
+      <c r="C30" s="1">
+        <v>32624562.699999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C30" s="1" t="s">
+      <c r="B32" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D32" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F30" s="1" t="s">
+      <c r="E32" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B31" s="1" t="s">
+      <c r="F32" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="C31" s="1">
-        <v>912570</v>
-      </c>
-      <c r="D31" s="1">
-        <v>7130.7</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C32" s="1">
-        <v>912570</v>
-      </c>
-      <c r="D32" s="1">
-        <v>970.8</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1800,19 +1788,19 @@
         <v>5</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C33" s="1">
-        <v>912570</v>
+        <v>913920</v>
       </c>
       <c r="D33" s="1">
-        <v>829.68</v>
+        <v>7310.7</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1820,19 +1808,19 @@
         <v>5</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C34" s="1">
-        <v>912570</v>
+        <v>913920</v>
       </c>
       <c r="D34" s="1">
-        <v>80.569999999999993</v>
+        <v>970.8</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1840,19 +1828,19 @@
         <v>5</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C35" s="1">
-        <v>912570</v>
+        <v>913920</v>
       </c>
       <c r="D35" s="1">
-        <v>32.03</v>
+        <v>829.68</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1860,13 +1848,13 @@
         <v>5</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C36" s="1">
-        <v>912570</v>
+        <v>913920</v>
       </c>
       <c r="D36" s="1">
-        <v>500</v>
+        <v>340</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>4</v>
@@ -1880,19 +1868,19 @@
         <v>6</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C37" s="1">
-        <v>75332174</v>
+        <v>75591302</v>
       </c>
       <c r="D37" s="1">
         <v>10162.93</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1900,13 +1888,13 @@
         <v>6</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C38" s="1">
-        <v>75332174</v>
+        <v>75591302</v>
       </c>
       <c r="D38" s="1">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>4</v>
@@ -1920,7 +1908,7 @@
         <v>7</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C39" s="1">
         <v>23040137</v>
@@ -1929,170 +1917,170 @@
         <v>411.72</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C40" s="1">
-        <v>75332174</v>
+        <v>75591302</v>
       </c>
       <c r="D40" s="1">
-        <v>1082057894.9000001</v>
+        <v>1082058768.1300001</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C41" s="1">
-        <v>75332174</v>
+        <v>75591302</v>
       </c>
       <c r="D41" s="1">
-        <v>1126520982.9300001</v>
+        <v>1126521856.1600001</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C42" s="1">
-        <v>75332174</v>
+        <v>75591302</v>
       </c>
       <c r="D42" s="1">
-        <v>34967683.009999998</v>
+        <v>1705110564.0899999</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C43" s="1">
+        <v>75591302</v>
+      </c>
+      <c r="D43" s="1">
+        <v>1434482060.2</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F43" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="C43" s="1">
-        <v>75332174</v>
-      </c>
-      <c r="D43" s="1">
-        <v>1705110564.0899999</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C44" s="1">
+        <v>75591302</v>
+      </c>
+      <c r="D44" s="1">
+        <v>1071232018.22</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F44" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="C44" s="1">
-        <v>75332174</v>
-      </c>
-      <c r="D44" s="1">
-        <v>1465481687.3599999</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C45" s="1">
+        <v>75591302</v>
+      </c>
+      <c r="D45" s="1">
+        <v>1070373171.46</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F45" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="C45" s="1">
-        <v>75332174</v>
-      </c>
-      <c r="D45" s="1">
-        <v>1071230749.54</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" s="1">
+        <v>75591302</v>
+      </c>
+      <c r="D46" s="1">
+        <v>1064061276.29</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F46" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="C46" s="1">
-        <v>75332174</v>
-      </c>
-      <c r="D46" s="1">
-        <v>1070372776.02</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C47" s="1">
+        <v>75591302</v>
+      </c>
+      <c r="D47" s="1">
+        <v>1570889775.0799999</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F47" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="C47" s="1">
-        <v>75332174</v>
-      </c>
-      <c r="D47" s="1">
-        <v>1064060403.05</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -2100,39 +2088,39 @@
         <v>22</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C48" s="1">
         <v>75332174</v>
       </c>
       <c r="D48" s="1">
-        <v>1570889775.0799999</v>
+        <v>922473805.94000006</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C49" s="1">
-        <v>75332174</v>
+        <v>23326594</v>
       </c>
       <c r="D49" s="1">
-        <v>922473805.94000006</v>
+        <v>331.13</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -2140,13 +2128,13 @@
         <v>11</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C50" s="1">
-        <v>23262182</v>
+        <v>23326594</v>
       </c>
       <c r="D50" s="1">
-        <v>5991.1</v>
+        <v>8591.1</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>4</v>
@@ -2160,7 +2148,7 @@
         <v>11</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>4</v>
@@ -2169,10 +2157,10 @@
         <v>4</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -2180,7 +2168,7 @@
         <v>11</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>4</v>
@@ -2189,10 +2177,10 @@
         <v>4</v>
       </c>
       <c r="E52" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F52" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -2200,7 +2188,7 @@
         <v>11</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>4</v>
@@ -2209,10 +2197,10 @@
         <v>4</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -2220,7 +2208,7 @@
         <v>11</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>4</v>
@@ -2229,10 +2217,10 @@
         <v>4</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -2240,19 +2228,19 @@
         <v>11</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C55" s="1">
-        <v>23262182</v>
+        <v>23326594</v>
       </c>
       <c r="D55" s="1">
-        <v>478.92</v>
+        <v>686.47</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -2260,19 +2248,19 @@
         <v>12</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C56" s="1">
-        <v>23262182</v>
+        <v>23326594</v>
       </c>
       <c r="D56" s="1">
-        <v>26344.65</v>
+        <v>26357.42</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -2280,13 +2268,13 @@
         <v>13</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C57" s="1">
-        <v>23262182</v>
+        <v>23326594</v>
       </c>
       <c r="D57" s="1">
-        <v>33478.94</v>
+        <v>33500.9</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>4</v>
@@ -2300,70 +2288,70 @@
         <v>13</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C58" s="1">
-        <v>23262182</v>
+        <v>23326594</v>
       </c>
       <c r="D58" s="1">
-        <v>40788.36</v>
+        <v>40815.11</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C59" s="1">
-        <v>23262182</v>
+        <v>23326594</v>
       </c>
       <c r="D59" s="1">
-        <v>129619650000</v>
+        <v>142206650000</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C60" s="1">
-        <v>23262182</v>
+        <v>23326594</v>
       </c>
       <c r="D60" s="1">
-        <v>7071629008.1000004</v>
+        <v>7379235291.5</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C61" s="1">
-        <v>23262182</v>
+        <v>23326594</v>
       </c>
       <c r="D61" s="1">
         <v>513239341638</v>
@@ -2380,7 +2368,7 @@
         <v>11</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>4</v>
@@ -2389,10 +2377,10 @@
         <v>4</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -2400,7 +2388,7 @@
         <v>11</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>4</v>
@@ -2409,10 +2397,10 @@
         <v>4</v>
       </c>
       <c r="E63" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F63" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -2420,7 +2408,7 @@
         <v>11</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>4</v>
@@ -2429,10 +2417,10 @@
         <v>4</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -2440,7 +2428,7 @@
         <v>11</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>4</v>
@@ -2449,44 +2437,44 @@
         <v>4</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C66" s="1">
-        <v>75332174</v>
+        <v>75591302</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C67" s="1">
-        <v>75332174</v>
+        <v>75591302</v>
       </c>
       <c r="D67" s="1">
-        <v>594892000000</v>
+        <v>534335000000</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>4</v>
@@ -2497,36 +2485,36 @@
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C68" s="1">
-        <v>75332174</v>
+        <v>75591302</v>
       </c>
       <c r="D68" s="1">
-        <v>96474504746.75</v>
+        <v>112378636975.81</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C69" s="1">
-        <v>363760458</v>
+        <v>365711359</v>
       </c>
       <c r="D69" s="1">
-        <v>16150.97</v>
+        <v>5550.97</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>4</v>
@@ -2537,16 +2525,16 @@
     </row>
     <row r="70" spans="1:6">
       <c r="A70" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C70" s="1">
-        <v>363760458</v>
+        <v>365711359</v>
       </c>
       <c r="D70" s="1">
-        <v>1185</v>
+        <v>1786.52</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>4</v>
@@ -2557,16 +2545,16 @@
     </row>
     <row r="71" spans="1:6">
       <c r="A71" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C71" s="1">
-        <v>363760458</v>
+        <v>365711359</v>
       </c>
       <c r="D71" s="1">
-        <v>276005.25</v>
+        <v>276876.5</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>4</v>
@@ -2577,36 +2565,36 @@
     </row>
     <row r="72" spans="1:6">
       <c r="A72" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C72" s="1">
-        <v>75332174</v>
+        <v>75591302</v>
       </c>
       <c r="D72" s="1">
-        <v>38633584.850000001</v>
+        <v>38662662.909999996</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C73" s="1">
-        <v>67943213</v>
+        <v>68482953</v>
       </c>
       <c r="D73" s="1">
-        <v>476754.81</v>
+        <v>541764.97</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>4</v>
@@ -2617,76 +2605,76 @@
     </row>
     <row r="74" spans="1:6">
       <c r="A74" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C74" s="1">
-        <v>75332174</v>
+        <v>75591302</v>
       </c>
       <c r="D74" s="1">
-        <v>21575194.140000001</v>
+        <v>96071462.310000002</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C75" s="1">
-        <v>23262182</v>
+        <v>23326594</v>
       </c>
       <c r="D75" s="1">
-        <v>6023080.46</v>
+        <v>2167893.16</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C76" s="1">
-        <v>23262182</v>
+        <v>23326594</v>
       </c>
       <c r="D76" s="1">
         <v>1045412.19</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C77" s="1">
-        <v>23262182</v>
+        <v>23326594</v>
       </c>
       <c r="D77" s="1">
-        <v>12727745.210000001</v>
+        <v>27311223.210000001</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>4</v>
@@ -2700,7 +2688,7 @@
         <v>11</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>4</v>
@@ -2709,10 +2697,10 @@
         <v>4</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -2720,7 +2708,7 @@
         <v>11</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>4</v>
@@ -2729,10 +2717,10 @@
         <v>4</v>
       </c>
       <c r="E79" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F79" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -2740,7 +2728,7 @@
         <v>11</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>4</v>
@@ -2749,10 +2737,10 @@
         <v>4</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -2760,7 +2748,7 @@
         <v>11</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>4</v>
@@ -2769,24 +2757,24 @@
         <v>4</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C82" s="1">
-        <v>75332174</v>
+        <v>75591302</v>
       </c>
       <c r="D82" s="1">
-        <v>21000010</v>
+        <v>50000000</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>4</v>
@@ -2797,16 +2785,16 @@
     </row>
     <row r="83" spans="1:6">
       <c r="A83" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C83" s="1">
-        <v>75332174</v>
+        <v>75591302</v>
       </c>
       <c r="D83" s="1">
-        <v>27631400.100000001</v>
+        <v>43864485.100000001</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>4</v>
@@ -2817,10 +2805,10 @@
     </row>
     <row r="84" spans="1:6">
       <c r="A84" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>4</v>
@@ -2829,18 +2817,18 @@
         <v>4</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>4</v>
@@ -2849,18 +2837,18 @@
         <v>4</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>4</v>
@@ -2869,64 +2857,64 @@
         <v>4</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="87" spans="1:6">
       <c r="A87" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C87" s="1">
-        <v>75332174</v>
+        <v>75591302</v>
       </c>
       <c r="D87" s="1">
-        <v>5202373.2699999996</v>
+        <v>2325772.66</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="88" spans="1:6">
       <c r="A88" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C88" s="1">
-        <v>23262182</v>
+        <v>23326594</v>
       </c>
       <c r="D88" s="1">
-        <v>1026509581.23</v>
+        <v>1142158162.01</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="A89" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C89" s="1">
-        <v>98537381</v>
+        <v>98738024</v>
       </c>
       <c r="D89" s="1">
-        <v>31687852.739999998</v>
+        <v>31887852.739999998</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>4</v>
@@ -2937,16 +2925,16 @@
     </row>
     <row r="90" spans="1:6">
       <c r="A90" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C90" s="1">
-        <v>98537381</v>
+        <v>98738024</v>
       </c>
       <c r="D90" s="1">
-        <v>1485768.19</v>
+        <v>609602.18999999994</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>4</v>
@@ -2957,16 +2945,16 @@
     </row>
     <row r="91" spans="1:6">
       <c r="A91" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C91" s="1">
-        <v>98537381</v>
+        <v>98738024</v>
       </c>
       <c r="D91" s="1">
-        <v>156397.12</v>
+        <v>127107.77</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>4</v>
@@ -2977,16 +2965,16 @@
     </row>
     <row r="92" spans="1:6">
       <c r="A92" s="1" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>103</v>
+        <v>68</v>
       </c>
       <c r="C92" s="1">
-        <v>5857586</v>
+        <v>23326594</v>
       </c>
       <c r="D92" s="1">
-        <v>21977000.760000002</v>
+        <v>55000002</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>4</v>
@@ -2997,42 +2985,42 @@
     </row>
     <row r="93" spans="1:6">
       <c r="A93" s="1" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>104</v>
+        <v>48</v>
       </c>
       <c r="C93" s="1">
-        <v>5857586</v>
+        <v>23326594</v>
       </c>
       <c r="D93" s="1">
-        <v>286206111.25999999</v>
+        <v>21991000</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
     </row>
     <row r="94" spans="1:6">
       <c r="A94" s="1" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>105</v>
+        <v>78</v>
       </c>
       <c r="C94" s="1">
-        <v>5857586</v>
+        <v>23326594</v>
       </c>
       <c r="D94" s="1">
-        <v>148769.64000000001</v>
+        <v>10841782.960000001</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>4</v>
+        <v>79</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -3040,13 +3028,13 @@
         <v>9</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C95" s="1">
-        <v>5857586</v>
+        <v>5869896</v>
       </c>
       <c r="D95" s="1">
-        <v>82781244.920000002</v>
+        <v>286206111.25999999</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>4</v>
@@ -3060,13 +3048,13 @@
         <v>9</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C96" s="1">
-        <v>5857586</v>
+        <v>5869896</v>
       </c>
       <c r="D96" s="1">
-        <v>624076.68000000005</v>
+        <v>82781244.920000002</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>4</v>
@@ -3080,13 +3068,13 @@
         <v>9</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C97" s="1">
-        <v>5857586</v>
+        <v>5869896</v>
       </c>
       <c r="D97" s="1">
-        <v>4631544.88</v>
+        <v>624076.68000000005</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>4</v>
@@ -3100,13 +3088,13 @@
         <v>9</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C98" s="1">
-        <v>5857586</v>
+        <v>5869896</v>
       </c>
       <c r="D98" s="1">
-        <v>4445950.8</v>
+        <v>4631544.88</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>4</v>
@@ -3120,13 +3108,13 @@
         <v>9</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C99" s="1">
-        <v>5857586</v>
+        <v>5869896</v>
       </c>
       <c r="D99" s="1">
-        <v>2866994</v>
+        <v>4445950.8</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>4</v>
@@ -3140,13 +3128,13 @@
         <v>9</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C100" s="1">
-        <v>5857586</v>
+        <v>5869896</v>
       </c>
       <c r="D100" s="1">
-        <v>2647816.5299999998</v>
+        <v>2866994</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>4</v>
@@ -3160,13 +3148,13 @@
         <v>9</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C101" s="1">
-        <v>5857586</v>
+        <v>5869896</v>
       </c>
       <c r="D101" s="1">
-        <v>2451906.98</v>
+        <v>2647816.5299999998</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>4</v>
@@ -3180,13 +3168,13 @@
         <v>9</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C102" s="1">
-        <v>5857586</v>
+        <v>5869896</v>
       </c>
       <c r="D102" s="1">
-        <v>1457329.63</v>
+        <v>2451906.98</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>4</v>
@@ -3200,13 +3188,13 @@
         <v>9</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C103" s="1">
-        <v>5857586</v>
+        <v>5869896</v>
       </c>
       <c r="D103" s="1">
-        <v>850746.71</v>
+        <v>1457329.63</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>4</v>
@@ -3220,13 +3208,13 @@
         <v>9</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C104" s="1">
-        <v>5857586</v>
+        <v>5869896</v>
       </c>
       <c r="D104" s="1">
-        <v>285678.89</v>
+        <v>850746.71</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>4</v>
@@ -3240,13 +3228,13 @@
         <v>9</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C105" s="1">
-        <v>5857586</v>
+        <v>5869896</v>
       </c>
       <c r="D105" s="1">
-        <v>170777.71</v>
+        <v>285678.89</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>4</v>
@@ -3260,13 +3248,13 @@
         <v>9</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C106" s="1">
-        <v>5857586</v>
+        <v>5869896</v>
       </c>
       <c r="D106" s="1">
-        <v>1066964.3</v>
+        <v>170777.71</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>4</v>
@@ -3280,13 +3268,13 @@
         <v>9</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C107" s="1">
-        <v>5857586</v>
+        <v>5869896</v>
       </c>
       <c r="D107" s="1">
-        <v>538350.48</v>
+        <v>1066964.3</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>4</v>
@@ -3300,13 +3288,13 @@
         <v>9</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C108" s="1">
-        <v>5857586</v>
+        <v>5869896</v>
       </c>
       <c r="D108" s="1">
-        <v>1101043.6599999999</v>
+        <v>538350.48</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>4</v>
@@ -3320,13 +3308,13 @@
         <v>9</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C109" s="1">
-        <v>5857586</v>
+        <v>5869896</v>
       </c>
       <c r="D109" s="1">
-        <v>127419.44</v>
+        <v>120247.67</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>4</v>
@@ -3340,13 +3328,13 @@
         <v>9</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C110" s="1">
-        <v>5857586</v>
+        <v>5869896</v>
       </c>
       <c r="D110" s="1">
-        <v>5077999.0999999996</v>
+        <v>127419.44</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>4</v>
@@ -3360,13 +3348,13 @@
         <v>9</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C111" s="1">
-        <v>5857586</v>
+        <v>5869896</v>
       </c>
       <c r="D111" s="1">
-        <v>3403999.07</v>
+        <v>4030998.06</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>4</v>
@@ -3380,13 +3368,13 @@
         <v>9</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C112" s="1">
-        <v>5857586</v>
+        <v>5869896</v>
       </c>
       <c r="D112" s="1">
-        <v>2975999.14</v>
+        <v>3627998.92</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>4</v>
@@ -3400,13 +3388,13 @@
         <v>9</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C113" s="1">
-        <v>5857586</v>
+        <v>5869896</v>
       </c>
       <c r="D113" s="1">
-        <v>2723994.1</v>
+        <v>2725997.87</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>4</v>
@@ -3420,13 +3408,13 @@
         <v>9</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C114" s="1">
-        <v>5857586</v>
+        <v>5869896</v>
       </c>
       <c r="D114" s="1">
-        <v>1998999.44</v>
+        <v>2306999.81</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>4</v>
@@ -3440,13 +3428,13 @@
         <v>9</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C115" s="1">
-        <v>5857586</v>
+        <v>5869896</v>
       </c>
       <c r="D115" s="1">
-        <v>589999.29</v>
+        <v>1560993.24</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>4</v>
@@ -3460,13 +3448,13 @@
         <v>9</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C116" s="1">
-        <v>5857586</v>
+        <v>5869896</v>
       </c>
       <c r="D116" s="1">
-        <v>313998.39</v>
+        <v>1397999.81</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>4</v>
@@ -3480,18 +3468,158 @@
         <v>9</v>
       </c>
       <c r="B117" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C117" s="1">
+        <v>5869896</v>
+      </c>
+      <c r="D117" s="1">
+        <v>1192999.6299999999</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6">
+      <c r="A118" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C118" s="1">
+        <v>5869896</v>
+      </c>
+      <c r="D118" s="1">
+        <v>961999.81</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6">
+      <c r="A119" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C119" s="1">
+        <v>5869896</v>
+      </c>
+      <c r="D119" s="1">
+        <v>792999.81</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6">
+      <c r="A120" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C120" s="1">
+        <v>5869896</v>
+      </c>
+      <c r="D120" s="1">
+        <v>714999.63</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6">
+      <c r="A121" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C121" s="1">
+        <v>5869896</v>
+      </c>
+      <c r="D121" s="1">
+        <v>679999.81</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F121" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6">
+      <c r="A122" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B122" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C117" s="1">
-        <v>5857586</v>
-      </c>
-      <c r="D117" s="1">
-        <v>147999.1</v>
-      </c>
-      <c r="E117" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F117" s="1" t="s">
+      <c r="C122" s="1">
+        <v>5869896</v>
+      </c>
+      <c r="D122" s="1">
+        <v>623997.65</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6">
+      <c r="A123" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C123" s="1">
+        <v>5869896</v>
+      </c>
+      <c r="D123" s="1">
+        <v>536999.63</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F123" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6">
+      <c r="A124" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C124" s="1">
+        <v>5869896</v>
+      </c>
+      <c r="D124" s="1">
+        <v>338998.77</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F124" s="1" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update snapshot 20251001;add support USDT-XPL,ERC20-USDC,STEAK-USDC,USDC-SOL; update tools and version
</commit_message>
<xml_diff>
--- a/snapshot/huobi_por.xlsx
+++ b/snapshot/huobi_por.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiangliqiang/Repo/Tool-Node.js-VerifyAddress/snapshot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4BFD7D70-5CE1-F041-8578-C891867E606C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4BCD1C0E-D96D-F54B-BEEF-8BC36A84F83D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{61F6E2F5-AE0B-B040-B17F-BAD31E87A5D9}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{60B29559-677B-DA4D-AA00-E4410F0FEE4D}"/>
   </bookViews>
   <sheets>
     <sheet name="huobi_por" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="136">
   <si>
     <t>coin</t>
   </si>
@@ -43,9 +43,6 @@
     <t>BTC-TRC20</t>
   </si>
   <si>
-    <t>WBTC-ERC20</t>
-  </si>
-  <si>
     <t>DOGE(All)</t>
   </si>
   <si>
@@ -67,13 +64,16 @@
     <t>HTX(ALL)</t>
   </si>
   <si>
+    <t>279469118029940.00</t>
+  </si>
+  <si>
     <t>HTX-ERC20</t>
   </si>
   <si>
     <t>HTX-TRC20</t>
   </si>
   <si>
-    <t>281357035978733.00</t>
+    <t>278673247252117.00</t>
   </si>
   <si>
     <t>SOL(All)</t>
@@ -91,6 +91,18 @@
     <t>jsTRX</t>
   </si>
   <si>
+    <t>USDC(All)</t>
+  </si>
+  <si>
+    <t>ERC20-USDC</t>
+  </si>
+  <si>
+    <t>STEAK-USDC</t>
+  </si>
+  <si>
+    <t>USDC-SOL</t>
+  </si>
+  <si>
     <t>USDT(ALL)</t>
   </si>
   <si>
@@ -112,6 +124,9 @@
     <t>USDT-aEthUSDT</t>
   </si>
   <si>
+    <t>USDT-XPL</t>
+  </si>
+  <si>
     <t>WLFI(All)</t>
   </si>
   <si>
@@ -154,6 +169,15 @@
     <t>IDxEvxbNOXY2KeARpazYGHu4ZPPx+/LJpG+dItGV1GFNZoR5+sVekMFAf2ICYE0CwULl9PDejDl8aM6fnGheCFM=</t>
   </si>
   <si>
+    <t>1AQLXAB6aXSVbRMjbhSBudLf1kcsbWSEjg</t>
+  </si>
+  <si>
+    <t>King will be back!</t>
+  </si>
+  <si>
+    <t>H1JDQp1uGjVNXcXdpUUUnbiRS1YyttPeo8btOTuA86tXLEIWrVeoNlZsjufIBkfR/f5wqxklyHg1wnNY3cHqIrw=</t>
+  </si>
+  <si>
     <t>3EpyhpDRu2wz5LtS4sPAmXaGozuxYWdRkN</t>
   </si>
   <si>
@@ -166,66 +190,66 @@
     <t>TK86Qm97uM848dMk8G7xNbJB7zG1uW3h1n</t>
   </si>
   <si>
+    <t>TYh6mgoMNZTCsgpYHBz7gttEfrQmDMABub</t>
+  </si>
+  <si>
+    <t>24d160af1f9f0c4ff530f85f6ed0850927727a7a4a576918d1d502c2af3eb4227417b1527e5eb5aae09529935d0662b5775d5f67db06d46ac34ee7e127c1582901</t>
+  </si>
+  <si>
+    <t>TKgD8Qnx9Zw3DNvG6o83PkufnMbtEXis4T</t>
+  </si>
+  <si>
+    <t>1acfc19531231fd17c1f28d0f3534a00afcbca453773d8840cd75a3d0ef51ee66a995f4149c4ddc5f713e13511ca2c242da9826b4d83c3730364d866f406e0cd01</t>
+  </si>
+  <si>
+    <t>TGn1uvntAVntT1pG8o7qoKkbViiYfeg6Gj</t>
+  </si>
+  <si>
+    <t>1d67ec16daee2603e595999693e2d4cec89207ba16fae4cf9d373edbcd362d5260468b7e57ac8205a9b6bf4cfca6cbd820173d4a4001422e3ce519ca2ced8cbf01</t>
+  </si>
+  <si>
+    <t>TAuUCiH4JVNBZmDnEDZkXEUXDARdGpXTmX</t>
+  </si>
+  <si>
+    <t>5982075dacfacbb88888b6e3cb44eb32f3d1f149a5d8587452f101964d588d58011f38d05d13fda5cedeccc8f4a7d1b7f31c4564bf6838da6d87163bd8a2bc9400</t>
+  </si>
+  <si>
+    <t>TF2fmSbg5HAD34KPUH7WtWCxxvgXHohzYM</t>
+  </si>
+  <si>
+    <t>72617d480d203e93a54d38a27361d96a761b12fa4ebf9bca61e34e720c232b3b27a6cddfca0e4fc92d5b51e9ef61d3d5a90abe39b693bb3ae5174d3a5b13e9c900</t>
+  </si>
+  <si>
+    <t>THZovMcKoZaV9zzFTWteQYd2f3NEvnzxAM</t>
+  </si>
+  <si>
+    <t>b23b3b34780d5d0a3fb62667aef5d598030660f22f508980bcb4f2fdc192f9d92307d7b73edd52c31fb057ebdb29ea18e304aac94a55c5dcd747946bfe5acc4d01</t>
+  </si>
+  <si>
+    <t>TZ1SsapyhKNWaVLca6P2qgVzkHTdk6nkXa</t>
+  </si>
+  <si>
+    <t>6a8a95f0830edb75eff19aac342c74554f9d027a925c55961cd073c7380dc7802eb1451d4041971397e3f1c330e6d412a8c51ca38e9fe10c21b3fd6c1227a21a01</t>
+  </si>
+  <si>
+    <t>TRSXRWudzfzY4jH7AaMowdMNUXDkHisbcd</t>
+  </si>
+  <si>
+    <t>2583d69f88055b1cab1905ea4f30845edd6b7bd5be58b3e9117ec1b13bfc501052872139bdb95749aa3132530757f589928f45106d7566555767952825e77ef600</t>
+  </si>
+  <si>
+    <t>TCiRCBNFrL6bFKWL94yWQi5hNMGNp1Nu27</t>
+  </si>
+  <si>
+    <t>51fbb14497b6f5265b44931dac48e23822b645598d7a9c5fee183c9a517db9491594b82a03e1dfea9072e3e95a29d5716610f5aefdbd934fab8b67d73f148d6900</t>
+  </si>
+  <si>
     <t>0x18709e89bd403f470088abdacebe86cc60dda12e</t>
   </si>
   <si>
     <t>0x68a79a40adfb16777e49206d60f9cd11de0fbaf3acad5be1e30dd955182475f43255dfec5fede4dc97fcf1fbce1583dd05ee419bf3939ca95919aff931eec41d01</t>
   </si>
   <si>
-    <t>TYh6mgoMNZTCsgpYHBz7gttEfrQmDMABub</t>
-  </si>
-  <si>
-    <t>24d160af1f9f0c4ff530f85f6ed0850927727a7a4a576918d1d502c2af3eb4227417b1527e5eb5aae09529935d0662b5775d5f67db06d46ac34ee7e127c1582901</t>
-  </si>
-  <si>
-    <t>TKgD8Qnx9Zw3DNvG6o83PkufnMbtEXis4T</t>
-  </si>
-  <si>
-    <t>1acfc19531231fd17c1f28d0f3534a00afcbca453773d8840cd75a3d0ef51ee66a995f4149c4ddc5f713e13511ca2c242da9826b4d83c3730364d866f406e0cd01</t>
-  </si>
-  <si>
-    <t>TGn1uvntAVntT1pG8o7qoKkbViiYfeg6Gj</t>
-  </si>
-  <si>
-    <t>1d67ec16daee2603e595999693e2d4cec89207ba16fae4cf9d373edbcd362d5260468b7e57ac8205a9b6bf4cfca6cbd820173d4a4001422e3ce519ca2ced8cbf01</t>
-  </si>
-  <si>
-    <t>TAuUCiH4JVNBZmDnEDZkXEUXDARdGpXTmX</t>
-  </si>
-  <si>
-    <t>5982075dacfacbb88888b6e3cb44eb32f3d1f149a5d8587452f101964d588d58011f38d05d13fda5cedeccc8f4a7d1b7f31c4564bf6838da6d87163bd8a2bc9400</t>
-  </si>
-  <si>
-    <t>TF2fmSbg5HAD34KPUH7WtWCxxvgXHohzYM</t>
-  </si>
-  <si>
-    <t>72617d480d203e93a54d38a27361d96a761b12fa4ebf9bca61e34e720c232b3b27a6cddfca0e4fc92d5b51e9ef61d3d5a90abe39b693bb3ae5174d3a5b13e9c900</t>
-  </si>
-  <si>
-    <t>THZovMcKoZaV9zzFTWteQYd2f3NEvnzxAM</t>
-  </si>
-  <si>
-    <t>b23b3b34780d5d0a3fb62667aef5d598030660f22f508980bcb4f2fdc192f9d92307d7b73edd52c31fb057ebdb29ea18e304aac94a55c5dcd747946bfe5acc4d01</t>
-  </si>
-  <si>
-    <t>TZ1SsapyhKNWaVLca6P2qgVzkHTdk6nkXa</t>
-  </si>
-  <si>
-    <t>6a8a95f0830edb75eff19aac342c74554f9d027a925c55961cd073c7380dc7802eb1451d4041971397e3f1c330e6d412a8c51ca38e9fe10c21b3fd6c1227a21a01</t>
-  </si>
-  <si>
-    <t>TRSXRWudzfzY4jH7AaMowdMNUXDkHisbcd</t>
-  </si>
-  <si>
-    <t>2583d69f88055b1cab1905ea4f30845edd6b7bd5be58b3e9117ec1b13bfc501052872139bdb95749aa3132530757f589928f45106d7566555767952825e77ef600</t>
-  </si>
-  <si>
-    <t>TCiRCBNFrL6bFKWL94yWQi5hNMGNp1Nu27</t>
-  </si>
-  <si>
-    <t>51fbb14497b6f5265b44931dac48e23822b645598d7a9c5fee183c9a517db9491594b82a03e1dfea9072e3e95a29d5716610f5aefdbd934fab8b67d73f148d6900</t>
-  </si>
-  <si>
     <t>0x4fb312915b779b1339388e14b6d079741ca83128</t>
   </si>
   <si>
@@ -259,16 +283,13 @@
     <t>0xa03400e098f4421b34a3a44a1b4e571419517687</t>
   </si>
   <si>
-    <t>King will be back!</t>
-  </si>
-  <si>
     <t>0xc24e6ba40bb68f98b4bfcf653e3557f7accde2c539937f2f865eda96c9d48688481d49e38bc31d0450d164eac66cb3c5e0bfd9e472684bfb3d9bc3ea3a3bc82a01</t>
   </si>
   <si>
     <t>0x6663613fbd927ce78abbf7f5ca7e2c3fe0d96d18</t>
   </si>
   <si>
-    <t>280710322341756.00</t>
+    <t>278210322341756.00</t>
   </si>
   <si>
     <t>TFTWNgDBkQ5wQoP8RXpRznnHvAVV8x5jLu</t>
@@ -316,6 +337,9 @@
     <t>0x3ca7a1fcc5306107b4bd37c82359ec2a1c62b32658bb01201f12bf5e9e1b5c54623f440d226165bf4d216cffe5a4e3fce9e636e7514eac5c29af97df12e88fd400</t>
   </si>
   <si>
+    <t>0x18709E89BD403F470088aBDAcEbE86CC60dda12e</t>
+  </si>
+  <si>
     <t>rKUDvXFJMFu65LqPTH3Yfpii4rbKT9bSQT</t>
   </si>
   <si>
@@ -325,19 +349,13 @@
     <t>rneMKXXdKMD1R9WZ4Yqv1bfst6bjpaD5tP</t>
   </si>
   <si>
+    <t>9ztZpRN3v9xv5JhAT7MTtmy4DfyMEAG8YU</t>
+  </si>
+  <si>
     <t>DRRU8L7fF4k9w7SF3Z6ei8onPCsh9hjGX1</t>
   </si>
   <si>
-    <t>DHaGhSzL2HTzyHyYxLXNKzGRKmQjWRbot3</t>
-  </si>
-  <si>
-    <t>DAG3cZ85wuf27tYeoqYNJnxSxKUR4DkCLN</t>
-  </si>
-  <si>
-    <t>DSRwLdyRey7CaRpvwwcH4KYWAXZiDtvitF</t>
-  </si>
-  <si>
-    <t>DHfXiSgDHzsiQukDPDJRATtGKsUr3V5FeJ</t>
+    <t>DJX3kCZfcDuREturnUNKEBQELi1PFaLkJC</t>
   </si>
   <si>
     <t>DN4FUEu7L9PpcnMntidGXNvasjUEyWV77F</t>
@@ -346,19 +364,13 @@
     <t>DQ17R1yDcLRM7SdQf1ZDJDeGih89yic7Px</t>
   </si>
   <si>
-    <t>DESQdg5SAy7SQfJyXLDbFwy3gWvFpyEtEe</t>
-  </si>
-  <si>
     <t>D9wh6cJXG9wFA87svpHRHGBxFtYGJHC13h</t>
   </si>
   <si>
     <t>DQkukxxY7LYdb2bchK8Zgo14wwyEPsHVJf</t>
   </si>
   <si>
-    <t>DL7qJ42gRYJWdguLewyNmZkvX63ZanFHez</t>
-  </si>
-  <si>
-    <t>DGp23eRrNArV2R72Wnrnsyj4azyjyCytDi</t>
+    <t>DQhEuTa5UkNcD8YFZK3pvjFfrtMqQpJhSa</t>
   </si>
   <si>
     <t>DJxVuu8KDh7qKfuieJoWQNFYmK1L3k773X</t>
@@ -367,52 +379,55 @@
     <t>DSqzssxy31fpuGFJfZjoM6TqP38oNPAPiN</t>
   </si>
   <si>
-    <t>DLzCvKskasu4Adj3XgbyNitKBukBSa5JPP</t>
+    <t>DKs2WBbiaAEe9RGzQTmtJj1o9bqsKTUTtC</t>
+  </si>
+  <si>
+    <t>DR6bwf8JVrLKWSKQUKhyFeB6bqWSgHRMHi</t>
   </si>
   <si>
     <t>DB5KWytcxHyphHPn9iC92Y9JqPRL1Fq21p</t>
   </si>
   <si>
-    <t>A7rh9YzPJvkHvmJ4CxZGLMH6za55GhHchC</t>
-  </si>
-  <si>
-    <t>A9nQnT5Q77vLVYhcMTgCTjsPuzx1B7fqxo</t>
-  </si>
-  <si>
-    <t>9zfbkebu6Cv4Jd853BXAGKnppnKqzEa8QN</t>
-  </si>
-  <si>
-    <t>9rvn4wnK25vwXECpnaZWzLPWe4i7EQVULq</t>
-  </si>
-  <si>
-    <t>9vruGagGajRTC1kFcmfeEK9z4yEYvLHUXd</t>
-  </si>
-  <si>
-    <t>9yoTs1Y8iDL3gdhmCHYeUbxBUbAfpd8UKf</t>
-  </si>
-  <si>
-    <t>AAyT52Ni4MGsYCGsAMUHQ5QNKiCkZzSaY7</t>
-  </si>
-  <si>
-    <t>A3DwCPWCEH5E2GBZ8nfiVeWPBRgvZpEHXz</t>
-  </si>
-  <si>
-    <t>A5iDSrbhUjo6jaian3FAafceyjnM5mYniK</t>
-  </si>
-  <si>
-    <t>A9VTrFUAZX2m5HNEM1BVoXh5A4ZjNgahYT</t>
-  </si>
-  <si>
-    <t>A4AB5tNJDoxaJZepa6ukvuHvwB7odp1wcV</t>
-  </si>
-  <si>
-    <t>A55jHGWNwfNChbH5Psz97xNwXSgbruwmJw</t>
-  </si>
-  <si>
-    <t>9y5Civ2PpDz84j4Lr5Vcna43ZTxUnER9f1</t>
-  </si>
-  <si>
-    <t>9uLxcGj4CZpDarfoozN6BrRo5aLv1YJuPS</t>
+    <t>DLGJevmtj8kVp6z212ct1ac7eVBZT4ErLP</t>
+  </si>
+  <si>
+    <t>D648HSkSaygeU1h54DcpRKv4xRJBeNowHH</t>
+  </si>
+  <si>
+    <t>DPqhyyBpjuULZRvdeRwtMMF9JGr1rHjszh</t>
+  </si>
+  <si>
+    <t>DHGb5BKsagXePRWwKqLx2vMH5uUNg8euvN</t>
+  </si>
+  <si>
+    <t>A1xsYWbqxNomsYsv9V74kDEDuR7eGoPcgB</t>
+  </si>
+  <si>
+    <t>A4Tz5x7iN1q3WjjNJqUzPAWvXFa66aNkop</t>
+  </si>
+  <si>
+    <t>ACYnWddL6LgdkgwTgrAgkgfnqam8P85tLs</t>
+  </si>
+  <si>
+    <t>9rrwvHTUu4H7tc1ZqU1JQS9543roMxfgFx</t>
+  </si>
+  <si>
+    <t>AD7WQj9SpBvhMMJ3Co9JkHckYhu7o16CvP</t>
+  </si>
+  <si>
+    <t>A6BzKcpAUNDUJDs6bbizq4cxJvoo9AnXqx</t>
+  </si>
+  <si>
+    <t>A4WXtiiy2WfSpgmsw468EfWaDDcc2AkiEs</t>
+  </si>
+  <si>
+    <t>9teUMjXoLDzjG6CK2BFPstG7UicMpQbSCV</t>
+  </si>
+  <si>
+    <t>A3jaABqQr9WHcMzYThJxegYEeDSt519ESe</t>
+  </si>
+  <si>
+    <t>DM17LVDVnSUxaVncoYNWLjsSq5bYSWDwmy</t>
   </si>
 </sst>
 </file>
@@ -1416,21 +1431,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A29CAB09-E350-9A47-A01D-958BA1FF6BE9}">
-  <dimension ref="A1:F124"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{326B0548-0CD8-274C-8928-67B4E2AEFCFC}">
+  <dimension ref="A1:F132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:F32"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="24.5" customWidth="1"/>
-    <col min="2" max="2" width="51.83203125" customWidth="1"/>
-    <col min="3" max="3" width="18.83203125" customWidth="1"/>
-    <col min="4" max="4" width="19.1640625" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="2" max="2" width="52.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.5" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="135.33203125" customWidth="1"/>
+    <col min="6" max="6" width="135.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1452,7 +1467,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="1">
-        <v>20089.828020000001</v>
+        <v>19873.490000000002</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1460,10 +1475,10 @@
         <v>5</v>
       </c>
       <c r="B3" s="1">
-        <v>913920</v>
+        <v>917089</v>
       </c>
       <c r="C3" s="1">
-        <v>9451.18</v>
+        <v>9424.57</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1471,54 +1486,54 @@
         <v>6</v>
       </c>
       <c r="B4" s="1">
-        <v>75591302</v>
+        <v>76195906</v>
       </c>
       <c r="C4" s="1">
-        <v>10226.93</v>
+        <v>10448.93</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1">
-        <v>23040137</v>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C5" s="1">
-        <v>411.72</v>
+        <v>410737710.67000002</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>4</v>
+      <c r="B6" s="1">
+        <v>5898541</v>
       </c>
       <c r="C6" s="1">
-        <v>412767143.30000001</v>
+        <v>410737710.67000002</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="1">
-        <v>55869896</v>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C7" s="1">
-        <v>412767143.30000001</v>
+        <v>115019.87</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>4</v>
+      <c r="B8" s="1">
+        <v>23476856</v>
       </c>
       <c r="C8" s="1">
-        <v>110282.13189999999</v>
+        <v>10606.84</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1526,10 +1541,10 @@
         <v>11</v>
       </c>
       <c r="B9" s="1">
-        <v>23326594</v>
+        <v>23476856</v>
       </c>
       <c r="C9" s="1">
-        <v>9608.7000000000007</v>
+        <v>29984.62</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1537,407 +1552,371 @@
         <v>12</v>
       </c>
       <c r="B10" s="1">
-        <v>23326594</v>
+        <v>23476856</v>
       </c>
       <c r="C10" s="1">
-        <v>26357.42</v>
+        <v>74428.41</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="1">
-        <v>23326594</v>
-      </c>
-      <c r="C11" s="1">
-        <v>74316.009999999995</v>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>4</v>
+        <v>15</v>
+      </c>
+      <c r="B12" s="1">
+        <v>23476856</v>
       </c>
       <c r="C12" s="1">
-        <v>282019861205662</v>
+        <v>795870777823.44995</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B13" s="1">
-        <v>23326594</v>
-      </c>
-      <c r="C13" s="1">
-        <v>662825226929.5</v>
+        <v>76195906</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="1">
-        <v>75591302</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="1">
+        <v>301039.46999999997</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>4</v>
+        <v>19</v>
+      </c>
+      <c r="B15" s="1">
+        <v>370291757</v>
       </c>
       <c r="C15" s="1">
-        <v>284213.9877</v>
+        <v>301039.46999999997</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="1">
-        <v>365711359</v>
+        <v>20</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C16" s="1">
-        <v>284213.99</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>11062263077.360001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>4</v>
+        <v>21</v>
+      </c>
+      <c r="B17" s="1">
+        <v>76195906</v>
       </c>
       <c r="C17" s="1">
-        <v>11047203296</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>10139789271.42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B18" s="1">
-        <v>75591302</v>
+        <v>75332174</v>
       </c>
       <c r="C18" s="1">
-        <v>10124729489.639999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>922473805.94000006</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="1">
-        <v>75332174</v>
+        <v>23</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C19" s="1">
-        <v>922473805.94000006</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>36380771.649999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>4</v>
+        <v>24</v>
+      </c>
+      <c r="B20" s="1">
+        <v>23326594</v>
       </c>
       <c r="C20" s="1">
-        <v>1404148839</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>13336481.23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B21" s="1">
-        <v>75591302</v>
+        <v>23326594</v>
       </c>
       <c r="C21" s="1">
-        <v>38662662.909999996</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>22286475.800000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B22" s="1">
-        <v>68482953</v>
+        <v>370291757</v>
       </c>
       <c r="C22" s="1">
-        <v>541764.97</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>757814.62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="1">
-        <v>23326594</v>
+        <v>27</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C23" s="1">
-        <v>30524528.559999999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>1405335153.97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B24" s="1">
-        <v>75591302</v>
+        <v>76195906</v>
       </c>
       <c r="C24" s="1">
-        <v>96190257.760000005</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>38802928.560000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B25" s="1">
-        <v>75591302</v>
+        <v>69548271</v>
       </c>
       <c r="C25" s="1">
+        <v>153657.43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="1">
+        <v>23476856</v>
+      </c>
+      <c r="C26" s="1">
+        <v>16732839.98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="1">
+        <v>76195906</v>
+      </c>
+      <c r="C27" s="1">
+        <v>92517202.319999993</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="1">
+        <v>76195906</v>
+      </c>
+      <c r="C28" s="1">
         <v>96071462.310000002</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="1">
-        <v>23326594</v>
-      </c>
-      <c r="C26" s="1">
-        <v>1142158162.01</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="1">
-        <v>87832784.959999993</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="1">
-        <v>23326594</v>
-      </c>
-      <c r="C28" s="1">
-        <v>87832784.959999993</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>4</v>
+        <v>33</v>
+      </c>
+      <c r="B29" s="1">
+        <v>23476856</v>
       </c>
       <c r="C29" s="1">
-        <v>32624562.699999999</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+        <v>311057063.38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B30" s="1">
-        <v>98738024</v>
+        <v>3442409</v>
       </c>
       <c r="C30" s="1">
-        <v>32624562.699999999</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E32" s="3" t="s">
+        <v>850000000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="B31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="1">
+        <v>105350005.37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="1" t="s">
         <v>36</v>
+      </c>
+      <c r="B32" s="1">
+        <v>23476856</v>
+      </c>
+      <c r="C32" s="1">
+        <v>105350005.37</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="1" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="C33" s="1">
-        <v>913920</v>
-      </c>
-      <c r="D33" s="1">
-        <v>7310.7</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>39</v>
+        <v>32422510.530000001</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" s="1">
+        <v>99206637</v>
+      </c>
+      <c r="C34" s="1">
+        <v>32422510.530000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E36" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C34" s="1">
-        <v>913920</v>
-      </c>
-      <c r="D34" s="1">
-        <v>970.8</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F34" s="1" t="s">
+      <c r="F36" s="3" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C35" s="1">
-        <v>913920</v>
-      </c>
-      <c r="D35" s="1">
-        <v>829.68</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C36" s="1">
-        <v>913920</v>
-      </c>
-      <c r="D36" s="1">
-        <v>340</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C37" s="1">
-        <v>75591302</v>
+        <v>917089</v>
       </c>
       <c r="D37" s="1">
-        <v>10162.93</v>
+        <v>7310.7</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C38" s="1">
-        <v>75591302</v>
+        <v>917089</v>
       </c>
       <c r="D38" s="1">
-        <v>64</v>
+        <v>970.8</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" s="1">
+        <v>917089</v>
+      </c>
+      <c r="D39" s="1">
+        <v>829.68</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F39" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="C39" s="1">
-        <v>23040137</v>
-      </c>
-      <c r="D39" s="1">
-        <v>411.72</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="1" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40" s="1">
+        <v>917089</v>
+      </c>
+      <c r="D40" s="1">
+        <v>52.81</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="C40" s="1">
-        <v>75591302</v>
-      </c>
-      <c r="D40" s="1">
-        <v>1082058768.1300001</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>51</v>
@@ -1945,62 +1924,62 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="1" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C41" s="1">
-        <v>75591302</v>
+        <v>917089</v>
       </c>
       <c r="D41" s="1">
-        <v>1126521856.1600001</v>
+        <v>180</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>53</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="1" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42" s="1">
+        <v>76195906</v>
+      </c>
+      <c r="D42" s="1">
+        <v>10478.5</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F42" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="C42" s="1">
-        <v>75591302</v>
-      </c>
-      <c r="D42" s="1">
-        <v>1705110564.0899999</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="1" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C43" s="1">
-        <v>75591302</v>
+        <v>76195906</v>
       </c>
       <c r="D43" s="1">
-        <v>1434482060.2</v>
+        <v>51</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>57</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -2008,19 +1987,19 @@
         <v>21</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C44" s="1">
-        <v>75591302</v>
+        <v>76195906</v>
       </c>
       <c r="D44" s="1">
-        <v>1071232018.22</v>
+        <v>1082060842.4000001</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -2028,19 +2007,19 @@
         <v>21</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C45" s="1">
-        <v>75591302</v>
+        <v>76195906</v>
       </c>
       <c r="D45" s="1">
-        <v>1070373171.46</v>
+        <v>1126523930.4300001</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -2048,19 +2027,19 @@
         <v>21</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C46" s="1">
-        <v>75591302</v>
+        <v>76195906</v>
       </c>
       <c r="D46" s="1">
-        <v>1064061276.29</v>
+        <v>15049612.199999999</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -2068,356 +2047,356 @@
         <v>21</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C47" s="1">
-        <v>75591302</v>
+        <v>76195906</v>
       </c>
       <c r="D47" s="1">
-        <v>1570889775.0799999</v>
+        <v>1705110564.0899999</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C48" s="1">
-        <v>75332174</v>
+        <v>76195906</v>
       </c>
       <c r="D48" s="1">
-        <v>922473805.94000006</v>
+        <v>1434482060.2</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="C49" s="1">
-        <v>23326594</v>
+        <v>76195906</v>
       </c>
       <c r="D49" s="1">
-        <v>331.13</v>
+        <v>1071235028.75</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C50" s="1">
-        <v>23326594</v>
+        <v>76195906</v>
       </c>
       <c r="D50" s="1">
-        <v>8591.1</v>
+        <v>1070374107.72</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>4</v>
+        <v>67</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C51" s="1">
+        <v>76195906</v>
+      </c>
+      <c r="D51" s="1">
+        <v>1064063350.5599999</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F51" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>4</v>
+        <v>70</v>
+      </c>
+      <c r="C52" s="1">
+        <v>76195906</v>
+      </c>
+      <c r="D52" s="1">
+        <v>1570889775.0799999</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="1" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>4</v>
+        <v>72</v>
+      </c>
+      <c r="C53" s="1">
+        <v>75332174</v>
+      </c>
+      <c r="D53" s="1">
+        <v>922473805.94000006</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>4</v>
+        <v>74</v>
+      </c>
+      <c r="C54" s="1">
+        <v>23476856</v>
+      </c>
+      <c r="D54" s="1">
+        <v>1121.1099999999999</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C55" s="1">
-        <v>23326594</v>
+        <v>23476856</v>
       </c>
       <c r="D55" s="1">
-        <v>686.47</v>
+        <v>8881.1</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>79</v>
+        <v>4</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>80</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C56" s="1">
-        <v>23326594</v>
-      </c>
-      <c r="D56" s="1">
-        <v>26357.42</v>
+        <v>77</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>38</v>
+        <v>78</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B57" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F57" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="C57" s="1">
-        <v>23326594</v>
-      </c>
-      <c r="D57" s="1">
-        <v>33500.9</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C58" s="1">
-        <v>23326594</v>
-      </c>
-      <c r="D58" s="1">
-        <v>40815.11</v>
+        <v>82</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>38</v>
+        <v>78</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>49</v>
+        <v>83</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C59" s="1">
-        <v>23326594</v>
-      </c>
-      <c r="D59" s="1">
-        <v>142206650000</v>
+        <v>84</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>38</v>
+        <v>78</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="C60" s="1">
-        <v>23326594</v>
+        <v>23476856</v>
       </c>
       <c r="D60" s="1">
-        <v>7379235291.5</v>
+        <v>604.63</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C61" s="1">
-        <v>23326594</v>
+        <v>23476856</v>
       </c>
       <c r="D61" s="1">
-        <v>513239341638</v>
+        <v>29984.62</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>4</v>
+        <v>75</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>4</v>
+        <v>88</v>
+      </c>
+      <c r="C62" s="1">
+        <v>23476856</v>
+      </c>
+      <c r="D62" s="1">
+        <v>33551.57</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>70</v>
+        <v>4</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>71</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>4</v>
+        <v>74</v>
+      </c>
+      <c r="C63" s="1">
+        <v>23476856</v>
+      </c>
+      <c r="D63" s="1">
+        <v>40876.839999999997</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>4</v>
+      <c r="C64" s="1">
+        <v>23476856</v>
+      </c>
+      <c r="D64" s="1">
+        <v>274763650000</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>75</v>
@@ -2425,256 +2404,256 @@
     </row>
     <row r="65" spans="1:6">
       <c r="A65" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>4</v>
+        <v>86</v>
+      </c>
+      <c r="C65" s="1">
+        <v>23476856</v>
+      </c>
+      <c r="D65" s="1">
+        <v>7867786185.4399996</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="C66" s="1">
-        <v>75591302</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>82</v>
+        <v>23476856</v>
+      </c>
+      <c r="D66" s="1">
+        <v>513239341638</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C67" s="1">
-        <v>75591302</v>
-      </c>
-      <c r="D67" s="1">
-        <v>534335000000</v>
+        <v>77</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>4</v>
+        <v>78</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>4</v>
+        <v>79</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C68" s="1">
-        <v>75591302</v>
-      </c>
-      <c r="D68" s="1">
-        <v>112378636975.81</v>
+        <v>80</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C69" s="1">
-        <v>365711359</v>
-      </c>
-      <c r="D69" s="1">
-        <v>5550.97</v>
+        <v>82</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>4</v>
+        <v>78</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>4</v>
+        <v>83</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C70" s="1">
-        <v>365711359</v>
-      </c>
-      <c r="D70" s="1">
-        <v>1786.52</v>
+        <v>84</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>4</v>
+        <v>78</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>87</v>
+        <v>53</v>
       </c>
       <c r="C71" s="1">
-        <v>365711359</v>
-      </c>
-      <c r="D71" s="1">
-        <v>276876.5</v>
+        <v>76195906</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C72" s="1">
-        <v>75591302</v>
+        <v>76195906</v>
       </c>
       <c r="D72" s="1">
-        <v>38662662.909999996</v>
+        <v>312313000000</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" s="1" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C73" s="1">
-        <v>68482953</v>
+        <v>76195906</v>
       </c>
       <c r="D73" s="1">
-        <v>541764.97</v>
+        <v>150611910359.92001</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>4</v>
+        <v>91</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>45</v>
+        <v>92</v>
       </c>
       <c r="C74" s="1">
-        <v>75591302</v>
+        <v>370291757</v>
       </c>
       <c r="D74" s="1">
-        <v>96071462.310000002</v>
+        <v>41550.97</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" s="1" t="s">
-        <v>89</v>
+        <v>19</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="C75" s="1">
-        <v>23326594</v>
+        <v>370291757</v>
       </c>
       <c r="D75" s="1">
-        <v>2167893.16</v>
+        <v>1673.88</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>79</v>
+        <v>4</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>80</v>
+        <v>4</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" s="1" t="s">
-        <v>89</v>
+        <v>19</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C76" s="1">
-        <v>23326594</v>
+        <v>370291757</v>
       </c>
       <c r="D76" s="1">
-        <v>1045412.19</v>
+        <v>257814.62</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>91</v>
+        <v>4</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" s="1" t="s">
-        <v>89</v>
+        <v>26</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>68</v>
+        <v>94</v>
       </c>
       <c r="C77" s="1">
-        <v>23326594</v>
+        <v>370291757</v>
       </c>
       <c r="D77" s="1">
-        <v>27311223.210000001</v>
+        <v>757814.62</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>4</v>
@@ -2685,116 +2664,116 @@
     </row>
     <row r="78" spans="1:6">
       <c r="A78" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>4</v>
+        <v>76</v>
+      </c>
+      <c r="C78" s="1">
+        <v>23326594</v>
+      </c>
+      <c r="D78" s="1">
+        <v>8294000</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>70</v>
+        <v>4</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>71</v>
+        <v>4</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c r="A79" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>4</v>
+        <v>74</v>
+      </c>
+      <c r="C79" s="1">
+        <v>23326594</v>
+      </c>
+      <c r="D79" s="1">
+        <v>3886000</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>4</v>
+        <v>86</v>
+      </c>
+      <c r="C80" s="1">
+        <v>23326594</v>
+      </c>
+      <c r="D80" s="1">
+        <v>1156481.23</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81" s="1" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>4</v>
+        <v>74</v>
+      </c>
+      <c r="C81" s="1">
+        <v>23326594</v>
+      </c>
+      <c r="D81" s="1">
+        <v>22286475.800000001</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="C82" s="1">
-        <v>75591302</v>
+        <v>76195906</v>
       </c>
       <c r="D82" s="1">
-        <v>50000000</v>
+        <v>38802928.560000002</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>47</v>
+        <v>95</v>
       </c>
       <c r="C83" s="1">
-        <v>75591302</v>
+        <v>69548271</v>
       </c>
       <c r="D83" s="1">
-        <v>43864485.100000001</v>
+        <v>153657.43</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>4</v>
@@ -2805,162 +2784,162 @@
     </row>
     <row r="84" spans="1:6">
       <c r="A84" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>4</v>
+        <v>53</v>
+      </c>
+      <c r="C84" s="1">
+        <v>76195906</v>
+      </c>
+      <c r="D84" s="1">
+        <v>96071462.310000002</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>93</v>
+        <v>54</v>
       </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85" s="1" t="s">
-        <v>27</v>
+        <v>96</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>4</v>
+        <v>86</v>
+      </c>
+      <c r="C85" s="1">
+        <v>23476856</v>
+      </c>
+      <c r="D85" s="1">
+        <v>3211393.58</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86" s="1" t="s">
-        <v>27</v>
+        <v>96</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>4</v>
+        <v>97</v>
+      </c>
+      <c r="C86" s="1">
+        <v>23476856</v>
+      </c>
+      <c r="D86" s="1">
+        <v>1045412.19</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="87" spans="1:6">
       <c r="A87" s="1" t="s">
-        <v>27</v>
+        <v>96</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C87" s="1">
-        <v>75591302</v>
+        <v>23476856</v>
       </c>
       <c r="D87" s="1">
-        <v>2325772.66</v>
+        <v>12476034.210000001</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>79</v>
+        <v>4</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>84</v>
+        <v>4</v>
       </c>
     </row>
     <row r="88" spans="1:6">
       <c r="A88" s="1" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C88" s="1">
-        <v>23326594</v>
-      </c>
-      <c r="D88" s="1">
-        <v>1142158162.01</v>
+        <v>77</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>38</v>
+        <v>78</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="A89" s="1" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C89" s="1">
-        <v>98738024</v>
-      </c>
-      <c r="D89" s="1">
-        <v>31887852.739999998</v>
+        <v>80</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>4</v>
+        <v>78</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>4</v>
+        <v>81</v>
       </c>
     </row>
     <row r="90" spans="1:6">
       <c r="A90" s="1" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C90" s="1">
-        <v>98738024</v>
-      </c>
-      <c r="D90" s="1">
-        <v>609602.18999999994</v>
+        <v>82</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>4</v>
+        <v>78</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>4</v>
+        <v>83</v>
       </c>
     </row>
     <row r="91" spans="1:6">
       <c r="A91" s="1" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C91" s="1">
-        <v>98738024</v>
-      </c>
-      <c r="D91" s="1">
-        <v>127107.77</v>
+        <v>84</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>4</v>
+        <v>78</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -2968,13 +2947,13 @@
         <v>31</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="C92" s="1">
-        <v>23326594</v>
+        <v>76195906</v>
       </c>
       <c r="D92" s="1">
-        <v>55000002</v>
+        <v>50000015.600000001</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>4</v>
@@ -2988,19 +2967,19 @@
         <v>31</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="C93" s="1">
-        <v>23326594</v>
+        <v>76195906</v>
       </c>
       <c r="D93" s="1">
-        <v>21991000</v>
+        <v>39055483.100000001</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>49</v>
+        <v>4</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -3008,133 +2987,133 @@
         <v>31</v>
       </c>
       <c r="B94" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E94" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C94" s="1">
-        <v>23326594</v>
-      </c>
-      <c r="D94" s="1">
-        <v>10841782.960000001</v>
-      </c>
-      <c r="E94" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="F94" s="1" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="95" spans="1:6">
       <c r="A95" s="1" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C95" s="1">
-        <v>5869896</v>
-      </c>
-      <c r="D95" s="1">
-        <v>286206111.25999999</v>
+      <c r="C95" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>4</v>
+        <v>78</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>4</v>
+        <v>102</v>
       </c>
     </row>
     <row r="96" spans="1:6">
       <c r="A96" s="1" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C96" s="1">
-        <v>5869896</v>
-      </c>
-      <c r="D96" s="1">
-        <v>82781244.920000002</v>
+        <v>103</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>4</v>
+        <v>78</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>4</v>
+        <v>104</v>
       </c>
     </row>
     <row r="97" spans="1:6">
       <c r="A97" s="1" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="C97" s="1">
-        <v>5869896</v>
+        <v>76195906</v>
       </c>
       <c r="D97" s="1">
-        <v>624076.68000000005</v>
+        <v>3461703.62</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>4</v>
+        <v>91</v>
       </c>
     </row>
     <row r="98" spans="1:6">
       <c r="A98" s="1" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
       <c r="C98" s="1">
-        <v>5869896</v>
+        <v>23476856</v>
       </c>
       <c r="D98" s="1">
-        <v>4631544.88</v>
+        <v>311057063.38</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>4</v>
+        <v>75</v>
       </c>
     </row>
     <row r="99" spans="1:6">
       <c r="A99" s="1" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>105</v>
       </c>
       <c r="C99" s="1">
-        <v>5869896</v>
+        <v>3442409</v>
       </c>
       <c r="D99" s="1">
-        <v>4445950.8</v>
+        <v>850000000</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>4</v>
+        <v>75</v>
       </c>
     </row>
     <row r="100" spans="1:6">
       <c r="A100" s="1" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>106</v>
       </c>
       <c r="C100" s="1">
-        <v>5869896</v>
+        <v>99206637</v>
       </c>
       <c r="D100" s="1">
-        <v>2866994</v>
+        <v>31587852.739999998</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>4</v>
@@ -3145,16 +3124,16 @@
     </row>
     <row r="101" spans="1:6">
       <c r="A101" s="1" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>107</v>
       </c>
       <c r="C101" s="1">
-        <v>5869896</v>
+        <v>99206637</v>
       </c>
       <c r="D101" s="1">
-        <v>2647816.5299999998</v>
+        <v>687036.19</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>4</v>
@@ -3165,16 +3144,16 @@
     </row>
     <row r="102" spans="1:6">
       <c r="A102" s="1" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>108</v>
       </c>
       <c r="C102" s="1">
-        <v>5869896</v>
+        <v>99206637</v>
       </c>
       <c r="D102" s="1">
-        <v>2451906.98</v>
+        <v>147621.6</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>4</v>
@@ -3185,16 +3164,16 @@
     </row>
     <row r="103" spans="1:6">
       <c r="A103" s="1" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>109</v>
+        <v>76</v>
       </c>
       <c r="C103" s="1">
-        <v>5869896</v>
+        <v>23476856</v>
       </c>
       <c r="D103" s="1">
-        <v>1457329.63</v>
+        <v>62438002</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>4</v>
@@ -3205,56 +3184,56 @@
     </row>
     <row r="104" spans="1:6">
       <c r="A104" s="1" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>110</v>
+        <v>74</v>
       </c>
       <c r="C104" s="1">
-        <v>5869896</v>
+        <v>23476856</v>
       </c>
       <c r="D104" s="1">
-        <v>850746.71</v>
+        <v>42156000</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>4</v>
+        <v>75</v>
       </c>
     </row>
     <row r="105" spans="1:6">
       <c r="A105" s="1" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="C105" s="1">
-        <v>5869896</v>
+        <v>23476856</v>
       </c>
       <c r="D105" s="1">
-        <v>285678.89</v>
+        <v>756003.37</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>4</v>
+        <v>87</v>
       </c>
     </row>
     <row r="106" spans="1:6">
       <c r="A106" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C106" s="1">
-        <v>5869896</v>
+        <v>5898541</v>
       </c>
       <c r="D106" s="1">
-        <v>170777.71</v>
+        <v>18558000.760000002</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>4</v>
@@ -3265,16 +3244,16 @@
     </row>
     <row r="107" spans="1:6">
       <c r="A107" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C107" s="1">
-        <v>5869896</v>
+        <v>5898541</v>
       </c>
       <c r="D107" s="1">
-        <v>1066964.3</v>
+        <v>277751003.25999999</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>4</v>
@@ -3285,16 +3264,16 @@
     </row>
     <row r="108" spans="1:6">
       <c r="A108" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C108" s="1">
-        <v>5869896</v>
+        <v>5898541</v>
       </c>
       <c r="D108" s="1">
-        <v>538350.48</v>
+        <v>7499952.3300000001</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>4</v>
@@ -3305,16 +3284,16 @@
     </row>
     <row r="109" spans="1:6">
       <c r="A109" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C109" s="1">
-        <v>5869896</v>
+        <v>5898541</v>
       </c>
       <c r="D109" s="1">
-        <v>120247.67</v>
+        <v>2866994</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>4</v>
@@ -3325,16 +3304,16 @@
     </row>
     <row r="110" spans="1:6">
       <c r="A110" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C110" s="1">
-        <v>5869896</v>
+        <v>5898541</v>
       </c>
       <c r="D110" s="1">
-        <v>127419.44</v>
+        <v>2647816.5299999998</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>4</v>
@@ -3345,16 +3324,16 @@
     </row>
     <row r="111" spans="1:6">
       <c r="A111" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C111" s="1">
-        <v>5869896</v>
+        <v>5898541</v>
       </c>
       <c r="D111" s="1">
-        <v>4030998.06</v>
+        <v>1457329.63</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>4</v>
@@ -3365,16 +3344,16 @@
     </row>
     <row r="112" spans="1:6">
       <c r="A112" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C112" s="1">
-        <v>5869896</v>
+        <v>5898541</v>
       </c>
       <c r="D112" s="1">
-        <v>3627998.92</v>
+        <v>850746.71</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>4</v>
@@ -3385,16 +3364,16 @@
     </row>
     <row r="113" spans="1:6">
       <c r="A113" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C113" s="1">
-        <v>5869896</v>
+        <v>5898541</v>
       </c>
       <c r="D113" s="1">
-        <v>2725997.87</v>
+        <v>2146027.41</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>4</v>
@@ -3405,16 +3384,16 @@
     </row>
     <row r="114" spans="1:6">
       <c r="A114" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C114" s="1">
-        <v>5869896</v>
+        <v>5898541</v>
       </c>
       <c r="D114" s="1">
-        <v>2306999.81</v>
+        <v>1066964.3</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>4</v>
@@ -3425,16 +3404,16 @@
     </row>
     <row r="115" spans="1:6">
       <c r="A115" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C115" s="1">
-        <v>5869896</v>
+        <v>5898541</v>
       </c>
       <c r="D115" s="1">
-        <v>1560993.24</v>
+        <v>538350.48</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>4</v>
@@ -3445,16 +3424,16 @@
     </row>
     <row r="116" spans="1:6">
       <c r="A116" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C116" s="1">
-        <v>5869896</v>
+        <v>5898541</v>
       </c>
       <c r="D116" s="1">
-        <v>1397999.81</v>
+        <v>1139517.8999999999</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>4</v>
@@ -3465,16 +3444,16 @@
     </row>
     <row r="117" spans="1:6">
       <c r="A117" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C117" s="1">
-        <v>5869896</v>
+        <v>5898541</v>
       </c>
       <c r="D117" s="1">
-        <v>1192999.6299999999</v>
+        <v>1415882.02</v>
       </c>
       <c r="E117" s="1" t="s">
         <v>4</v>
@@ -3485,16 +3464,16 @@
     </row>
     <row r="118" spans="1:6">
       <c r="A118" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C118" s="1">
-        <v>5869896</v>
+        <v>5898541</v>
       </c>
       <c r="D118" s="1">
-        <v>961999.81</v>
+        <v>127419.44</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>4</v>
@@ -3505,16 +3484,16 @@
     </row>
     <row r="119" spans="1:6">
       <c r="A119" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C119" s="1">
-        <v>5869896</v>
+        <v>5898541</v>
       </c>
       <c r="D119" s="1">
-        <v>792999.81</v>
+        <v>701267.06</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>4</v>
@@ -3525,16 +3504,16 @@
     </row>
     <row r="120" spans="1:6">
       <c r="A120" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C120" s="1">
-        <v>5869896</v>
+        <v>5898541</v>
       </c>
       <c r="D120" s="1">
-        <v>714999.63</v>
+        <v>412420.03</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>4</v>
@@ -3545,16 +3524,16 @@
     </row>
     <row r="121" spans="1:6">
       <c r="A121" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C121" s="1">
-        <v>5869896</v>
+        <v>5898541</v>
       </c>
       <c r="D121" s="1">
-        <v>679999.81</v>
+        <v>1926995.04</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>4</v>
@@ -3565,16 +3544,16 @@
     </row>
     <row r="122" spans="1:6">
       <c r="A122" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C122" s="1">
-        <v>5869896</v>
+        <v>5898541</v>
       </c>
       <c r="D122" s="1">
-        <v>623997.65</v>
+        <v>68603667.329999998</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>4</v>
@@ -3585,16 +3564,16 @@
     </row>
     <row r="123" spans="1:6">
       <c r="A123" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C123" s="1">
-        <v>5869896</v>
+        <v>5898541</v>
       </c>
       <c r="D123" s="1">
-        <v>536999.63</v>
+        <v>5519998.04</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>4</v>
@@ -3605,21 +3584,181 @@
     </row>
     <row r="124" spans="1:6">
       <c r="A124" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B124" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C124" s="1">
+        <v>5898541</v>
+      </c>
+      <c r="D124" s="1">
+        <v>2786999.81</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6">
+      <c r="A125" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C125" s="1">
+        <v>5898541</v>
+      </c>
+      <c r="D125" s="1">
+        <v>2655996.87</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6">
+      <c r="A126" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C126" s="1">
+        <v>5898541</v>
+      </c>
+      <c r="D126" s="1">
+        <v>2547998.9900000002</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6">
+      <c r="A127" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B127" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C124" s="1">
-        <v>5869896</v>
-      </c>
-      <c r="D124" s="1">
-        <v>338998.77</v>
-      </c>
-      <c r="E124" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F124" s="1" t="s">
+      <c r="C127" s="1">
+        <v>5898541</v>
+      </c>
+      <c r="D127" s="1">
+        <v>1968999.52</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6">
+      <c r="A128" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C128" s="1">
+        <v>5898541</v>
+      </c>
+      <c r="D128" s="1">
+        <v>1664999.66</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F128" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6">
+      <c r="A129" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C129" s="1">
+        <v>5898541</v>
+      </c>
+      <c r="D129" s="1">
+        <v>1346999.81</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F129" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6">
+      <c r="A130" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C130" s="1">
+        <v>5898541</v>
+      </c>
+      <c r="D130" s="1">
+        <v>1329999.81</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F130" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6">
+      <c r="A131" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C131" s="1">
+        <v>5898541</v>
+      </c>
+      <c r="D131" s="1">
+        <v>625999.81000000006</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F131" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6">
+      <c r="A132" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C132" s="1">
+        <v>5898541</v>
+      </c>
+      <c r="D132" s="1">
+        <v>579364.13</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F132" s="1" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update snapshot 20251201; add support BEP20-USDC; update node version to 22 LTS; update tools and its version;
</commit_message>
<xml_diff>
--- a/snapshot/huobi_por.xlsx
+++ b/snapshot/huobi_por.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiangliqiang/Repo/Tool-Node.js-VerifyAddress/snapshot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4BCD1C0E-D96D-F54B-BEEF-8BC36A84F83D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D6D7D5B9-6067-124F-B29C-FFD57D228FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{60B29559-677B-DA4D-AA00-E4410F0FEE4D}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{411BB281-6367-B440-9EF5-E7547829EACC}"/>
   </bookViews>
   <sheets>
     <sheet name="huobi_por" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" calcOnSave="0"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="137">
   <si>
     <t>coin</t>
   </si>
@@ -64,7 +64,7 @@
     <t>HTX(ALL)</t>
   </si>
   <si>
-    <t>279469118029940.00</t>
+    <t>264152465223381.00</t>
   </si>
   <si>
     <t>HTX-ERC20</t>
@@ -73,7 +73,7 @@
     <t>HTX-TRC20</t>
   </si>
   <si>
-    <t>278673247252117.00</t>
+    <t>263294682471342.00</t>
   </si>
   <si>
     <t>SOL(All)</t>
@@ -100,6 +100,9 @@
     <t>STEAK-USDC</t>
   </si>
   <si>
+    <t>BEP20-USDC</t>
+  </si>
+  <si>
     <t>USDC-SOL</t>
   </si>
   <si>
@@ -124,9 +127,6 @@
     <t>USDT-aEthUSDT</t>
   </si>
   <si>
-    <t>USDT-XPL</t>
-  </si>
-  <si>
     <t>WLFI(All)</t>
   </si>
   <si>
@@ -169,6 +169,9 @@
     <t>IDxEvxbNOXY2KeARpazYGHu4ZPPx+/LJpG+dItGV1GFNZoR5+sVekMFAf2ICYE0CwULl9PDejDl8aM6fnGheCFM=</t>
   </si>
   <si>
+    <t>12AxQ3mM2rwY2mwLa5qNVY65uHoQGfvSVF</t>
+  </si>
+  <si>
     <t>1AQLXAB6aXSVbRMjbhSBudLf1kcsbWSEjg</t>
   </si>
   <si>
@@ -196,10 +199,10 @@
     <t>24d160af1f9f0c4ff530f85f6ed0850927727a7a4a576918d1d502c2af3eb4227417b1527e5eb5aae09529935d0662b5775d5f67db06d46ac34ee7e127c1582901</t>
   </si>
   <si>
-    <t>TKgD8Qnx9Zw3DNvG6o83PkufnMbtEXis4T</t>
-  </si>
-  <si>
-    <t>1acfc19531231fd17c1f28d0f3534a00afcbca453773d8840cd75a3d0ef51ee66a995f4149c4ddc5f713e13511ca2c242da9826b4d83c3730364d866f406e0cd01</t>
+    <t>TCQQjfccKdMi4CnPAzmZW5TALH4HbwceVb</t>
+  </si>
+  <si>
+    <t>4d3baf9ceb963cb5224005d1f1dc769bbb57c4710ffe5a2432d46c9b8ad22cd90ae94a5f53af14314b68808802aa944a4a99b0c5c181e95b87f32a3f0aeefef700</t>
   </si>
   <si>
     <t>TGn1uvntAVntT1pG8o7qoKkbViiYfeg6Gj</t>
@@ -250,6 +253,12 @@
     <t>0x68a79a40adfb16777e49206d60f9cd11de0fbaf3acad5be1e30dd955182475f43255dfec5fede4dc97fcf1fbce1583dd05ee419bf3939ca95919aff931eec41d01</t>
   </si>
   <si>
+    <t>0x2a4bf9bbca7a91661087f52571eea36a004b83eb</t>
+  </si>
+  <si>
+    <t>0x9e2b154db03c9cf389c2ff9f3921299f2ec7fb4893b91893855a7e2627783a7159f2e798c0450013d11961db1f100fc8a59dbd49384a1cbae160820f6165457c1c</t>
+  </si>
+  <si>
     <t>0x4fb312915b779b1339388e14b6d079741ca83128</t>
   </si>
   <si>
@@ -289,7 +298,7 @@
     <t>0x6663613fbd927ce78abbf7f5ca7e2c3fe0d96d18</t>
   </si>
   <si>
-    <t>278210322341756.00</t>
+    <t>261879720157182.00</t>
   </si>
   <si>
     <t>TFTWNgDBkQ5wQoP8RXpRznnHvAVV8x5jLu</t>
@@ -307,18 +316,21 @@
     <t>8NBEbxLknGv5aRYefFrW2qFXoDZyi9fSHJNiJRvEcMBE</t>
   </si>
   <si>
+    <t>0xafdfd157d9361e621e476036fee62f688450692b</t>
+  </si>
+  <si>
+    <t>0xdd3cb5c974601bc3974d908ea4a86020f9999e0c</t>
+  </si>
+  <si>
+    <t>0xd073bd9a42e935972c048fe2a3b7acfbb5d107d5fc22562efc88834f4b8ff83c359ce34f8d0c3c847f8d1c10afdd9ea126df84bb6bd11df486c920f826f828d400</t>
+  </si>
+  <si>
     <t>0xa77ff0e1c52f58363a53282624c7baa5fa91687d</t>
   </si>
   <si>
     <t>USDT-ETH</t>
   </si>
   <si>
-    <t>0x2a4bf9bbca7a91661087f52571eea36a004b83eb</t>
-  </si>
-  <si>
-    <t>0x9e2b154db03c9cf389c2ff9f3921299f2ec7fb4893b91893855a7e2627783a7159f2e798c0450013d11961db1f100fc8a59dbd49384a1cbae160820f6165457c1c</t>
-  </si>
-  <si>
     <t>TWN6yGR6VzYmThSy2CmkpEASyvwV4VKRDs</t>
   </si>
   <si>
@@ -337,9 +349,6 @@
     <t>0x3ca7a1fcc5306107b4bd37c82359ec2a1c62b32658bb01201f12bf5e9e1b5c54623f440d226165bf4d216cffe5a4e3fce9e636e7514eac5c29af97df12e88fd400</t>
   </si>
   <si>
-    <t>0x18709E89BD403F470088aBDAcEbE86CC60dda12e</t>
-  </si>
-  <si>
     <t>rKUDvXFJMFu65LqPTH3Yfpii4rbKT9bSQT</t>
   </si>
   <si>
@@ -370,64 +379,58 @@
     <t>DQkukxxY7LYdb2bchK8Zgo14wwyEPsHVJf</t>
   </si>
   <si>
-    <t>DQhEuTa5UkNcD8YFZK3pvjFfrtMqQpJhSa</t>
-  </si>
-  <si>
     <t>DJxVuu8KDh7qKfuieJoWQNFYmK1L3k773X</t>
   </si>
   <si>
     <t>DSqzssxy31fpuGFJfZjoM6TqP38oNPAPiN</t>
   </si>
   <si>
-    <t>DKs2WBbiaAEe9RGzQTmtJj1o9bqsKTUTtC</t>
-  </si>
-  <si>
-    <t>DR6bwf8JVrLKWSKQUKhyFeB6bqWSgHRMHi</t>
+    <t>DLzCvKskasu4Adj3XgbyNitKBukBSa5JPP</t>
   </si>
   <si>
     <t>DB5KWytcxHyphHPn9iC92Y9JqPRL1Fq21p</t>
   </si>
   <si>
-    <t>DLGJevmtj8kVp6z212ct1ac7eVBZT4ErLP</t>
-  </si>
-  <si>
-    <t>D648HSkSaygeU1h54DcpRKv4xRJBeNowHH</t>
-  </si>
-  <si>
-    <t>DPqhyyBpjuULZRvdeRwtMMF9JGr1rHjszh</t>
+    <t>DL2EGukahtib57Sg7FtHsvf8HgwMJtbBA3</t>
   </si>
   <si>
     <t>DHGb5BKsagXePRWwKqLx2vMH5uUNg8euvN</t>
   </si>
   <si>
-    <t>A1xsYWbqxNomsYsv9V74kDEDuR7eGoPcgB</t>
-  </si>
-  <si>
-    <t>A4Tz5x7iN1q3WjjNJqUzPAWvXFa66aNkop</t>
-  </si>
-  <si>
-    <t>ACYnWddL6LgdkgwTgrAgkgfnqam8P85tLs</t>
-  </si>
-  <si>
-    <t>9rrwvHTUu4H7tc1ZqU1JQS9543roMxfgFx</t>
-  </si>
-  <si>
-    <t>AD7WQj9SpBvhMMJ3Co9JkHckYhu7o16CvP</t>
-  </si>
-  <si>
-    <t>A6BzKcpAUNDUJDs6bbizq4cxJvoo9AnXqx</t>
-  </si>
-  <si>
-    <t>A4WXtiiy2WfSpgmsw468EfWaDDcc2AkiEs</t>
-  </si>
-  <si>
-    <t>9teUMjXoLDzjG6CK2BFPstG7UicMpQbSCV</t>
-  </si>
-  <si>
-    <t>A3jaABqQr9WHcMzYThJxegYEeDSt519ESe</t>
-  </si>
-  <si>
     <t>DM17LVDVnSUxaVncoYNWLjsSq5bYSWDwmy</t>
+  </si>
+  <si>
+    <t>A1NxyPuaxiPm24RJR1DYU7tVYwcFqRtgEf</t>
+  </si>
+  <si>
+    <t>9xzSxYs2w8s6EGbzrj1qXgoSefbc9B4u4Z</t>
+  </si>
+  <si>
+    <t>9uCrSKxDtYQb3ogf4Z93qQcnihy5mzwGMs</t>
+  </si>
+  <si>
+    <t>AFAocif1boV7t9NQsSJuZFj1MjAMugurAJ</t>
+  </si>
+  <si>
+    <t>9tezKrvR5zoYv5sc67KWRi5fUwSdM7nHnF</t>
+  </si>
+  <si>
+    <t>9vjmf33smeHJksTLiDZ9xbD6AQtqxB6NAB</t>
+  </si>
+  <si>
+    <t>A6z32fmFDejWyQfQH3Vp9bxQjJ8Qw2Ad4c</t>
+  </si>
+  <si>
+    <t>AFERVSFd9Q3aBX3sWUMbfVWnrcCVyBrUMv</t>
+  </si>
+  <si>
+    <t>A7HHQEqvdZugErQmVPRpZ5VP6sHH7ziKN1</t>
+  </si>
+  <si>
+    <t>A96kc8NYE8itzvo14dbrnBv8UDusU71hQW</t>
+  </si>
+  <si>
+    <t>9vhUDyKZ3ths23UeDNUxRBUMaVvCEsAkFr</t>
   </si>
 </sst>
 </file>
@@ -1431,21 +1434,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{326B0548-0CD8-274C-8928-67B4E2AEFCFC}">
-  <dimension ref="A1:F132"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{551DE6D8-23DE-D340-B153-F7BA258674FF}">
+  <dimension ref="A1:F134"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="A36" sqref="A36:F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" customWidth="1"/>
-    <col min="2" max="2" width="52.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20.5" customWidth="1"/>
-    <col min="4" max="4" width="18.83203125" customWidth="1"/>
-    <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="135.6640625" customWidth="1"/>
+    <col min="1" max="1" width="23.1640625" customWidth="1"/>
+    <col min="2" max="2" width="52.5" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="136.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1467,7 +1470,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="1">
-        <v>19873.490000000002</v>
+        <v>20320.689999999999</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1475,10 +1478,10 @@
         <v>5</v>
       </c>
       <c r="B3" s="1">
-        <v>917089</v>
+        <v>925888</v>
       </c>
       <c r="C3" s="1">
-        <v>9424.57</v>
+        <v>9368.77</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1486,10 +1489,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="1">
-        <v>76195906</v>
+        <v>77952195</v>
       </c>
       <c r="C4" s="1">
-        <v>10448.93</v>
+        <v>10951.93</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1500,7 +1503,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="1">
-        <v>410737710.67000002</v>
+        <v>439849388.82999998</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1508,10 +1511,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="1">
-        <v>5898541</v>
+        <v>5981741</v>
       </c>
       <c r="C6" s="1">
-        <v>410737710.67000002</v>
+        <v>439849388.82999998</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1522,7 +1525,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="1">
-        <v>115019.87</v>
+        <v>118675.34</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1530,10 +1533,10 @@
         <v>10</v>
       </c>
       <c r="B8" s="1">
-        <v>23476856</v>
+        <v>23912531</v>
       </c>
       <c r="C8" s="1">
-        <v>10606.84</v>
+        <v>10421.459999999999</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1541,10 +1544,10 @@
         <v>11</v>
       </c>
       <c r="B9" s="1">
-        <v>23476856</v>
+        <v>23912531</v>
       </c>
       <c r="C9" s="1">
-        <v>29984.62</v>
+        <v>8449.5400000000009</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1552,10 +1555,10 @@
         <v>12</v>
       </c>
       <c r="B10" s="1">
-        <v>23476856</v>
+        <v>23912531</v>
       </c>
       <c r="C10" s="1">
-        <v>74428.41</v>
+        <v>99804.33</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1574,10 +1577,10 @@
         <v>15</v>
       </c>
       <c r="B12" s="1">
-        <v>23476856</v>
+        <v>23912531</v>
       </c>
       <c r="C12" s="1">
-        <v>795870777823.44995</v>
+        <v>857782752038.81006</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1585,7 +1588,7 @@
         <v>16</v>
       </c>
       <c r="B13" s="1">
-        <v>76195906</v>
+        <v>77952195</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>17</v>
@@ -1599,7 +1602,7 @@
         <v>4</v>
       </c>
       <c r="C14" s="1">
-        <v>301039.46999999997</v>
+        <v>357844.83</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1607,10 +1610,10 @@
         <v>19</v>
       </c>
       <c r="B15" s="1">
-        <v>370291757</v>
+        <v>383565184</v>
       </c>
       <c r="C15" s="1">
-        <v>301039.46999999997</v>
+        <v>357844.83</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1621,7 +1624,7 @@
         <v>4</v>
       </c>
       <c r="C16" s="1">
-        <v>11062263077.360001</v>
+        <v>9937833805.9300003</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1629,10 +1632,10 @@
         <v>21</v>
       </c>
       <c r="B17" s="1">
-        <v>76195906</v>
+        <v>77952195</v>
       </c>
       <c r="C17" s="1">
-        <v>10139789271.42</v>
+        <v>9015359999.9799995</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1654,7 +1657,7 @@
         <v>4</v>
       </c>
       <c r="C19" s="1">
-        <v>36380771.649999999</v>
+        <v>53101640.619999997</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1662,10 +1665,10 @@
         <v>24</v>
       </c>
       <c r="B20" s="1">
-        <v>23326594</v>
+        <v>23912531</v>
       </c>
       <c r="C20" s="1">
-        <v>13336481.23</v>
+        <v>16265656.890000001</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1676,7 +1679,7 @@
         <v>23326594</v>
       </c>
       <c r="C21" s="1">
-        <v>22286475.800000001</v>
+        <v>29807884.100000001</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1684,32 +1687,32 @@
         <v>26</v>
       </c>
       <c r="B22" s="1">
-        <v>370291757</v>
+        <v>69863728</v>
       </c>
       <c r="C22" s="1">
-        <v>757814.62</v>
+        <v>6270285</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>4</v>
+      <c r="B23" s="1">
+        <v>370291757</v>
       </c>
       <c r="C23" s="1">
-        <v>1405335153.97</v>
+        <v>757814.62</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="1">
-        <v>76195906</v>
+      <c r="B24" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C24" s="1">
-        <v>38802928.560000002</v>
+        <v>1783063060.8900001</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1717,10 +1720,10 @@
         <v>29</v>
       </c>
       <c r="B25" s="1">
-        <v>69548271</v>
+        <v>77952195</v>
       </c>
       <c r="C25" s="1">
-        <v>153657.43</v>
+        <v>18203565.989999998</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1728,10 +1731,10 @@
         <v>30</v>
       </c>
       <c r="B26" s="1">
-        <v>23476856</v>
+        <v>72861177</v>
       </c>
       <c r="C26" s="1">
-        <v>16732839.98</v>
+        <v>906956</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1739,10 +1742,10 @@
         <v>31</v>
       </c>
       <c r="B27" s="1">
-        <v>76195906</v>
+        <v>23912531</v>
       </c>
       <c r="C27" s="1">
-        <v>92517202.319999993</v>
+        <v>148850579.63999999</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1750,10 +1753,10 @@
         <v>32</v>
       </c>
       <c r="B28" s="1">
-        <v>76195906</v>
+        <v>77952195</v>
       </c>
       <c r="C28" s="1">
-        <v>96071462.310000002</v>
+        <v>71480688.719999999</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1761,10 +1764,10 @@
         <v>33</v>
       </c>
       <c r="B29" s="1">
-        <v>23476856</v>
+        <v>76195906</v>
       </c>
       <c r="C29" s="1">
-        <v>311057063.38</v>
+        <v>96071462.310000002</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1772,10 +1775,10 @@
         <v>34</v>
       </c>
       <c r="B30" s="1">
-        <v>3442409</v>
+        <v>23912531</v>
       </c>
       <c r="C30" s="1">
-        <v>850000000</v>
+        <v>1447549808.22</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1786,7 +1789,7 @@
         <v>4</v>
       </c>
       <c r="C31" s="1">
-        <v>105350005.37</v>
+        <v>49162220.68</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1794,10 +1797,10 @@
         <v>36</v>
       </c>
       <c r="B32" s="1">
-        <v>23476856</v>
+        <v>23912531</v>
       </c>
       <c r="C32" s="1">
-        <v>105350005.37</v>
+        <v>49162220.68</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1808,7 +1811,7 @@
         <v>4</v>
       </c>
       <c r="C33" s="1">
-        <v>32422510.530000001</v>
+        <v>32671206.449999999</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1816,10 +1819,10 @@
         <v>38</v>
       </c>
       <c r="B34" s="1">
-        <v>99206637</v>
+        <v>100562863</v>
       </c>
       <c r="C34" s="1">
-        <v>32422510.530000001</v>
+        <v>32671206.449999999</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1850,10 +1853,10 @@
         <v>42</v>
       </c>
       <c r="C37" s="1">
-        <v>917089</v>
+        <v>925888</v>
       </c>
       <c r="D37" s="1">
-        <v>7310.7</v>
+        <v>7270.7</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>43</v>
@@ -1870,7 +1873,7 @@
         <v>45</v>
       </c>
       <c r="C38" s="1">
-        <v>917089</v>
+        <v>925888</v>
       </c>
       <c r="D38" s="1">
         <v>970.8</v>
@@ -1890,7 +1893,7 @@
         <v>47</v>
       </c>
       <c r="C39" s="1">
-        <v>917089</v>
+        <v>925888</v>
       </c>
       <c r="D39" s="1">
         <v>829.68</v>
@@ -1910,16 +1913,16 @@
         <v>49</v>
       </c>
       <c r="C40" s="1">
-        <v>917089</v>
+        <v>925888</v>
       </c>
       <c r="D40" s="1">
-        <v>52.81</v>
+        <v>80.569999999999993</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>51</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1927,39 +1930,39 @@
         <v>5</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C41" s="1">
+        <v>925888</v>
+      </c>
+      <c r="D41" s="1">
+        <v>37.01</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="C41" s="1">
-        <v>917089</v>
-      </c>
-      <c r="D41" s="1">
-        <v>180</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>53</v>
       </c>
       <c r="C42" s="1">
-        <v>76195906</v>
+        <v>925888</v>
       </c>
       <c r="D42" s="1">
-        <v>10478.5</v>
+        <v>180</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>54</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1967,39 +1970,39 @@
         <v>6</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C43" s="1">
+        <v>77952195</v>
+      </c>
+      <c r="D43" s="1">
+        <v>10825.93</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F43" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="C43" s="1">
-        <v>76195906</v>
-      </c>
-      <c r="D43" s="1">
-        <v>51</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="1" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C44" s="1">
-        <v>76195906</v>
+        <v>77952195</v>
       </c>
       <c r="D44" s="1">
-        <v>1082060842.4000001</v>
+        <v>126</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>57</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -2007,19 +2010,19 @@
         <v>21</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C45" s="1">
-        <v>76195906</v>
+        <v>77952195</v>
       </c>
       <c r="D45" s="1">
-        <v>1126523930.4300001</v>
+        <v>1082067000.8800001</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>43</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -2027,19 +2030,19 @@
         <v>21</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C46" s="1">
-        <v>76195906</v>
+        <v>77952195</v>
       </c>
       <c r="D46" s="1">
-        <v>15049612.199999999</v>
+        <v>40828.28</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>43</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -2047,19 +2050,19 @@
         <v>21</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C47" s="1">
-        <v>76195906</v>
+        <v>77952195</v>
       </c>
       <c r="D47" s="1">
-        <v>1705110564.0899999</v>
+        <v>17079810.449999999</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>43</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -2067,19 +2070,19 @@
         <v>21</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C48" s="1">
-        <v>76195906</v>
+        <v>77952195</v>
       </c>
       <c r="D48" s="1">
-        <v>1434482060.2</v>
+        <v>1705110564.0899999</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>43</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -2087,19 +2090,19 @@
         <v>21</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C49" s="1">
-        <v>76195906</v>
+        <v>77952195</v>
       </c>
       <c r="D49" s="1">
-        <v>1071235028.75</v>
+        <v>1434482060.2</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>43</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -2107,19 +2110,19 @@
         <v>21</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C50" s="1">
-        <v>76195906</v>
+        <v>77952195</v>
       </c>
       <c r="D50" s="1">
-        <v>1070374107.72</v>
+        <v>1071243765.73</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>43</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -2127,19 +2130,19 @@
         <v>21</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C51" s="1">
-        <v>76195906</v>
+        <v>77952195</v>
       </c>
       <c r="D51" s="1">
-        <v>1064063350.5599999</v>
+        <v>1070376686.22</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>43</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -2147,59 +2150,59 @@
         <v>21</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C52" s="1">
-        <v>76195906</v>
+        <v>77952195</v>
       </c>
       <c r="D52" s="1">
-        <v>1570889775.0799999</v>
+        <v>1064069509.04</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>43</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C53" s="1">
-        <v>75332174</v>
+        <v>77952195</v>
       </c>
       <c r="D53" s="1">
-        <v>922473805.94000006</v>
+        <v>1570889775.0799999</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>43</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C54" s="1">
-        <v>23476856</v>
+        <v>75332174</v>
       </c>
       <c r="D54" s="1">
-        <v>1121.1099999999999</v>
+        <v>922473805.94000006</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>43</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -2207,19 +2210,19 @@
         <v>10</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C55" s="1">
+        <v>23912531</v>
+      </c>
+      <c r="D55" s="1">
+        <v>1261.0899999999999</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F55" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="C55" s="1">
-        <v>23476856</v>
-      </c>
-      <c r="D55" s="1">
-        <v>8881.1</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -2229,17 +2232,17 @@
       <c r="B56" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>4</v>
+      <c r="C56" s="1">
+        <v>23912531</v>
+      </c>
+      <c r="D56" s="1">
+        <v>48.89</v>
       </c>
       <c r="E56" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F56" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -2247,19 +2250,19 @@
         <v>10</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>4</v>
+        <v>79</v>
+      </c>
+      <c r="C57" s="1">
+        <v>23912531</v>
+      </c>
+      <c r="D57" s="1">
+        <v>8591.09</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>81</v>
+        <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -2267,19 +2270,19 @@
         <v>10</v>
       </c>
       <c r="B58" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F58" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -2287,19 +2290,19 @@
         <v>10</v>
       </c>
       <c r="B59" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F59" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -2307,119 +2310,119 @@
         <v>10</v>
       </c>
       <c r="B60" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F60" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="C60" s="1">
-        <v>23476856</v>
-      </c>
-      <c r="D60" s="1">
-        <v>604.63</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C61" s="1">
-        <v>23476856</v>
-      </c>
-      <c r="D61" s="1">
-        <v>29984.62</v>
+        <v>87</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>43</v>
+        <v>81</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C62" s="1">
-        <v>23476856</v>
+        <v>23912531</v>
       </c>
       <c r="D62" s="1">
-        <v>33551.57</v>
+        <v>520.4</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>4</v>
+        <v>90</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C63" s="1">
-        <v>23476856</v>
+        <v>23912531</v>
       </c>
       <c r="D63" s="1">
-        <v>40876.839999999997</v>
+        <v>8449.5400000000009</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>43</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="C64" s="1">
-        <v>23476856</v>
+        <v>23912531</v>
       </c>
       <c r="D64" s="1">
-        <v>274763650000</v>
+        <v>28687.95</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>75</v>
+        <v>4</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C65" s="1">
-        <v>23476856</v>
+        <v>23912531</v>
       </c>
       <c r="D65" s="1">
-        <v>7867786185.4399996</v>
+        <v>71116.38</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -2427,59 +2430,59 @@
         <v>15</v>
       </c>
       <c r="B66" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C66" s="1">
+        <v>23912531</v>
+      </c>
+      <c r="D66" s="1">
+        <v>299675650000</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F66" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="C66" s="1">
-        <v>23476856</v>
-      </c>
-      <c r="D66" s="1">
-        <v>513239341638</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>4</v>
+        <v>89</v>
+      </c>
+      <c r="C67" s="1">
+        <v>23912531</v>
+      </c>
+      <c r="D67" s="1">
+        <v>3547760400.8099999</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>4</v>
+        <v>79</v>
+      </c>
+      <c r="C68" s="1">
+        <v>23912531</v>
+      </c>
+      <c r="D68" s="1">
+        <v>554559341638</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>81</v>
+        <v>4</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -2487,19 +2490,19 @@
         <v>10</v>
       </c>
       <c r="B69" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F69" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -2507,59 +2510,59 @@
         <v>10</v>
       </c>
       <c r="B70" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F70" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C71" s="1">
-        <v>76195906</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>43</v>
+        <v>81</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>54</v>
+        <v>86</v>
       </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C72" s="1">
-        <v>76195906</v>
-      </c>
-      <c r="D72" s="1">
-        <v>312313000000</v>
+        <v>87</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>4</v>
+        <v>81</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>4</v>
+        <v>88</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -2567,33 +2570,33 @@
         <v>16</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>90</v>
+        <v>54</v>
       </c>
       <c r="C73" s="1">
-        <v>76195906</v>
-      </c>
-      <c r="D73" s="1">
-        <v>150611910359.92001</v>
+        <v>77952195</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>91</v>
+        <v>55</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>92</v>
+        <v>56</v>
       </c>
       <c r="C74" s="1">
-        <v>370291757</v>
+        <v>77952195</v>
       </c>
       <c r="D74" s="1">
-        <v>41550.97</v>
+        <v>1179142000000</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>4</v>
@@ -2604,22 +2607,22 @@
     </row>
     <row r="75" spans="1:6">
       <c r="A75" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>93</v>
       </c>
       <c r="C75" s="1">
-        <v>370291757</v>
+        <v>77952195</v>
       </c>
       <c r="D75" s="1">
-        <v>1673.88</v>
+        <v>235820314159.44</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>4</v>
+        <v>94</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -2627,13 +2630,13 @@
         <v>19</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C76" s="1">
-        <v>370291757</v>
+        <v>383565184</v>
       </c>
       <c r="D76" s="1">
-        <v>257814.62</v>
+        <v>27450.97</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>4</v>
@@ -2644,16 +2647,16 @@
     </row>
     <row r="77" spans="1:6">
       <c r="A77" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C77" s="1">
-        <v>370291757</v>
+        <v>383565184</v>
       </c>
       <c r="D77" s="1">
-        <v>757814.62</v>
+        <v>2931.34</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>4</v>
@@ -2664,16 +2667,16 @@
     </row>
     <row r="78" spans="1:6">
       <c r="A78" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="C78" s="1">
-        <v>23326594</v>
+        <v>383565184</v>
       </c>
       <c r="D78" s="1">
-        <v>8294000</v>
+        <v>327462.52</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>4</v>
@@ -2684,22 +2687,22 @@
     </row>
     <row r="79" spans="1:6">
       <c r="A79" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>74</v>
+        <v>97</v>
       </c>
       <c r="C79" s="1">
-        <v>23326594</v>
+        <v>370291757</v>
       </c>
       <c r="D79" s="1">
-        <v>3886000</v>
+        <v>757814.62</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>75</v>
+        <v>4</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -2707,273 +2710,273 @@
         <v>24</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C80" s="1">
-        <v>23326594</v>
+        <v>23912531</v>
       </c>
       <c r="D80" s="1">
-        <v>1156481.23</v>
+        <v>6666000</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>87</v>
+        <v>4</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C81" s="1">
-        <v>23326594</v>
+        <v>23912531</v>
       </c>
       <c r="D81" s="1">
-        <v>22286475.800000001</v>
+        <v>2004.81</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>43</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="C82" s="1">
-        <v>76195906</v>
+        <v>23912531</v>
       </c>
       <c r="D82" s="1">
-        <v>38802928.560000002</v>
+        <v>8652000</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>43</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C83" s="1">
-        <v>69548271</v>
+        <v>23912531</v>
       </c>
       <c r="D83" s="1">
-        <v>153657.43</v>
+        <v>945652.09</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>4</v>
+        <v>90</v>
       </c>
     </row>
     <row r="84" spans="1:6">
       <c r="A84" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="C84" s="1">
-        <v>76195906</v>
+        <v>23326594</v>
       </c>
       <c r="D84" s="1">
-        <v>96071462.310000002</v>
+        <v>29807884.100000001</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>43</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85" s="1" t="s">
-        <v>96</v>
+        <v>26</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="C85" s="1">
-        <v>23476856</v>
+        <v>69863728</v>
       </c>
       <c r="D85" s="1">
-        <v>3211393.58</v>
+        <v>2537000</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>87</v>
+        <v>4</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86" s="1" t="s">
-        <v>96</v>
+        <v>26</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C86" s="1">
-        <v>23476856</v>
+        <v>69863728</v>
       </c>
       <c r="D86" s="1">
-        <v>1045412.19</v>
+        <v>3733285</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="87" spans="1:6">
       <c r="A87" s="1" t="s">
-        <v>96</v>
+        <v>29</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="C87" s="1">
-        <v>23476856</v>
+        <v>77952195</v>
       </c>
       <c r="D87" s="1">
-        <v>12476034.210000001</v>
+        <v>18203565.989999998</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
     </row>
     <row r="88" spans="1:6">
       <c r="A88" s="1" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>4</v>
+        <v>101</v>
+      </c>
+      <c r="C88" s="1">
+        <v>72861177</v>
+      </c>
+      <c r="D88" s="1">
+        <v>906956</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>79</v>
+        <v>4</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="A89" s="1" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>4</v>
+        <v>54</v>
+      </c>
+      <c r="C89" s="1">
+        <v>76195906</v>
+      </c>
+      <c r="D89" s="1">
+        <v>96071462.310000002</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>78</v>
+        <v>43</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
     </row>
     <row r="90" spans="1:6">
       <c r="A90" s="1" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>4</v>
+        <v>75</v>
+      </c>
+      <c r="C90" s="1">
+        <v>23912531</v>
+      </c>
+      <c r="D90" s="1">
+        <v>90000001.019999996</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>78</v>
+        <v>43</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="91" spans="1:6">
       <c r="A91" s="1" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>4</v>
+        <v>89</v>
+      </c>
+      <c r="C91" s="1">
+        <v>23912531</v>
+      </c>
+      <c r="D91" s="1">
+        <v>3931165.32</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="92" spans="1:6">
       <c r="A92" s="1" t="s">
-        <v>31</v>
+        <v>102</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="C92" s="1">
-        <v>76195906</v>
+        <v>23912531</v>
       </c>
       <c r="D92" s="1">
-        <v>50000015.600000001</v>
+        <v>1045412.19</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>4</v>
+        <v>78</v>
       </c>
     </row>
     <row r="93" spans="1:6">
       <c r="A93" s="1" t="s">
-        <v>31</v>
+        <v>102</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="C93" s="1">
-        <v>76195906</v>
+        <v>23912531</v>
       </c>
       <c r="D93" s="1">
-        <v>39055483.100000001</v>
+        <v>53874001.119999997</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>4</v>
@@ -2984,10 +2987,10 @@
     </row>
     <row r="94" spans="1:6">
       <c r="A94" s="1" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>4</v>
@@ -2996,18 +2999,18 @@
         <v>4</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
     </row>
     <row r="95" spans="1:6">
       <c r="A95" s="1" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>4</v>
@@ -3016,18 +3019,18 @@
         <v>4</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
     </row>
     <row r="96" spans="1:6">
       <c r="A96" s="1" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>4</v>
@@ -3036,204 +3039,204 @@
         <v>4</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
     </row>
     <row r="97" spans="1:6">
       <c r="A97" s="1" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C97" s="1">
-        <v>76195906</v>
-      </c>
-      <c r="D97" s="1">
-        <v>3461703.62</v>
+        <v>87</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>50</v>
+        <v>81</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="98" spans="1:6">
       <c r="A98" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="C98" s="1">
-        <v>23476856</v>
+        <v>77952195</v>
       </c>
       <c r="D98" s="1">
-        <v>311057063.38</v>
+        <v>68766001</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>75</v>
+        <v>4</v>
       </c>
     </row>
     <row r="99" spans="1:6">
       <c r="A99" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C99" s="1">
-        <v>3442409</v>
-      </c>
-      <c r="D99" s="1">
-        <v>850000000</v>
+        <v>103</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>43</v>
+        <v>81</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
     </row>
     <row r="100" spans="1:6">
       <c r="A100" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B100" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F100" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="C100" s="1">
-        <v>99206637</v>
-      </c>
-      <c r="D100" s="1">
-        <v>31587852.739999998</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F100" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="101" spans="1:6">
       <c r="A101" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C101" s="1">
-        <v>99206637</v>
-      </c>
-      <c r="D101" s="1">
-        <v>687036.19</v>
+      <c r="C101" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>4</v>
+        <v>81</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>4</v>
+        <v>108</v>
       </c>
     </row>
     <row r="102" spans="1:6">
       <c r="A102" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="C102" s="1">
-        <v>99206637</v>
+        <v>77952195</v>
       </c>
       <c r="D102" s="1">
-        <v>147621.6</v>
+        <v>2714687.72</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>4</v>
+        <v>94</v>
       </c>
     </row>
     <row r="103" spans="1:6">
       <c r="A103" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B103" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C103" s="1">
+        <v>23912531</v>
+      </c>
+      <c r="D103" s="1">
+        <v>1447549808.22</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F103" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="C103" s="1">
-        <v>23476856</v>
-      </c>
-      <c r="D103" s="1">
-        <v>62438002</v>
-      </c>
-      <c r="E103" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F103" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="104" spans="1:6">
       <c r="A104" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>74</v>
+        <v>109</v>
       </c>
       <c r="C104" s="1">
-        <v>23476856</v>
+        <v>100562863</v>
       </c>
       <c r="D104" s="1">
-        <v>42156000</v>
+        <v>31387852.739999998</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>75</v>
+        <v>4</v>
       </c>
     </row>
     <row r="105" spans="1:6">
       <c r="A105" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="C105" s="1">
-        <v>23476856</v>
+        <v>100562863</v>
       </c>
       <c r="D105" s="1">
-        <v>756003.37</v>
+        <v>1099001</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>87</v>
+        <v>4</v>
       </c>
     </row>
     <row r="106" spans="1:6">
       <c r="A106" s="1" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C106" s="1">
-        <v>5898541</v>
+        <v>100562863</v>
       </c>
       <c r="D106" s="1">
-        <v>18558000.760000002</v>
+        <v>184352.71</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>4</v>
@@ -3244,16 +3247,16 @@
     </row>
     <row r="107" spans="1:6">
       <c r="A107" s="1" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>110</v>
+        <v>79</v>
       </c>
       <c r="C107" s="1">
-        <v>5898541</v>
+        <v>23912531</v>
       </c>
       <c r="D107" s="1">
-        <v>277751003.25999999</v>
+        <v>4374002</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>4</v>
@@ -3264,42 +3267,42 @@
     </row>
     <row r="108" spans="1:6">
       <c r="A108" s="1" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="C108" s="1">
-        <v>5898541</v>
+        <v>23912531</v>
       </c>
       <c r="D108" s="1">
-        <v>7499952.3300000001</v>
+        <v>42156000</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>4</v>
+        <v>76</v>
       </c>
     </row>
     <row r="109" spans="1:6">
       <c r="A109" s="1" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="C109" s="1">
-        <v>5898541</v>
+        <v>23912531</v>
       </c>
       <c r="D109" s="1">
-        <v>2866994</v>
+        <v>2632218.6800000002</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>4</v>
+        <v>90</v>
       </c>
     </row>
     <row r="110" spans="1:6">
@@ -3307,13 +3310,13 @@
         <v>8</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C110" s="1">
-        <v>5898541</v>
+        <v>5981741</v>
       </c>
       <c r="D110" s="1">
-        <v>2647816.5299999998</v>
+        <v>13066000.76</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>4</v>
@@ -3327,13 +3330,13 @@
         <v>8</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C111" s="1">
-        <v>5898541</v>
+        <v>5981741</v>
       </c>
       <c r="D111" s="1">
-        <v>1457329.63</v>
+        <v>332468003.27999997</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>4</v>
@@ -3347,13 +3350,13 @@
         <v>8</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C112" s="1">
-        <v>5898541</v>
+        <v>5981741</v>
       </c>
       <c r="D112" s="1">
-        <v>850746.71</v>
+        <v>134072.28</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>4</v>
@@ -3367,13 +3370,13 @@
         <v>8</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C113" s="1">
-        <v>5898541</v>
+        <v>5981741</v>
       </c>
       <c r="D113" s="1">
-        <v>2146027.41</v>
+        <v>2866994</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>4</v>
@@ -3387,13 +3390,13 @@
         <v>8</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C114" s="1">
-        <v>5898541</v>
+        <v>5981741</v>
       </c>
       <c r="D114" s="1">
-        <v>1066964.3</v>
+        <v>2647816.5299999998</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>4</v>
@@ -3407,13 +3410,13 @@
         <v>8</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C115" s="1">
-        <v>5898541</v>
+        <v>5981741</v>
       </c>
       <c r="D115" s="1">
-        <v>538350.48</v>
+        <v>1457329.63</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>4</v>
@@ -3427,13 +3430,13 @@
         <v>8</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C116" s="1">
-        <v>5898541</v>
+        <v>5981741</v>
       </c>
       <c r="D116" s="1">
-        <v>1139517.8999999999</v>
+        <v>850746.71</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>4</v>
@@ -3447,13 +3450,13 @@
         <v>8</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C117" s="1">
-        <v>5898541</v>
+        <v>5981741</v>
       </c>
       <c r="D117" s="1">
-        <v>1415882.02</v>
+        <v>1066964.3</v>
       </c>
       <c r="E117" s="1" t="s">
         <v>4</v>
@@ -3467,13 +3470,13 @@
         <v>8</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C118" s="1">
-        <v>5898541</v>
+        <v>5981741</v>
       </c>
       <c r="D118" s="1">
-        <v>127419.44</v>
+        <v>538350.48</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>4</v>
@@ -3487,13 +3490,13 @@
         <v>8</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C119" s="1">
-        <v>5898541</v>
+        <v>5981741</v>
       </c>
       <c r="D119" s="1">
-        <v>701267.06</v>
+        <v>168809.44</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>4</v>
@@ -3507,13 +3510,13 @@
         <v>8</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C120" s="1">
-        <v>5898541</v>
+        <v>5981741</v>
       </c>
       <c r="D120" s="1">
-        <v>412420.03</v>
+        <v>127419.44</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>4</v>
@@ -3527,13 +3530,13 @@
         <v>8</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C121" s="1">
-        <v>5898541</v>
+        <v>5981741</v>
       </c>
       <c r="D121" s="1">
-        <v>1926995.04</v>
+        <v>337972.77</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>4</v>
@@ -3547,13 +3550,13 @@
         <v>8</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C122" s="1">
-        <v>5898541</v>
+        <v>5981741</v>
       </c>
       <c r="D122" s="1">
-        <v>68603667.329999998</v>
+        <v>66276570.240000002</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>4</v>
@@ -3567,13 +3570,13 @@
         <v>8</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C123" s="1">
-        <v>5898541</v>
+        <v>5981741</v>
       </c>
       <c r="D123" s="1">
-        <v>5519998.04</v>
+        <v>579364.13</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>4</v>
@@ -3587,13 +3590,13 @@
         <v>8</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C124" s="1">
-        <v>5898541</v>
+        <v>5981741</v>
       </c>
       <c r="D124" s="1">
-        <v>2786999.81</v>
+        <v>5369989.6900000004</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>4</v>
@@ -3607,13 +3610,13 @@
         <v>8</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C125" s="1">
-        <v>5898541</v>
+        <v>5981741</v>
       </c>
       <c r="D125" s="1">
-        <v>2655996.87</v>
+        <v>2515998.2799999998</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>4</v>
@@ -3627,13 +3630,13 @@
         <v>8</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C126" s="1">
-        <v>5898541</v>
+        <v>5981741</v>
       </c>
       <c r="D126" s="1">
-        <v>2547998.9900000002</v>
+        <v>2404999.81</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>4</v>
@@ -3647,13 +3650,13 @@
         <v>8</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C127" s="1">
-        <v>5898541</v>
+        <v>5981741</v>
       </c>
       <c r="D127" s="1">
-        <v>1968999.52</v>
+        <v>1754998.02</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>4</v>
@@ -3667,13 +3670,13 @@
         <v>8</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C128" s="1">
-        <v>5898541</v>
+        <v>5981741</v>
       </c>
       <c r="D128" s="1">
-        <v>1664999.66</v>
+        <v>1012992.59</v>
       </c>
       <c r="E128" s="1" t="s">
         <v>4</v>
@@ -3687,13 +3690,13 @@
         <v>8</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C129" s="1">
-        <v>5898541</v>
+        <v>5981741</v>
       </c>
       <c r="D129" s="1">
-        <v>1346999.81</v>
+        <v>982999.48</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>4</v>
@@ -3707,13 +3710,13 @@
         <v>8</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C130" s="1">
-        <v>5898541</v>
+        <v>5981741</v>
       </c>
       <c r="D130" s="1">
-        <v>1329999.81</v>
+        <v>981999.81</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>4</v>
@@ -3727,13 +3730,13 @@
         <v>8</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C131" s="1">
-        <v>5898541</v>
+        <v>5981741</v>
       </c>
       <c r="D131" s="1">
-        <v>625999.81000000006</v>
+        <v>783999.48</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>4</v>
@@ -3747,18 +3750,58 @@
         <v>8</v>
       </c>
       <c r="B132" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C132" s="1">
+        <v>5981741</v>
+      </c>
+      <c r="D132" s="1">
+        <v>643999.14</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F132" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6">
+      <c r="A133" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B133" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C132" s="1">
-        <v>5898541</v>
-      </c>
-      <c r="D132" s="1">
-        <v>579364.13</v>
-      </c>
-      <c r="E132" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F132" s="1" t="s">
+      <c r="C133" s="1">
+        <v>5981741</v>
+      </c>
+      <c r="D133" s="1">
+        <v>553998.73</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F133" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6">
+      <c r="A134" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C134" s="1">
+        <v>5981741</v>
+      </c>
+      <c r="D134" s="1">
+        <v>256999.81</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F134" s="1" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update snapshot 20260101; add support ERC20-AETHUSDC jWBTC-TRC20; update dependencies; fix security vulnerabilities; add SECURITY.md; update README.md
</commit_message>
<xml_diff>
--- a/snapshot/huobi_por.xlsx
+++ b/snapshot/huobi_por.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiangliqiang/Repo/Tool-Node.js-VerifyAddress/snapshot/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Zhuanz/Code/wallet/huobi/Tool-Node.js-VerifyAddress/snapshot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D6D7D5B9-6067-124F-B29C-FFD57D228FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5C92D6-B35F-BA45-9CC9-BC83C4514A1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{411BB281-6367-B440-9EF5-E7547829EACC}"/>
+    <workbookView xWindow="1960" yWindow="1260" windowWidth="28800" windowHeight="16360" xr2:uid="{411BB281-6367-B440-9EF5-E7547829EACC}"/>
   </bookViews>
   <sheets>
     <sheet name="huobi_por" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="134">
   <si>
     <t>coin</t>
   </si>
@@ -64,18 +64,12 @@
     <t>HTX(ALL)</t>
   </si>
   <si>
-    <t>264152465223381.00</t>
-  </si>
-  <si>
     <t>HTX-ERC20</t>
   </si>
   <si>
     <t>HTX-TRC20</t>
   </si>
   <si>
-    <t>263294682471342.00</t>
-  </si>
-  <si>
     <t>SOL(All)</t>
   </si>
   <si>
@@ -103,9 +97,6 @@
     <t>BEP20-USDC</t>
   </si>
   <si>
-    <t>USDC-SOL</t>
-  </si>
-  <si>
     <t>USDT(ALL)</t>
   </si>
   <si>
@@ -199,12 +190,6 @@
     <t>24d160af1f9f0c4ff530f85f6ed0850927727a7a4a576918d1d502c2af3eb4227417b1527e5eb5aae09529935d0662b5775d5f67db06d46ac34ee7e127c1582901</t>
   </si>
   <si>
-    <t>TCQQjfccKdMi4CnPAzmZW5TALH4HbwceVb</t>
-  </si>
-  <si>
-    <t>4d3baf9ceb963cb5224005d1f1dc769bbb57c4710ffe5a2432d46c9b8ad22cd90ae94a5f53af14314b68808802aa944a4a99b0c5c181e95b87f32a3f0aeefef700</t>
-  </si>
-  <si>
     <t>TGn1uvntAVntT1pG8o7qoKkbViiYfeg6Gj</t>
   </si>
   <si>
@@ -298,9 +283,6 @@
     <t>0x6663613fbd927ce78abbf7f5ca7e2c3fe0d96d18</t>
   </si>
   <si>
-    <t>261879720157182.00</t>
-  </si>
-  <si>
     <t>TFTWNgDBkQ5wQoP8RXpRznnHvAVV8x5jLu</t>
   </si>
   <si>
@@ -364,9 +346,6 @@
     <t>DRRU8L7fF4k9w7SF3Z6ei8onPCsh9hjGX1</t>
   </si>
   <si>
-    <t>DJX3kCZfcDuREturnUNKEBQELi1PFaLkJC</t>
-  </si>
-  <si>
     <t>DN4FUEu7L9PpcnMntidGXNvasjUEyWV77F</t>
   </si>
   <si>
@@ -385,9 +364,6 @@
     <t>DSqzssxy31fpuGFJfZjoM6TqP38oNPAPiN</t>
   </si>
   <si>
-    <t>DLzCvKskasu4Adj3XgbyNitKBukBSa5JPP</t>
-  </si>
-  <si>
     <t>DB5KWytcxHyphHPn9iC92Y9JqPRL1Fq21p</t>
   </si>
   <si>
@@ -400,43 +376,62 @@
     <t>DM17LVDVnSUxaVncoYNWLjsSq5bYSWDwmy</t>
   </si>
   <si>
-    <t>A1NxyPuaxiPm24RJR1DYU7tVYwcFqRtgEf</t>
-  </si>
-  <si>
-    <t>9xzSxYs2w8s6EGbzrj1qXgoSefbc9B4u4Z</t>
-  </si>
-  <si>
-    <t>9uCrSKxDtYQb3ogf4Z93qQcnihy5mzwGMs</t>
-  </si>
-  <si>
-    <t>AFAocif1boV7t9NQsSJuZFj1MjAMugurAJ</t>
-  </si>
-  <si>
-    <t>9tezKrvR5zoYv5sc67KWRi5fUwSdM7nHnF</t>
-  </si>
-  <si>
-    <t>9vjmf33smeHJksTLiDZ9xbD6AQtqxB6NAB</t>
-  </si>
-  <si>
-    <t>A6z32fmFDejWyQfQH3Vp9bxQjJ8Qw2Ad4c</t>
-  </si>
-  <si>
-    <t>AFERVSFd9Q3aBX3sWUMbfVWnrcCVyBrUMv</t>
-  </si>
-  <si>
-    <t>A7HHQEqvdZugErQmVPRpZ5VP6sHH7ziKN1</t>
-  </si>
-  <si>
-    <t>A96kc8NYE8itzvo14dbrnBv8UDusU71hQW</t>
-  </si>
-  <si>
-    <t>9vhUDyKZ3ths23UeDNUxRBUMaVvCEsAkFr</t>
+    <t>jWBTC-TRC20</t>
+  </si>
+  <si>
+    <t>ERC20-AETHUSDC</t>
+  </si>
+  <si>
+    <t>1HckjUpRGcrrRAtFaaCAUaGjsPx9oYmLaZ</t>
+  </si>
+  <si>
+    <t>IJtEWgK2V8QxKUCWpVlfMTpVhwS2My/2Notvcw2lPBuHACHkxUESh8BoPL1vzQ4hkqYg/EZbQm9hpPKKcZJwY7E=</t>
+  </si>
+  <si>
+    <t>260029720157182.81</t>
+  </si>
+  <si>
+    <t>DQhEuTa5UkNcD8YFZK3pvjFfrtMqQpJhSa</t>
+  </si>
+  <si>
+    <t>DKs2WBbiaAEe9RGzQTmtJj1o9bqsKTUTtC</t>
+  </si>
+  <si>
+    <t>A6MxoQbb4GanMdLRxLkexZC7m2DBH629fY</t>
+  </si>
+  <si>
+    <t>9sFCBgBszYBeFSQLdSQdSEPA35ZCfPLiCd</t>
+  </si>
+  <si>
+    <t>AAdvDHUdAAcCRRrhH6mDWdM3cvjzbLHsPJ</t>
+  </si>
+  <si>
+    <t>AAYU7frmWQPspbvbKU9BPFY5u1xsgTYMQN</t>
+  </si>
+  <si>
+    <t>A6tCf4eW82xEY91vCJEmHFr8RoH2mv8gbg</t>
+  </si>
+  <si>
+    <t>A6b5c1rmmWFjHbpwj6KXaJUjJTHJwsqVDu</t>
+  </si>
+  <si>
+    <t>9xcnXTBYyJRG3oFDJRyTX994o8rbQZ9ELi</t>
+  </si>
+  <si>
+    <t>9wRLiu1JnbvKw73K3rETWou6titXYUrKbJ</t>
+  </si>
+  <si>
+    <t>9xcUwVrSxhx6ckM8BhcvpdEfT2r5CyfJVE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
+    <numFmt numFmtId="177" formatCode="0.00_);[Red]\(0.00\)"/>
+  </numFmts>
   <fonts count="20">
     <font>
       <sz val="12"/>
@@ -1047,18 +1042,33 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1435,30 +1445,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{551DE6D8-23DE-D340-B153-F7BA258674FF}">
-  <dimension ref="A1:F134"/>
+  <dimension ref="A1:F131"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:F36"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="132" workbookViewId="0">
+      <selection activeCell="D87" sqref="D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="23.1640625" customWidth="1"/>
     <col min="2" max="2" width="52.5" customWidth="1"/>
-    <col min="3" max="3" width="18.83203125" customWidth="1"/>
-    <col min="4" max="4" width="16.1640625" customWidth="1"/>
+    <col min="3" max="3" width="27.1640625" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
     <col min="5" max="5" width="16.33203125" customWidth="1"/>
     <col min="6" max="6" width="136.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1469,8 +1479,8 @@
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1">
-        <v>20320.689999999999</v>
+      <c r="C2" s="5">
+        <v>20397.22</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1478,10 +1488,10 @@
         <v>5</v>
       </c>
       <c r="B3" s="1">
-        <v>925888</v>
-      </c>
-      <c r="C3" s="1">
-        <v>9368.77</v>
+        <v>930288</v>
+      </c>
+      <c r="C3" s="5">
+        <v>9793.2999999999993</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1489,380 +1499,371 @@
         <v>6</v>
       </c>
       <c r="B4" s="1">
-        <v>77952195</v>
-      </c>
-      <c r="C4" s="1">
-        <v>10951.93</v>
+        <v>78844633</v>
+      </c>
+      <c r="C4" s="5">
+        <v>10514.93</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1">
-        <v>439849388.82999998</v>
+        <v>118</v>
+      </c>
+      <c r="B5" s="1">
+        <v>78844633</v>
+      </c>
+      <c r="C5" s="5">
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="1">
-        <v>5981741</v>
-      </c>
-      <c r="C6" s="1">
-        <v>439849388.82999998</v>
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="5">
+        <v>460086642.47000003</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="1">
-        <v>118675.34</v>
+        <v>8</v>
+      </c>
+      <c r="B7" s="1">
+        <v>6023980</v>
+      </c>
+      <c r="C7" s="5">
+        <v>460086642.47000003</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="1">
-        <v>23912531</v>
-      </c>
-      <c r="C8" s="1">
-        <v>10421.459999999999</v>
+        <v>9</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="5">
+        <v>125756.86</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1">
-        <v>23912531</v>
-      </c>
-      <c r="C9" s="1">
-        <v>8449.5400000000009</v>
+        <v>24133662</v>
+      </c>
+      <c r="C9" s="5">
+        <v>15887.45</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" s="1">
-        <v>23912531</v>
-      </c>
-      <c r="C10" s="1">
-        <v>99804.33</v>
+        <v>24133662</v>
+      </c>
+      <c r="C10" s="5">
+        <v>9848.5400000000009</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+      <c r="B11" s="1">
+        <v>24133662</v>
+      </c>
+      <c r="C11" s="6">
+        <v>100020.87</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="1">
-        <v>23912531</v>
-      </c>
-      <c r="C12" s="1">
-        <v>857782752038.81006</v>
+        <v>13</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="7">
+        <v>263047306759681</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B13" s="1">
-        <v>77952195</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>17</v>
+        <v>24133662</v>
+      </c>
+      <c r="C13" s="7">
+        <v>887452525329.31995</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="1">
-        <v>357844.83</v>
+        <v>15</v>
+      </c>
+      <c r="B14" s="1">
+        <v>78844633</v>
+      </c>
+      <c r="C14" s="8">
+        <v>262159854234352</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="1">
-        <v>383565184</v>
-      </c>
-      <c r="C15" s="1">
-        <v>357844.83</v>
+        <v>16</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="5">
+        <v>363818.58</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="1">
-        <v>9937833805.9300003</v>
+        <v>17</v>
+      </c>
+      <c r="B16" s="1">
+        <v>390417216</v>
+      </c>
+      <c r="C16" s="5">
+        <v>363818.58</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="1">
-        <v>77952195</v>
-      </c>
-      <c r="C17" s="1">
-        <v>9015359999.9799995</v>
+        <v>18</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="5">
+        <v>9940804554.1800003</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B18" s="1">
-        <v>75332174</v>
-      </c>
-      <c r="C18" s="1">
-        <v>922473805.94000006</v>
+        <v>78844633</v>
+      </c>
+      <c r="C18" s="5">
+        <v>9018330748.2399998</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="1">
-        <v>53101640.619999997</v>
+        <v>20</v>
+      </c>
+      <c r="B19" s="1">
+        <v>78844633</v>
+      </c>
+      <c r="C19" s="5">
+        <v>922473805.94000006</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="1">
-        <v>23912531</v>
-      </c>
-      <c r="C20" s="1">
-        <v>16265656.890000001</v>
+        <v>21</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="5">
+        <v>42057071.670000002</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B21" s="1">
-        <v>23326594</v>
-      </c>
-      <c r="C21" s="1">
-        <v>29807884.100000001</v>
+        <v>24133662</v>
+      </c>
+      <c r="C21" s="5">
+        <v>6088171.0999999996</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B22" s="1">
-        <v>69863728</v>
-      </c>
-      <c r="C22" s="1">
-        <v>6270285</v>
+        <v>24133662</v>
+      </c>
+      <c r="C22" s="5">
+        <v>29807884.100000001</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B23" s="1">
-        <v>370291757</v>
-      </c>
-      <c r="C23" s="1">
-        <v>757814.62</v>
+        <v>73539895</v>
+      </c>
+      <c r="C23" s="5">
+        <v>3504160.82</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="1">
-        <v>1783063060.8900001</v>
+        <v>119</v>
+      </c>
+      <c r="B24" s="1">
+        <v>24133662</v>
+      </c>
+      <c r="C24" s="5">
+        <v>2656855.66</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="1">
-        <v>77952195</v>
-      </c>
-      <c r="C25" s="1">
-        <v>18203565.989999998</v>
+        <v>25</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="5">
+        <v>1566324944.5999999</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B26" s="1">
-        <v>72861177</v>
-      </c>
-      <c r="C26" s="1">
-        <v>906956</v>
+        <v>78844633</v>
+      </c>
+      <c r="C26" s="5">
+        <v>18203565.989999998</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B27" s="1">
-        <v>23912531</v>
-      </c>
-      <c r="C27" s="1">
-        <v>148850579.63999999</v>
+        <v>74803670</v>
+      </c>
+      <c r="C27" s="5">
+        <v>244080.67</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B28" s="1">
-        <v>77952195</v>
-      </c>
-      <c r="C28" s="1">
-        <v>71480688.719999999</v>
+        <v>24133662</v>
+      </c>
+      <c r="C28" s="5">
+        <v>430691866.25</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B29" s="1">
-        <v>76195906</v>
-      </c>
-      <c r="C29" s="1">
-        <v>96071462.310000002</v>
+        <v>78844633</v>
+      </c>
+      <c r="C29" s="5">
+        <v>526851010</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B30" s="1">
-        <v>23912531</v>
-      </c>
-      <c r="C30" s="1">
-        <v>1447549808.22</v>
+        <v>78844633</v>
+      </c>
+      <c r="C30" s="5">
+        <v>96071462.310000002</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C31" s="1">
-        <v>49162220.68</v>
+        <v>31</v>
+      </c>
+      <c r="B31" s="1">
+        <v>24133662</v>
+      </c>
+      <c r="C31" s="5">
+        <v>494262959.38</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B32" s="1">
-        <v>23912531</v>
-      </c>
-      <c r="C32" s="1">
-        <v>49162220.68</v>
+        <v>32</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="5">
+        <v>41896243.240000002</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33" s="1">
-        <v>32671206.449999999</v>
+        <v>33</v>
+      </c>
+      <c r="B33" s="1">
+        <v>24133662</v>
+      </c>
+      <c r="C33" s="5">
+        <v>41896243.240000002</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="5">
+        <v>32240579.739999998</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="1">
+        <v>101250049</v>
+      </c>
+      <c r="C35" s="5">
+        <v>32240579.739999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F37" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="B34" s="1">
-        <v>100562863</v>
-      </c>
-      <c r="C34" s="1">
-        <v>32671206.449999999</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C37" s="1">
-        <v>925888</v>
-      </c>
-      <c r="D37" s="1">
-        <v>7270.7</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1870,19 +1871,19 @@
         <v>5</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C38" s="1">
-        <v>925888</v>
-      </c>
-      <c r="D38" s="1">
-        <v>970.8</v>
+        <v>930288</v>
+      </c>
+      <c r="D38" s="5">
+        <v>7680.7</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1890,19 +1891,19 @@
         <v>5</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C39" s="1">
-        <v>925888</v>
-      </c>
-      <c r="D39" s="1">
-        <v>829.68</v>
+        <v>930288</v>
+      </c>
+      <c r="D39" s="5">
+        <v>970.8</v>
       </c>
       <c r="E39" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F39" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1910,19 +1911,19 @@
         <v>5</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>49</v>
+        <v>120</v>
       </c>
       <c r="C40" s="1">
-        <v>925888</v>
-      </c>
-      <c r="D40" s="1">
-        <v>80.569999999999993</v>
+        <v>930288</v>
+      </c>
+      <c r="D40" s="5">
+        <v>11.19</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>4</v>
+        <v>121</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1930,19 +1931,19 @@
         <v>5</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C41" s="1">
-        <v>925888</v>
-      </c>
-      <c r="D41" s="1">
-        <v>37.01</v>
+        <v>930288</v>
+      </c>
+      <c r="D41" s="5">
+        <v>829.68</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1950,13 +1951,13 @@
         <v>5</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C42" s="1">
-        <v>925888</v>
-      </c>
-      <c r="D42" s="1">
-        <v>180</v>
+        <v>930288</v>
+      </c>
+      <c r="D42" s="5">
+        <v>80.569999999999993</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>4</v>
@@ -1967,36 +1968,36 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C43" s="1">
-        <v>77952195</v>
-      </c>
-      <c r="D43" s="1">
-        <v>10825.93</v>
+        <v>930288</v>
+      </c>
+      <c r="D43" s="5">
+        <v>40.35</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C44" s="1">
-        <v>77952195</v>
-      </c>
-      <c r="D44" s="1">
-        <v>126</v>
+        <v>930288</v>
+      </c>
+      <c r="D44" s="5">
+        <v>180</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>4</v>
@@ -2007,242 +2008,242 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="1" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C45" s="1">
-        <v>77952195</v>
-      </c>
-      <c r="D45" s="1">
-        <v>1082067000.8800001</v>
+        <v>78844633</v>
+      </c>
+      <c r="D45" s="5">
+        <v>10393.93</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="1" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C46" s="1">
-        <v>77952195</v>
-      </c>
-      <c r="D46" s="1">
-        <v>40828.28</v>
+        <v>78844633</v>
+      </c>
+      <c r="D46" s="5">
+        <v>121</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>60</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="1" t="s">
-        <v>21</v>
+        <v>118</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C47" s="1">
-        <v>77952195</v>
-      </c>
-      <c r="D47" s="1">
-        <v>17079810.449999999</v>
+        <v>78844633</v>
+      </c>
+      <c r="D47" s="5">
+        <v>89</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C48" s="1">
-        <v>77952195</v>
-      </c>
-      <c r="D48" s="1">
-        <v>1705110564.0899999</v>
+        <v>78844633</v>
+      </c>
+      <c r="D48" s="5">
+        <v>1082070082.8699999</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="C49" s="1">
-        <v>77952195</v>
-      </c>
-      <c r="D49" s="1">
-        <v>1434482060.2</v>
+        <v>78844633</v>
+      </c>
+      <c r="D49" s="5">
+        <v>20079635.449999999</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C50" s="1">
-        <v>77952195</v>
-      </c>
-      <c r="D50" s="1">
-        <v>1071243765.73</v>
+        <v>78844633</v>
+      </c>
+      <c r="D50" s="5">
+        <v>1705110564.0899999</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="C51" s="1">
-        <v>77952195</v>
-      </c>
-      <c r="D51" s="1">
-        <v>1070376686.22</v>
+        <v>78844633</v>
+      </c>
+      <c r="D51" s="5">
+        <v>1434482060.2</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="C52" s="1">
-        <v>77952195</v>
-      </c>
-      <c r="D52" s="1">
-        <v>1064069509.04</v>
+        <v>78844633</v>
+      </c>
+      <c r="D52" s="5">
+        <v>1071248100.5</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C53" s="1">
-        <v>77952195</v>
-      </c>
-      <c r="D53" s="1">
-        <v>1570889775.0799999</v>
+        <v>78844633</v>
+      </c>
+      <c r="D53" s="5">
+        <v>1070377939.01</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C54" s="1">
-        <v>75332174</v>
-      </c>
-      <c r="D54" s="1">
-        <v>922473805.94000006</v>
+        <v>78844633</v>
+      </c>
+      <c r="D54" s="5">
+        <v>1064072591.03</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C55" s="1">
-        <v>23912531</v>
-      </c>
-      <c r="D55" s="1">
-        <v>1261.0899999999999</v>
+        <v>78844633</v>
+      </c>
+      <c r="D55" s="5">
+        <v>1570889775.0799999</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C56" s="1">
-        <v>23912531</v>
-      </c>
-      <c r="D56" s="1">
-        <v>48.89</v>
+        <v>78844633</v>
+      </c>
+      <c r="D56" s="5">
+        <v>922473805.94000006</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -2250,19 +2251,19 @@
         <v>10</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C57" s="1">
-        <v>23912531</v>
-      </c>
-      <c r="D57" s="1">
-        <v>8591.09</v>
+        <v>24133662</v>
+      </c>
+      <c r="D57" s="5">
+        <v>13691.08</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>4</v>
+        <v>71</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -2270,19 +2271,19 @@
         <v>10</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>4</v>
+        <v>74</v>
+      </c>
+      <c r="C58" s="1">
+        <v>24133662</v>
+      </c>
+      <c r="D58" s="5">
+        <v>1981.09</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>81</v>
+        <v>4</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>82</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -2290,7 +2291,7 @@
         <v>10</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>4</v>
@@ -2299,10 +2300,10 @@
         <v>4</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -2310,7 +2311,7 @@
         <v>10</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>4</v>
@@ -2319,10 +2320,10 @@
         <v>4</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -2330,7 +2331,7 @@
         <v>10</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>4</v>
@@ -2339,10 +2340,10 @@
         <v>4</v>
       </c>
       <c r="E61" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F61" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -2350,59 +2351,59 @@
         <v>10</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C62" s="1">
-        <v>23912531</v>
-      </c>
-      <c r="D62" s="1">
-        <v>520.4</v>
+        <v>82</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="C63" s="1">
-        <v>23912531</v>
+        <v>24133662</v>
       </c>
       <c r="D63" s="1">
-        <v>8449.5400000000009</v>
+        <v>215.27</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="C64" s="1">
-        <v>23912531</v>
+        <v>24133662</v>
       </c>
       <c r="D64" s="1">
-        <v>28687.95</v>
+        <v>9848.5300000000007</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>4</v>
+        <v>71</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -2410,99 +2411,99 @@
         <v>12</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C65" s="1">
-        <v>23912531</v>
+        <v>24133662</v>
       </c>
       <c r="D65" s="1">
-        <v>71116.38</v>
+        <v>28750.19</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>76</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C66" s="1">
-        <v>23912531</v>
+        <v>24133662</v>
       </c>
       <c r="D66" s="1">
-        <v>299675650000</v>
+        <v>71270.679999999993</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="C67" s="1">
-        <v>23912531</v>
-      </c>
-      <c r="D67" s="1">
-        <v>3547760400.8099999</v>
+        <v>24133662</v>
+      </c>
+      <c r="D67" s="4">
+        <v>299675650000</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C68" s="1">
-        <v>23912531</v>
-      </c>
-      <c r="D68" s="1">
-        <v>554559341638</v>
+        <v>24133662</v>
+      </c>
+      <c r="D68" s="4">
+        <v>1208533691.3199999</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>4</v>
+        <v>74</v>
+      </c>
+      <c r="C69" s="1">
+        <v>24133662</v>
+      </c>
+      <c r="D69" s="4">
+        <v>586568341638</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>81</v>
+        <v>4</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>82</v>
+        <v>4</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -2510,7 +2511,7 @@
         <v>10</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>4</v>
@@ -2519,10 +2520,10 @@
         <v>4</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -2530,7 +2531,7 @@
         <v>10</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>4</v>
@@ -2539,10 +2540,10 @@
         <v>4</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -2550,7 +2551,7 @@
         <v>10</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>4</v>
@@ -2559,104 +2560,104 @@
         <v>4</v>
       </c>
       <c r="E72" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F72" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C73" s="1">
-        <v>77952195</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>92</v>
+        <v>82</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>43</v>
+        <v>76</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C74" s="1">
-        <v>77952195</v>
-      </c>
-      <c r="D74" s="1">
-        <v>1179142000000</v>
+        <v>78844633</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>93</v>
+        <v>53</v>
       </c>
       <c r="C75" s="1">
-        <v>77952195</v>
-      </c>
-      <c r="D75" s="1">
-        <v>235820314159.44</v>
+        <v>78844633</v>
+      </c>
+      <c r="D75" s="4">
+        <v>1999583000000</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>51</v>
+        <v>4</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>94</v>
+        <v>4</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C76" s="1">
-        <v>383565184</v>
-      </c>
-      <c r="D76" s="1">
-        <v>27450.97</v>
+        <v>78844633</v>
+      </c>
+      <c r="D76" s="4">
+        <v>130551077169.2</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>4</v>
+        <v>88</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C77" s="1">
-        <v>383565184</v>
+        <v>390417216</v>
       </c>
       <c r="D77" s="1">
-        <v>2931.34</v>
+        <v>26350.97</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>4</v>
@@ -2667,16 +2668,16 @@
     </row>
     <row r="78" spans="1:6">
       <c r="A78" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C78" s="1">
-        <v>383565184</v>
+        <v>390417216</v>
       </c>
       <c r="D78" s="1">
-        <v>327462.52</v>
+        <v>1718.68</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>4</v>
@@ -2687,16 +2688,16 @@
     </row>
     <row r="79" spans="1:6">
       <c r="A79" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C79" s="1">
-        <v>370291757</v>
+        <v>390417216</v>
       </c>
       <c r="D79" s="1">
-        <v>757814.62</v>
+        <v>335748.93</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>4</v>
@@ -2707,16 +2708,16 @@
     </row>
     <row r="80" spans="1:6">
       <c r="A80" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C80" s="1">
-        <v>23912531</v>
-      </c>
-      <c r="D80" s="1">
-        <v>6666000</v>
+        <v>24133662</v>
+      </c>
+      <c r="D80" s="4">
+        <v>5396000</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>4</v>
@@ -2727,96 +2728,96 @@
     </row>
     <row r="81" spans="1:6">
       <c r="A81" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C81" s="1">
-        <v>23912531</v>
+        <v>24133662</v>
       </c>
       <c r="D81" s="1">
-        <v>2004.81</v>
+        <v>692171.09</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C82" s="1">
-        <v>23912531</v>
+        <v>24133662</v>
       </c>
       <c r="D82" s="1">
-        <v>8652000</v>
+        <v>29807884.100000001</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" s="1" t="s">
-        <v>24</v>
+        <v>119</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="C83" s="1">
-        <v>23912531</v>
+        <v>24133662</v>
       </c>
       <c r="D83" s="1">
-        <v>945652.09</v>
+        <v>2656855.66</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
     </row>
     <row r="84" spans="1:6">
       <c r="A84" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="C84" s="1">
-        <v>23326594</v>
+        <v>73539895</v>
       </c>
       <c r="D84" s="1">
-        <v>29807884.100000001</v>
+        <v>874160.82</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C85" s="1">
-        <v>69863728</v>
-      </c>
-      <c r="D85" s="1">
-        <v>2537000</v>
+        <v>73539895</v>
+      </c>
+      <c r="D85" s="4">
+        <v>2630000</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>4</v>
@@ -2830,39 +2831,39 @@
         <v>26</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>99</v>
+        <v>51</v>
       </c>
       <c r="C86" s="1">
-        <v>69863728</v>
+        <v>78844633</v>
       </c>
       <c r="D86" s="1">
-        <v>3733285</v>
+        <v>18203565.989999998</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
     </row>
     <row r="87" spans="1:6">
       <c r="A87" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>54</v>
+        <v>95</v>
       </c>
       <c r="C87" s="1">
-        <v>77952195</v>
-      </c>
-      <c r="D87" s="1">
-        <v>18203565.989999998</v>
+        <v>74803670</v>
+      </c>
+      <c r="D87" s="4">
+        <v>244080.7</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>55</v>
+        <v>4</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -2870,119 +2871,119 @@
         <v>30</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>101</v>
+        <v>51</v>
       </c>
       <c r="C88" s="1">
-        <v>72861177</v>
+        <v>78844633</v>
       </c>
       <c r="D88" s="1">
-        <v>906956</v>
+        <v>96071462.310000002</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="A89" s="1" t="s">
-        <v>33</v>
+        <v>96</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="C89" s="1">
-        <v>76195906</v>
+        <v>24133662</v>
       </c>
       <c r="D89" s="1">
-        <v>96071462.310000002</v>
+        <v>380000000.10000002</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
     </row>
     <row r="90" spans="1:6">
       <c r="A90" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="C90" s="1">
-        <v>23912531</v>
+        <v>24133662</v>
       </c>
       <c r="D90" s="1">
-        <v>90000001.019999996</v>
+        <v>9092462.8399999999</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
     </row>
     <row r="91" spans="1:6">
       <c r="A91" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="C91" s="1">
-        <v>23912531</v>
+        <v>24133662</v>
       </c>
       <c r="D91" s="1">
-        <v>3931165.32</v>
+        <v>1045412.19</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
     </row>
     <row r="92" spans="1:6">
       <c r="A92" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C92" s="1">
-        <v>23912531</v>
+        <v>24133662</v>
       </c>
       <c r="D92" s="1">
-        <v>1045412.19</v>
+        <v>40553991.119999997</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
     </row>
     <row r="93" spans="1:6">
       <c r="A93" s="1" t="s">
-        <v>102</v>
+        <v>10</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C93" s="1">
-        <v>23912531</v>
-      </c>
-      <c r="D93" s="1">
-        <v>53874001.119999997</v>
+        <v>75</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>4</v>
+        <v>76</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>4</v>
+        <v>77</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -2990,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>4</v>
@@ -2999,10 +3000,10 @@
         <v>4</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -3010,7 +3011,7 @@
         <v>10</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>4</v>
@@ -3019,10 +3020,10 @@
         <v>4</v>
       </c>
       <c r="E95" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F95" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="F95" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -3030,7 +3031,7 @@
         <v>10</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>4</v>
@@ -3039,58 +3040,58 @@
         <v>4</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="97" spans="1:6">
       <c r="A97" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>4</v>
+        <v>53</v>
+      </c>
+      <c r="C97" s="1">
+        <v>78844633</v>
+      </c>
+      <c r="D97" s="4">
+        <v>26851000</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>81</v>
+        <v>4</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>88</v>
+        <v>4</v>
       </c>
     </row>
     <row r="98" spans="1:6">
       <c r="A98" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C98" s="1">
-        <v>77952195</v>
-      </c>
-      <c r="D98" s="1">
-        <v>68766001</v>
+        <v>97</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>4</v>
+        <v>76</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>4</v>
+        <v>98</v>
       </c>
     </row>
     <row r="99" spans="1:6">
       <c r="A99" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>4</v>
@@ -3099,18 +3100,18 @@
         <v>4</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="100" spans="1:6">
       <c r="A100" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>4</v>
@@ -3119,84 +3120,84 @@
         <v>4</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="101" spans="1:6">
       <c r="A101" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>4</v>
+        <v>51</v>
+      </c>
+      <c r="C101" s="1">
+        <v>78844633</v>
+      </c>
+      <c r="D101" s="5">
+        <v>500000010</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>81</v>
+        <v>40</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>108</v>
+        <v>52</v>
       </c>
     </row>
     <row r="102" spans="1:6">
       <c r="A102" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="C102" s="1">
-        <v>77952195</v>
-      </c>
-      <c r="D102" s="1">
-        <v>2714687.72</v>
+        <v>24133662</v>
+      </c>
+      <c r="D102" s="5">
+        <v>494262959.38</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
     </row>
     <row r="103" spans="1:6">
       <c r="A103" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>75</v>
+        <v>103</v>
       </c>
       <c r="C103" s="1">
-        <v>23912531</v>
-      </c>
-      <c r="D103" s="1">
-        <v>1447549808.22</v>
+        <v>101250049</v>
+      </c>
+      <c r="D103" s="5">
+        <v>31087852.739765</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>76</v>
+        <v>4</v>
       </c>
     </row>
     <row r="104" spans="1:6">
       <c r="A104" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C104" s="1">
-        <v>100562863</v>
-      </c>
-      <c r="D104" s="1">
-        <v>31387852.739999998</v>
+        <v>101250049</v>
+      </c>
+      <c r="D104" s="5">
+        <v>898001</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>4</v>
@@ -3207,16 +3208,16 @@
     </row>
     <row r="105" spans="1:6">
       <c r="A105" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C105" s="1">
-        <v>100562863</v>
-      </c>
-      <c r="D105" s="1">
-        <v>1099001</v>
+        <v>101250049</v>
+      </c>
+      <c r="D105" s="5">
+        <v>254726</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>4</v>
@@ -3227,16 +3228,16 @@
     </row>
     <row r="106" spans="1:6">
       <c r="A106" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>111</v>
+        <v>74</v>
       </c>
       <c r="C106" s="1">
-        <v>100562863</v>
-      </c>
-      <c r="D106" s="1">
-        <v>184352.71</v>
+        <v>24133662</v>
+      </c>
+      <c r="D106" s="5">
+        <v>6746000</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>4</v>
@@ -3247,62 +3248,62 @@
     </row>
     <row r="107" spans="1:6">
       <c r="A107" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C107" s="1">
-        <v>23912531</v>
-      </c>
-      <c r="D107" s="1">
-        <v>4374002</v>
+        <v>24133662</v>
+      </c>
+      <c r="D107" s="5">
+        <v>34156000</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>4</v>
+        <v>71</v>
       </c>
     </row>
     <row r="108" spans="1:6">
       <c r="A108" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="C108" s="1">
-        <v>23912531</v>
-      </c>
-      <c r="D108" s="1">
-        <v>42156000</v>
+        <v>24133662</v>
+      </c>
+      <c r="D108" s="5">
+        <v>994243.24</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
     </row>
     <row r="109" spans="1:6">
       <c r="A109" s="1" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="C109" s="1">
-        <v>23912531</v>
-      </c>
-      <c r="D109" s="1">
-        <v>2632218.6800000002</v>
+        <v>6023980</v>
+      </c>
+      <c r="D109" s="5">
+        <v>12393000.76</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>51</v>
+        <v>4</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>90</v>
+        <v>4</v>
       </c>
     </row>
     <row r="110" spans="1:6">
@@ -3310,13 +3311,13 @@
         <v>8</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C110" s="1">
-        <v>5981741</v>
-      </c>
-      <c r="D110" s="1">
-        <v>13066000.76</v>
+        <v>6023980</v>
+      </c>
+      <c r="D110" s="5">
+        <v>344066003.31999999</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>4</v>
@@ -3330,13 +3331,13 @@
         <v>8</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C111" s="1">
-        <v>5981741</v>
-      </c>
-      <c r="D111" s="1">
-        <v>332468003.27999997</v>
+        <v>6023980</v>
+      </c>
+      <c r="D111" s="5">
+        <v>2866994</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>4</v>
@@ -3350,13 +3351,13 @@
         <v>8</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C112" s="1">
-        <v>5981741</v>
-      </c>
-      <c r="D112" s="1">
-        <v>134072.28</v>
+        <v>6023980</v>
+      </c>
+      <c r="D112" s="5">
+        <v>2647816.52</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>4</v>
@@ -3370,13 +3371,13 @@
         <v>8</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C113" s="1">
-        <v>5981741</v>
-      </c>
-      <c r="D113" s="1">
-        <v>2866994</v>
+        <v>6023980</v>
+      </c>
+      <c r="D113" s="5">
+        <v>1457329.62</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>4</v>
@@ -3390,13 +3391,13 @@
         <v>8</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C114" s="1">
-        <v>5981741</v>
-      </c>
-      <c r="D114" s="1">
-        <v>2647816.5299999998</v>
+        <v>6023980</v>
+      </c>
+      <c r="D114" s="5">
+        <v>850746.71</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>4</v>
@@ -3410,13 +3411,13 @@
         <v>8</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="C115" s="1">
-        <v>5981741</v>
-      </c>
-      <c r="D115" s="1">
-        <v>1457329.63</v>
+        <v>6023980</v>
+      </c>
+      <c r="D115" s="5">
+        <v>615169.91</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>4</v>
@@ -3430,13 +3431,13 @@
         <v>8</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C116" s="1">
-        <v>5981741</v>
-      </c>
-      <c r="D116" s="1">
-        <v>850746.71</v>
+        <v>6023980</v>
+      </c>
+      <c r="D116" s="5">
+        <v>1066964.3</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>4</v>
@@ -3450,13 +3451,13 @@
         <v>8</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C117" s="1">
-        <v>5981741</v>
-      </c>
-      <c r="D117" s="1">
-        <v>1066964.3</v>
+        <v>6023980</v>
+      </c>
+      <c r="D117" s="5">
+        <v>538350.48</v>
       </c>
       <c r="E117" s="1" t="s">
         <v>4</v>
@@ -3470,13 +3471,13 @@
         <v>8</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C118" s="1">
-        <v>5981741</v>
-      </c>
-      <c r="D118" s="1">
-        <v>538350.48</v>
+        <v>6023980</v>
+      </c>
+      <c r="D118" s="5">
+        <v>992885.38</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>4</v>
@@ -3490,13 +3491,13 @@
         <v>8</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C119" s="1">
-        <v>5981741</v>
-      </c>
-      <c r="D119" s="1">
-        <v>168809.44</v>
+        <v>6023980</v>
+      </c>
+      <c r="D119" s="5">
+        <v>127419.44</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>4</v>
@@ -3510,13 +3511,13 @@
         <v>8</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C120" s="1">
-        <v>5981741</v>
-      </c>
-      <c r="D120" s="1">
-        <v>127419.44</v>
+        <v>6023980</v>
+      </c>
+      <c r="D120" s="5">
+        <v>369407.15</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>4</v>
@@ -3530,13 +3531,13 @@
         <v>8</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C121" s="1">
-        <v>5981741</v>
-      </c>
-      <c r="D121" s="1">
-        <v>337972.77</v>
+        <v>6023980</v>
+      </c>
+      <c r="D121" s="5">
+        <v>66573200.600000001</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>4</v>
@@ -3550,13 +3551,13 @@
         <v>8</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C122" s="1">
-        <v>5981741</v>
-      </c>
-      <c r="D122" s="1">
-        <v>66276570.240000002</v>
+        <v>6023980</v>
+      </c>
+      <c r="D122" s="5">
+        <v>579364.13</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>4</v>
@@ -3573,10 +3574,10 @@
         <v>125</v>
       </c>
       <c r="C123" s="1">
-        <v>5981741</v>
-      </c>
-      <c r="D123" s="1">
-        <v>579364.13</v>
+        <v>6023980</v>
+      </c>
+      <c r="D123" s="5">
+        <v>766998.1</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>4</v>
@@ -3593,10 +3594,10 @@
         <v>126</v>
       </c>
       <c r="C124" s="1">
-        <v>5981741</v>
-      </c>
-      <c r="D124" s="1">
-        <v>5369989.6900000004</v>
+        <v>6023980</v>
+      </c>
+      <c r="D124" s="5">
+        <v>1992999.81</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>4</v>
@@ -3613,10 +3614,10 @@
         <v>127</v>
       </c>
       <c r="C125" s="1">
-        <v>5981741</v>
-      </c>
-      <c r="D125" s="1">
-        <v>2515998.2799999998</v>
+        <v>6023980</v>
+      </c>
+      <c r="D125" s="5">
+        <v>525999.63</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>4</v>
@@ -3633,10 +3634,10 @@
         <v>128</v>
       </c>
       <c r="C126" s="1">
-        <v>5981741</v>
-      </c>
-      <c r="D126" s="1">
-        <v>2404999.81</v>
+        <v>6023980</v>
+      </c>
+      <c r="D126" s="5">
+        <v>2708999.63</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>4</v>
@@ -3653,10 +3654,10 @@
         <v>129</v>
       </c>
       <c r="C127" s="1">
-        <v>5981741</v>
-      </c>
-      <c r="D127" s="1">
-        <v>1754998.02</v>
+        <v>6023980</v>
+      </c>
+      <c r="D127" s="5">
+        <v>4832999.8099999996</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>4</v>
@@ -3673,10 +3674,10 @@
         <v>130</v>
       </c>
       <c r="C128" s="1">
-        <v>5981741</v>
-      </c>
-      <c r="D128" s="1">
-        <v>1012992.59</v>
+        <v>6023980</v>
+      </c>
+      <c r="D128" s="5">
+        <v>6283996.4900000002</v>
       </c>
       <c r="E128" s="1" t="s">
         <v>4</v>
@@ -3693,10 +3694,10 @@
         <v>131</v>
       </c>
       <c r="C129" s="1">
-        <v>5981741</v>
-      </c>
-      <c r="D129" s="1">
-        <v>982999.48</v>
+        <v>6023980</v>
+      </c>
+      <c r="D129" s="5">
+        <v>4877997.57</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>4</v>
@@ -3713,10 +3714,10 @@
         <v>132</v>
       </c>
       <c r="C130" s="1">
-        <v>5981741</v>
-      </c>
-      <c r="D130" s="1">
-        <v>981999.81</v>
+        <v>6023980</v>
+      </c>
+      <c r="D130" s="5">
+        <v>1077999.48</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>4</v>
@@ -3733,75 +3734,15 @@
         <v>133</v>
       </c>
       <c r="C131" s="1">
-        <v>5981741</v>
-      </c>
-      <c r="D131" s="1">
-        <v>783999.48</v>
+        <v>6023980</v>
+      </c>
+      <c r="D131" s="5">
+        <v>1873999.63</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6">
-      <c r="A132" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B132" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C132" s="1">
-        <v>5981741</v>
-      </c>
-      <c r="D132" s="1">
-        <v>643999.14</v>
-      </c>
-      <c r="E132" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F132" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6">
-      <c r="A133" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B133" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C133" s="1">
-        <v>5981741</v>
-      </c>
-      <c r="D133" s="1">
-        <v>553998.73</v>
-      </c>
-      <c r="E133" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F133" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6">
-      <c r="A134" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B134" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C134" s="1">
-        <v>5981741</v>
-      </c>
-      <c r="D134" s="1">
-        <v>256999.81</v>
-      </c>
-      <c r="E134" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F134" s="1" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
upgrade: update snapshot 20260201; add support BASE-USDC;
</commit_message>
<xml_diff>
--- a/snapshot/huobi_por.xlsx
+++ b/snapshot/huobi_por.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Zhuanz/Code/wallet/huobi/Tool-Node.js-VerifyAddress/snapshot/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alefxu/Desktop/visa01_10/visa-hydrogen/packages/standalone/merkle-proof/snapshot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5C92D6-B35F-BA45-9CC9-BC83C4514A1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76E8C13-1CE8-894F-9913-CA2B41D012E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1960" yWindow="1260" windowWidth="28800" windowHeight="16360" xr2:uid="{411BB281-6367-B440-9EF5-E7547829EACC}"/>
+    <workbookView xWindow="1940" yWindow="1260" windowWidth="28800" windowHeight="16360" xr2:uid="{411BB281-6367-B440-9EF5-E7547829EACC}"/>
   </bookViews>
   <sheets>
     <sheet name="huobi_por" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="137">
   <si>
     <t>coin</t>
   </si>
@@ -301,12 +301,6 @@
     <t>0xafdfd157d9361e621e476036fee62f688450692b</t>
   </si>
   <si>
-    <t>0xdd3cb5c974601bc3974d908ea4a86020f9999e0c</t>
-  </si>
-  <si>
-    <t>0xd073bd9a42e935972c048fe2a3b7acfbb5d107d5fc22562efc88834f4b8ff83c359ce34f8d0c3c847f8d1c10afdd9ea126df84bb6bd11df486c920f826f828d400</t>
-  </si>
-  <si>
     <t>0xa77ff0e1c52f58363a53282624c7baa5fa91687d</t>
   </si>
   <si>
@@ -337,9 +331,6 @@
     <t>rPzT7GA6vWU3PvYSXBpdP5fQPnzwVLwL24</t>
   </si>
   <si>
-    <t>rneMKXXdKMD1R9WZ4Yqv1bfst6bjpaD5tP</t>
-  </si>
-  <si>
     <t>9ztZpRN3v9xv5JhAT7MTtmy4DfyMEAG8YU</t>
   </si>
   <si>
@@ -367,9 +358,6 @@
     <t>DB5KWytcxHyphHPn9iC92Y9JqPRL1Fq21p</t>
   </si>
   <si>
-    <t>DL2EGukahtib57Sg7FtHsvf8HgwMJtbBA3</t>
-  </si>
-  <si>
     <t>DHGb5BKsagXePRWwKqLx2vMH5uUNg8euvN</t>
   </si>
   <si>
@@ -379,49 +367,70 @@
     <t>jWBTC-TRC20</t>
   </si>
   <si>
-    <t>ERC20-AETHUSDC</t>
-  </si>
-  <si>
     <t>1HckjUpRGcrrRAtFaaCAUaGjsPx9oYmLaZ</t>
   </si>
   <si>
     <t>IJtEWgK2V8QxKUCWpVlfMTpVhwS2My/2Notvcw2lPBuHACHkxUESh8BoPL1vzQ4hkqYg/EZbQm9hpPKKcZJwY7E=</t>
   </si>
   <si>
-    <t>260029720157182.81</t>
-  </si>
-  <si>
-    <t>DQhEuTa5UkNcD8YFZK3pvjFfrtMqQpJhSa</t>
-  </si>
-  <si>
     <t>DKs2WBbiaAEe9RGzQTmtJj1o9bqsKTUTtC</t>
   </si>
   <si>
-    <t>A6MxoQbb4GanMdLRxLkexZC7m2DBH629fY</t>
-  </si>
-  <si>
-    <t>9sFCBgBszYBeFSQLdSQdSEPA35ZCfPLiCd</t>
-  </si>
-  <si>
-    <t>AAdvDHUdAAcCRRrhH6mDWdM3cvjzbLHsPJ</t>
-  </si>
-  <si>
-    <t>AAYU7frmWQPspbvbKU9BPFY5u1xsgTYMQN</t>
-  </si>
-  <si>
-    <t>A6tCf4eW82xEY91vCJEmHFr8RoH2mv8gbg</t>
-  </si>
-  <si>
-    <t>A6b5c1rmmWFjHbpwj6KXaJUjJTHJwsqVDu</t>
-  </si>
-  <si>
-    <t>9xcnXTBYyJRG3oFDJRyTX994o8rbQZ9ELi</t>
-  </si>
-  <si>
-    <t>9wRLiu1JnbvKw73K3rETWou6titXYUrKbJ</t>
-  </si>
-  <si>
-    <t>9xcUwVrSxhx6ckM8BhcvpdEfT2r5CyfJVE</t>
+    <t>wBTC-ERC20</t>
+  </si>
+  <si>
+    <t>BASE-USDC</t>
+  </si>
+  <si>
+    <t>SOL-USDC</t>
+  </si>
+  <si>
+    <t>USDT-BEP20</t>
+  </si>
+  <si>
+    <t>1JnrLZzvRSc7QngWvQwZjXQ43E1JaYYz2i</t>
+  </si>
+  <si>
+    <t>WBTC-ERC20</t>
+  </si>
+  <si>
+    <t>0xd5eb44e88c27f972d96f58677c7ebcf581102286</t>
+  </si>
+  <si>
+    <t>USDC-SOL</t>
+  </si>
+  <si>
+    <t>Cw32Ny2xcYdpfJmvFd7h2pRhcbcjoJFq8KrrA8YLwZeh</t>
+  </si>
+  <si>
+    <t>DFfSQtwuHTdHYjtDcxEVj9nkiKRFTDoG6g</t>
+  </si>
+  <si>
+    <t>DPqhyyBpjuULZRvdeRwtMMF9JGr1rHjszh</t>
+  </si>
+  <si>
+    <t>DGhM7zKE3Fyq7gsV1iZDAzNdGxBe2ncEcD</t>
+  </si>
+  <si>
+    <t>DN9kymtd8jbi1daJ8WDsUcTfC4xYcwZfLj</t>
+  </si>
+  <si>
+    <t>A1Gu7nUxXaWZaqkEoFKou3ZiLDXprLLNc4</t>
+  </si>
+  <si>
+    <t>ADgPXkXEcc9arydZc5oJH1HNx8YRzACeQ3</t>
+  </si>
+  <si>
+    <t>ACELftry9PkuRkWr86njdGUC3xbbkZyhfc</t>
+  </si>
+  <si>
+    <t>AAnFqXhQAHnsgaLjH39FmfaQaSGXpEkVpJ</t>
+  </si>
+  <si>
+    <t>AA4VcBX1GnxuFt13rTbag3ANi87Fg9y4ze</t>
+  </si>
+  <si>
+    <t>AE8tRm7ffSkM3uaaoQkgMnNtK3eSUtVbnm</t>
   </si>
 </sst>
 </file>
@@ -1445,10 +1454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{551DE6D8-23DE-D340-B153-F7BA258674FF}">
-  <dimension ref="A1:F131"/>
+  <dimension ref="A1:F134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="132" workbookViewId="0">
-      <selection activeCell="D87" sqref="D87"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="132" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1480,7 +1489,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="5">
-        <v>20397.22</v>
+        <v>20876.59</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1488,442 +1497,415 @@
         <v>5</v>
       </c>
       <c r="B3" s="1">
-        <v>930288</v>
+        <v>934496</v>
       </c>
       <c r="C3" s="5">
-        <v>9793.2999999999993</v>
+        <v>9185.9500000000007</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>118</v>
       </c>
       <c r="B4" s="1">
-        <v>78844633</v>
+        <v>24355911</v>
       </c>
       <c r="C4" s="5">
-        <v>10514.93</v>
+        <v>1212.72</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>118</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1">
-        <v>78844633</v>
+        <v>79736938</v>
       </c>
       <c r="C5" s="5">
-        <v>89</v>
+        <v>10388.92</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>4</v>
+        <v>114</v>
+      </c>
+      <c r="B6" s="1">
+        <v>79736938</v>
       </c>
       <c r="C6" s="5">
-        <v>460086642.47000003</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1">
-        <v>6023980</v>
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C7" s="5">
-        <v>460086642.47000003</v>
+        <v>461459547.61000001</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="B8" s="1">
+        <v>6066323</v>
       </c>
       <c r="C8" s="5">
-        <v>125756.86</v>
+        <v>461459547.61000001</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="1">
-        <v>24133662</v>
+        <v>9</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C9" s="5">
-        <v>15887.45</v>
+        <v>126386.02</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1">
-        <v>24133662</v>
+        <v>24355911</v>
       </c>
       <c r="C10" s="5">
-        <v>9848.5400000000009</v>
+        <v>12513.95</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="1">
-        <v>24133662</v>
+        <v>24355911</v>
       </c>
       <c r="C11" s="6">
-        <v>100020.87</v>
+        <v>13643.17</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>4</v>
+        <v>12</v>
+      </c>
+      <c r="B12" s="1">
+        <v>24355911</v>
       </c>
       <c r="C12" s="7">
-        <v>263047306759681</v>
+        <v>100228.9</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="1">
-        <v>24133662</v>
+        <v>13</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C13" s="7">
-        <v>887452525329.31995</v>
+        <v>250640810380508</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="1">
-        <v>78844633</v>
+        <v>24355911</v>
       </c>
       <c r="C14" s="8">
-        <v>262159854234352</v>
+        <v>934247605185</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>4</v>
+        <v>15</v>
+      </c>
+      <c r="B15" s="1">
+        <v>79736938</v>
       </c>
       <c r="C15" s="5">
-        <v>363818.58</v>
+        <v>249706562775323</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="1">
-        <v>390417216</v>
+        <v>16</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C16" s="5">
-        <v>363818.58</v>
+        <v>371618.58</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>4</v>
+        <v>17</v>
+      </c>
+      <c r="B17" s="1">
+        <v>397161865</v>
       </c>
       <c r="C17" s="5">
-        <v>9940804554.1800003</v>
+        <v>371618.58</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="1">
-        <v>78844633</v>
+        <v>18</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C18" s="5">
-        <v>9018330748.2399998</v>
+        <v>9941020242.5799999</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" s="1">
-        <v>78844633</v>
+        <v>79736938</v>
       </c>
       <c r="C19" s="5">
-        <v>922473805.94000006</v>
+        <v>9018546436.6299992</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>4</v>
+        <v>20</v>
+      </c>
+      <c r="B20" s="1">
+        <v>79736938</v>
       </c>
       <c r="C20" s="5">
-        <v>42057071.670000002</v>
+        <v>922473805.94000006</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="1">
-        <v>24133662</v>
+        <v>21</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C21" s="5">
-        <v>6088171.0999999996</v>
+        <v>46086599.560000002</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" s="1">
-        <v>24133662</v>
+        <v>24355911</v>
       </c>
       <c r="C22" s="5">
-        <v>29807884.100000001</v>
+        <v>3061847.26</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1">
-        <v>73539895</v>
+        <v>24355911</v>
       </c>
       <c r="C23" s="5">
-        <v>3504160.82</v>
+        <v>33093720.210000001</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="1" t="s">
-        <v>119</v>
+        <v>24</v>
       </c>
       <c r="B24" s="1">
-        <v>24133662</v>
+        <v>78649895</v>
       </c>
       <c r="C24" s="5">
-        <v>2656855.66</v>
+        <v>3051032.09</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>4</v>
+        <v>119</v>
+      </c>
+      <c r="B25" s="1">
+        <v>41602368</v>
       </c>
       <c r="C25" s="5">
-        <v>1566324944.5999999</v>
+        <v>3974000</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="1" t="s">
-        <v>26</v>
+        <v>120</v>
       </c>
       <c r="B26" s="1">
-        <v>78844633</v>
+        <v>397161865</v>
       </c>
       <c r="C26" s="5">
-        <v>18203565.989999998</v>
+        <v>2906000</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" s="1">
-        <v>74803670</v>
+        <v>25</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C27" s="5">
-        <v>244080.67</v>
+        <v>1313451824.1300001</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B28" s="1">
-        <v>24133662</v>
+        <v>79736938</v>
       </c>
       <c r="C28" s="5">
-        <v>430691866.25</v>
+        <v>39168013.420000002</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B29" s="1">
-        <v>78844633</v>
+        <v>76961605</v>
       </c>
       <c r="C29" s="5">
-        <v>526851010</v>
+        <v>937706.17</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B30" s="1">
-        <v>78844633</v>
+        <v>24355911</v>
       </c>
       <c r="C30" s="5">
-        <v>96071462.310000002</v>
+        <v>17856625.370000001</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B31" s="1">
-        <v>24133662</v>
+        <v>79736938</v>
       </c>
       <c r="C31" s="5">
-        <v>494262959.38</v>
+        <v>36105076.590000004</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
+      </c>
+      <c r="B32" s="1">
+        <v>79736938</v>
       </c>
       <c r="C32" s="5">
-        <v>41896243.240000002</v>
+        <v>22228377.32</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B33" s="1">
-        <v>24133662</v>
+        <v>24355911</v>
       </c>
       <c r="C33" s="5">
-        <v>41896243.240000002</v>
+        <v>1189639856.55</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>4</v>
+        <v>121</v>
+      </c>
+      <c r="B34" s="1">
+        <v>78649895</v>
       </c>
       <c r="C34" s="5">
-        <v>32240579.739999998</v>
+        <v>7516168.7000000002</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B35" s="1">
-        <v>101250049</v>
+        <v>32</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C35" s="5">
-        <v>32240579.739999998</v>
+        <v>39622259.079999998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" s="1">
+        <v>24355911</v>
+      </c>
+      <c r="C36" s="5">
+        <v>39622259.079999998</v>
       </c>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>38</v>
+      <c r="A37" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="5">
+        <v>30807853.739999998</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C38" s="1">
-        <v>930288</v>
-      </c>
-      <c r="D38" s="5">
-        <v>7680.7</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C39" s="1">
-        <v>930288</v>
-      </c>
-      <c r="D39" s="5">
-        <v>970.8</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
+      </c>
+      <c r="B38" s="1">
+        <v>101934884</v>
+      </c>
+      <c r="C38" s="5">
+        <v>30807853.739999998</v>
       </c>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C40" s="1">
-        <v>930288</v>
-      </c>
-      <c r="D40" s="5">
-        <v>11.19</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>121</v>
+      <c r="A40" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1931,19 +1913,19 @@
         <v>5</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C41" s="1">
-        <v>930288</v>
+        <v>934496</v>
       </c>
       <c r="D41" s="5">
-        <v>829.68</v>
+        <v>6983.7</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1951,19 +1933,19 @@
         <v>5</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C42" s="1">
-        <v>930288</v>
+        <v>934496</v>
       </c>
       <c r="D42" s="5">
-        <v>80.569999999999993</v>
+        <v>970.8</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1971,19 +1953,19 @@
         <v>5</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>47</v>
+        <v>115</v>
       </c>
       <c r="C43" s="1">
-        <v>930288</v>
+        <v>934496</v>
       </c>
       <c r="D43" s="5">
-        <v>40.35</v>
+        <v>8.3800000000000008</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>48</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>49</v>
+        <v>116</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1991,159 +1973,159 @@
         <v>5</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C44" s="1">
-        <v>930288</v>
+        <v>934496</v>
       </c>
       <c r="D44" s="5">
-        <v>180</v>
+        <v>829.68</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C45" s="1">
-        <v>78844633</v>
+        <v>934496</v>
       </c>
       <c r="D45" s="5">
-        <v>10393.93</v>
+        <v>80.569999999999993</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>52</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C46" s="1">
-        <v>78844633</v>
+        <v>934496</v>
       </c>
       <c r="D46" s="5">
-        <v>121</v>
+        <v>31.94</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="1" t="s">
-        <v>118</v>
+        <v>5</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C47" s="1">
-        <v>78844633</v>
+        <v>934496</v>
       </c>
       <c r="D47" s="5">
-        <v>89</v>
+        <v>272</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>52</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="1" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>54</v>
+        <v>122</v>
       </c>
       <c r="C48" s="1">
-        <v>78844633</v>
+        <v>934496</v>
       </c>
       <c r="D48" s="5">
-        <v>1082070082.8699999</v>
+        <v>8.8699999999999992</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>55</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="1" t="s">
-        <v>19</v>
+        <v>123</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="C49" s="1">
-        <v>78844633</v>
+        <v>24355911</v>
       </c>
       <c r="D49" s="5">
-        <v>20079635.449999999</v>
+        <v>1212.72</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="1" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C50" s="1">
-        <v>78844633</v>
+        <v>79736938</v>
       </c>
       <c r="D50" s="5">
-        <v>1705110564.0899999</v>
+        <v>10388.92</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="1" t="s">
-        <v>19</v>
+        <v>114</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C51" s="1">
-        <v>78844633</v>
+        <v>79736938</v>
       </c>
       <c r="D51" s="5">
-        <v>1434482060.2</v>
+        <v>89</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -2151,19 +2133,19 @@
         <v>19</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C52" s="1">
-        <v>78844633</v>
+        <v>79736938</v>
       </c>
       <c r="D52" s="5">
-        <v>1071248100.5</v>
+        <v>1082073166.3499999</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -2171,19 +2153,19 @@
         <v>19</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C53" s="1">
-        <v>78844633</v>
+        <v>79736938</v>
       </c>
       <c r="D53" s="5">
-        <v>1070377939.01</v>
+        <v>20284026.289999999</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -2191,19 +2173,19 @@
         <v>19</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C54" s="1">
-        <v>78844633</v>
+        <v>79736938</v>
       </c>
       <c r="D54" s="5">
-        <v>1064072591.03</v>
+        <v>1705110564.0899999</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -2211,119 +2193,119 @@
         <v>19</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C55" s="1">
-        <v>78844633</v>
+        <v>79736938</v>
       </c>
       <c r="D55" s="5">
-        <v>1570889775.0799999</v>
+        <v>1434482060.2</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C56" s="1">
-        <v>78844633</v>
+        <v>79736938</v>
       </c>
       <c r="D56" s="5">
-        <v>922473805.94000006</v>
+        <v>1071252207.55</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C57" s="1">
-        <v>24133662</v>
+        <v>79736938</v>
       </c>
       <c r="D57" s="5">
-        <v>13691.08</v>
+        <v>1070378962.5700001</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C58" s="1">
-        <v>24133662</v>
+        <v>79736938</v>
       </c>
       <c r="D58" s="5">
-        <v>1981.09</v>
+        <v>1064075674.5</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>4</v>
+        <v>65</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>4</v>
+        <v>66</v>
+      </c>
+      <c r="C59" s="1">
+        <v>79736938</v>
+      </c>
+      <c r="D59" s="5">
+        <v>1570889775.0799999</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>4</v>
+        <v>68</v>
+      </c>
+      <c r="C60" s="1">
+        <v>79736938</v>
+      </c>
+      <c r="D60" s="5">
+        <v>922473805.94000006</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -2331,19 +2313,19 @@
         <v>10</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>4</v>
+        <v>70</v>
+      </c>
+      <c r="C61" s="1">
+        <v>24355911</v>
+      </c>
+      <c r="D61" s="5">
+        <v>1840.24</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -2351,19 +2333,19 @@
         <v>10</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>4</v>
+        <v>74</v>
+      </c>
+      <c r="C62" s="1">
+        <v>24355911</v>
+      </c>
+      <c r="D62" s="1">
+        <v>10180.09</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>76</v>
+        <v>4</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -2371,113 +2353,113 @@
         <v>10</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C63" s="1">
-        <v>24133662</v>
-      </c>
-      <c r="D63" s="1">
-        <v>215.27</v>
+        <v>75</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C64" s="1">
-        <v>24133662</v>
-      </c>
-      <c r="D64" s="1">
-        <v>9848.5300000000007</v>
+        <v>78</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C65" s="1">
-        <v>24133662</v>
-      </c>
-      <c r="D65" s="1">
-        <v>28750.19</v>
+        <v>80</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>4</v>
+        <v>76</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>4</v>
+        <v>81</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C66" s="1">
-        <v>24133662</v>
-      </c>
-      <c r="D66" s="1">
-        <v>71270.679999999993</v>
+        <v>82</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C67" s="1">
-        <v>24133662</v>
-      </c>
-      <c r="D67" s="4">
-        <v>299675650000</v>
+        <v>24355911</v>
+      </c>
+      <c r="D67" s="1">
+        <v>48.89</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>84</v>
       </c>
       <c r="C68" s="1">
-        <v>24133662</v>
-      </c>
-      <c r="D68" s="4">
-        <v>1208533691.3199999</v>
+        <v>24355911</v>
+      </c>
+      <c r="D68" s="1">
+        <v>444.73</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>48</v>
@@ -2488,236 +2470,236 @@
     </row>
     <row r="69" spans="1:6">
       <c r="A69" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C69" s="1">
-        <v>24133662</v>
-      </c>
-      <c r="D69" s="4">
-        <v>586568341638</v>
+        <v>24355911</v>
+      </c>
+      <c r="D69" s="1">
+        <v>13643.17</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>4</v>
+        <v>71</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>4</v>
+        <v>86</v>
+      </c>
+      <c r="C70" s="1">
+        <v>24355911</v>
+      </c>
+      <c r="D70" s="4">
+        <v>28809.99</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>76</v>
+        <v>4</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>77</v>
+        <v>4</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>4</v>
+        <v>70</v>
+      </c>
+      <c r="C71" s="1">
+        <v>24355911</v>
+      </c>
+      <c r="D71" s="4">
+        <v>71418.91</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>4</v>
+        <v>70</v>
+      </c>
+      <c r="C72" s="1">
+        <v>24355911</v>
+      </c>
+      <c r="D72" s="4">
+        <v>343701650000</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>4</v>
+        <v>84</v>
+      </c>
+      <c r="C73" s="1">
+        <v>24355911</v>
+      </c>
+      <c r="D73" s="1">
+        <v>3977613547.4200001</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="C74" s="1">
-        <v>78844633</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>122</v>
+        <v>24355911</v>
+      </c>
+      <c r="D74" s="1">
+        <v>586568341638</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>52</v>
+        <v>4</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C75" s="1">
-        <v>78844633</v>
-      </c>
-      <c r="D75" s="4">
-        <v>1999583000000</v>
+        <v>75</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>4</v>
+        <v>76</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>4</v>
+        <v>77</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C76" s="1">
-        <v>78844633</v>
-      </c>
-      <c r="D76" s="4">
-        <v>130551077169.2</v>
+        <v>78</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C77" s="1">
-        <v>390417216</v>
-      </c>
-      <c r="D77" s="1">
-        <v>26350.97</v>
+        <v>80</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>4</v>
+        <v>76</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>4</v>
+        <v>81</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C78" s="1">
-        <v>390417216</v>
-      </c>
-      <c r="D78" s="1">
-        <v>1718.68</v>
+        <v>82</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>4</v>
+        <v>76</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>4</v>
+        <v>83</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c r="A79" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>91</v>
+        <v>51</v>
       </c>
       <c r="C79" s="1">
-        <v>390417216</v>
-      </c>
-      <c r="D79" s="1">
-        <v>335748.93</v>
+        <v>79736938</v>
+      </c>
+      <c r="D79" s="4">
+        <v>246413348367579</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="C80" s="1">
-        <v>24133662</v>
-      </c>
-      <c r="D80" s="4">
-        <v>5396000</v>
+        <v>79736938</v>
+      </c>
+      <c r="D80" s="1">
+        <v>3062751000000</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>4</v>
@@ -2728,136 +2710,136 @@
     </row>
     <row r="81" spans="1:6">
       <c r="A81" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C81" s="1">
-        <v>24133662</v>
+        <v>79736938</v>
       </c>
       <c r="D81" s="1">
-        <v>692171.09</v>
+        <v>230463407743.48999</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>48</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="C82" s="1">
-        <v>24133662</v>
+        <v>397161865</v>
       </c>
       <c r="D82" s="1">
-        <v>29807884.100000001</v>
+        <v>42680.97</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>71</v>
+        <v>4</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" s="1" t="s">
-        <v>119</v>
+        <v>17</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="C83" s="1">
-        <v>24133662</v>
-      </c>
-      <c r="D83" s="1">
-        <v>2656855.66</v>
+        <v>397161865</v>
+      </c>
+      <c r="D83" s="4">
+        <v>710.2</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>71</v>
+        <v>4</v>
       </c>
     </row>
     <row r="84" spans="1:6">
       <c r="A84" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C84" s="1">
-        <v>73539895</v>
+        <v>397161865</v>
       </c>
       <c r="D84" s="1">
-        <v>874160.82</v>
+        <v>328227.42</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>48</v>
+        <v>4</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>94</v>
+        <v>4</v>
       </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C85" s="1">
-        <v>73539895</v>
-      </c>
-      <c r="D85" s="4">
-        <v>2630000</v>
+        <v>24355911</v>
+      </c>
+      <c r="D85" s="1">
+        <v>412847.26</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="C86" s="1">
-        <v>78844633</v>
+        <v>24355911</v>
       </c>
       <c r="D86" s="1">
-        <v>18203565.989999998</v>
+        <v>2649000</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>52</v>
+        <v>4</v>
       </c>
     </row>
     <row r="87" spans="1:6">
       <c r="A87" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C87" s="1">
-        <v>74803670</v>
-      </c>
-      <c r="D87" s="4">
-        <v>244080.7</v>
+        <v>78649895</v>
+      </c>
+      <c r="D87" s="1">
+        <v>3051032.09</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>4</v>
@@ -2868,96 +2850,96 @@
     </row>
     <row r="88" spans="1:6">
       <c r="A88" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="C88" s="1">
-        <v>78844633</v>
-      </c>
-      <c r="D88" s="1">
-        <v>96071462.310000002</v>
+        <v>24355911</v>
+      </c>
+      <c r="D88" s="4">
+        <v>33093720.210000001</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="A89" s="1" t="s">
-        <v>96</v>
+        <v>119</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>70</v>
+        <v>124</v>
       </c>
       <c r="C89" s="1">
-        <v>24133662</v>
+        <v>41602368</v>
       </c>
       <c r="D89" s="1">
-        <v>380000000.10000002</v>
+        <v>3974000</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>71</v>
+        <v>4</v>
       </c>
     </row>
     <row r="90" spans="1:6">
       <c r="A90" s="1" t="s">
-        <v>96</v>
+        <v>125</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>84</v>
+        <v>126</v>
       </c>
       <c r="C90" s="1">
-        <v>24133662</v>
-      </c>
-      <c r="D90" s="1">
-        <v>9092462.8399999999</v>
+        <v>397161865</v>
+      </c>
+      <c r="D90" s="4">
+        <v>2906000</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>48</v>
+        <v>4</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>85</v>
+        <v>4</v>
       </c>
     </row>
     <row r="91" spans="1:6">
       <c r="A91" s="1" t="s">
-        <v>96</v>
+        <v>26</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="C91" s="1">
-        <v>24133662</v>
+        <v>79736938</v>
       </c>
       <c r="D91" s="1">
-        <v>1045412.19</v>
+        <v>39168013.420000002</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
     </row>
     <row r="92" spans="1:6">
       <c r="A92" s="1" t="s">
-        <v>96</v>
+        <v>27</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>74</v>
+        <v>93</v>
       </c>
       <c r="C92" s="1">
-        <v>24133662</v>
+        <v>76961605</v>
       </c>
       <c r="D92" s="1">
-        <v>40553991.119999997</v>
+        <v>937706.17</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>4</v>
@@ -2968,110 +2950,110 @@
     </row>
     <row r="93" spans="1:6">
       <c r="A93" s="1" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>4</v>
+        <v>51</v>
+      </c>
+      <c r="C93" s="1">
+        <v>79736938</v>
+      </c>
+      <c r="D93" s="1">
+        <v>22228377.32</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
     </row>
     <row r="94" spans="1:6">
       <c r="A94" s="1" t="s">
-        <v>10</v>
+        <v>94</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D94" s="1" t="s">
-        <v>4</v>
+        <v>84</v>
+      </c>
+      <c r="C94" s="1">
+        <v>24355911</v>
+      </c>
+      <c r="D94" s="1">
+        <v>5001212.18</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
     </row>
     <row r="95" spans="1:6">
       <c r="A95" s="1" t="s">
-        <v>10</v>
+        <v>94</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>4</v>
+        <v>72</v>
+      </c>
+      <c r="C95" s="1">
+        <v>24355911</v>
+      </c>
+      <c r="D95" s="1">
+        <v>1045412.19</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="96" spans="1:6">
       <c r="A96" s="1" t="s">
-        <v>10</v>
+        <v>94</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>4</v>
+        <v>74</v>
+      </c>
+      <c r="C96" s="1">
+        <v>24355911</v>
+      </c>
+      <c r="D96" s="1">
+        <v>11810001</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>76</v>
+        <v>4</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="97" spans="1:6">
       <c r="A97" s="1" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C97" s="1">
-        <v>78844633</v>
-      </c>
-      <c r="D97" s="4">
-        <v>26851000</v>
+        <v>75</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>4</v>
+        <v>76</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>4</v>
+        <v>77</v>
       </c>
     </row>
     <row r="98" spans="1:6">
       <c r="A98" s="1" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>4</v>
@@ -3083,15 +3065,15 @@
         <v>76</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
     </row>
     <row r="99" spans="1:6">
       <c r="A99" s="1" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>4</v>
@@ -3103,27 +3085,27 @@
         <v>76</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
     </row>
     <row r="100" spans="1:6">
       <c r="A100" s="1" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D100" s="1" t="s">
+      <c r="D100" s="4" t="s">
         <v>4</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>76</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -3131,173 +3113,173 @@
         <v>29</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C101" s="1">
-        <v>78844633</v>
-      </c>
-      <c r="D101" s="5">
-        <v>500000010</v>
+        <v>79736938</v>
+      </c>
+      <c r="D101" s="1">
+        <v>23842000</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>52</v>
+        <v>4</v>
       </c>
     </row>
     <row r="102" spans="1:6">
       <c r="A102" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C102" s="1">
-        <v>24133662</v>
-      </c>
-      <c r="D102" s="5">
-        <v>494262959.38</v>
+        <v>95</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
     </row>
     <row r="103" spans="1:6">
       <c r="A103" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C103" s="1">
-        <v>101250049</v>
-      </c>
-      <c r="D103" s="5">
-        <v>31087852.739765</v>
+        <v>97</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>4</v>
+        <v>76</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>4</v>
+        <v>98</v>
       </c>
     </row>
     <row r="104" spans="1:6">
       <c r="A104" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C104" s="1">
-        <v>101250049</v>
-      </c>
-      <c r="D104" s="5">
-        <v>898001</v>
+        <v>99</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D104" s="5" t="s">
+        <v>4</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>4</v>
+        <v>76</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>4</v>
+        <v>100</v>
       </c>
     </row>
     <row r="105" spans="1:6">
       <c r="A105" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="C105" s="1">
-        <v>101250049</v>
+        <v>79736938</v>
       </c>
       <c r="D105" s="5">
-        <v>254726</v>
+        <v>12263076.6</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>4</v>
+        <v>88</v>
       </c>
     </row>
     <row r="106" spans="1:6">
       <c r="A106" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C106" s="1">
-        <v>24133662</v>
+        <v>24355911</v>
       </c>
       <c r="D106" s="5">
-        <v>6746000</v>
+        <v>1189639856.55</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>4</v>
+        <v>71</v>
       </c>
     </row>
     <row r="107" spans="1:6">
       <c r="A107" s="1" t="s">
-        <v>33</v>
+        <v>121</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="C107" s="1">
-        <v>24133662</v>
+        <v>78649895</v>
       </c>
       <c r="D107" s="5">
-        <v>34156000</v>
+        <v>7516168.7000000002</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>71</v>
+        <v>4</v>
       </c>
     </row>
     <row r="108" spans="1:6">
       <c r="A108" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="C108" s="1">
-        <v>24133662</v>
+        <v>101934884</v>
       </c>
       <c r="D108" s="5">
-        <v>994243.24</v>
+        <v>29187852.739999998</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>48</v>
+        <v>4</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>85</v>
+        <v>4</v>
       </c>
     </row>
     <row r="109" spans="1:6">
       <c r="A109" s="1" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C109" s="1">
-        <v>6023980</v>
+        <v>101934884</v>
       </c>
       <c r="D109" s="5">
-        <v>12393000.76</v>
+        <v>1620001</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>4</v>
@@ -3308,16 +3290,16 @@
     </row>
     <row r="110" spans="1:6">
       <c r="A110" s="1" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>107</v>
+        <v>74</v>
       </c>
       <c r="C110" s="1">
-        <v>6023980</v>
+        <v>24355911</v>
       </c>
       <c r="D110" s="5">
-        <v>344066003.31999999</v>
+        <v>4441000</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>4</v>
@@ -3328,42 +3310,42 @@
     </row>
     <row r="111" spans="1:6">
       <c r="A111" s="1" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>108</v>
+        <v>70</v>
       </c>
       <c r="C111" s="1">
-        <v>6023980</v>
+        <v>24355911</v>
       </c>
       <c r="D111" s="5">
-        <v>2866994</v>
+        <v>34156000</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>4</v>
+        <v>71</v>
       </c>
     </row>
     <row r="112" spans="1:6">
       <c r="A112" s="1" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="C112" s="1">
-        <v>6023980</v>
+        <v>24355911</v>
       </c>
       <c r="D112" s="5">
-        <v>2647816.52</v>
+        <v>1025259.08</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
     </row>
     <row r="113" spans="1:6">
@@ -3371,13 +3353,13 @@
         <v>8</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C113" s="1">
-        <v>6023980</v>
+        <v>6066323</v>
       </c>
       <c r="D113" s="5">
-        <v>1457329.62</v>
+        <v>27082000.763</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>4</v>
@@ -3391,13 +3373,13 @@
         <v>8</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C114" s="1">
-        <v>6023980</v>
+        <v>6066323</v>
       </c>
       <c r="D114" s="5">
-        <v>850746.71</v>
+        <v>345813003.32800001</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>4</v>
@@ -3411,13 +3393,13 @@
         <v>8</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="C115" s="1">
-        <v>6023980</v>
+        <v>6066323</v>
       </c>
       <c r="D115" s="5">
-        <v>615169.91</v>
+        <v>2866993.9984026002</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>4</v>
@@ -3431,13 +3413,13 @@
         <v>8</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C116" s="1">
-        <v>6023980</v>
+        <v>6066323</v>
       </c>
       <c r="D116" s="5">
-        <v>1066964.3</v>
+        <v>2647816.5263509499</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>4</v>
@@ -3451,13 +3433,13 @@
         <v>8</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C117" s="1">
-        <v>6023980</v>
+        <v>6066323</v>
       </c>
       <c r="D117" s="5">
-        <v>538350.48</v>
+        <v>1457329.6256335201</v>
       </c>
       <c r="E117" s="1" t="s">
         <v>4</v>
@@ -3471,13 +3453,13 @@
         <v>8</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="C118" s="1">
-        <v>6023980</v>
+        <v>6066323</v>
       </c>
       <c r="D118" s="5">
-        <v>992885.38</v>
+        <v>850746.71291593998</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>4</v>
@@ -3491,13 +3473,13 @@
         <v>8</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C119" s="1">
-        <v>6023980</v>
+        <v>6066323</v>
       </c>
       <c r="D119" s="5">
-        <v>127419.44</v>
+        <v>1066964.2965422401</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>4</v>
@@ -3511,13 +3493,13 @@
         <v>8</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C120" s="1">
-        <v>6023980</v>
+        <v>6066323</v>
       </c>
       <c r="D120" s="5">
-        <v>369407.15</v>
+        <v>538350.47626451997</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>4</v>
@@ -3531,13 +3513,13 @@
         <v>8</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C121" s="1">
-        <v>6023980</v>
+        <v>6066323</v>
       </c>
       <c r="D121" s="5">
-        <v>66573200.600000001</v>
+        <v>1056186.80422258</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>4</v>
@@ -3551,13 +3533,13 @@
         <v>8</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C122" s="1">
-        <v>6023980</v>
+        <v>6066323</v>
       </c>
       <c r="D122" s="5">
-        <v>579364.13</v>
+        <v>127419.4406821</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>4</v>
@@ -3571,13 +3553,13 @@
         <v>8</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C123" s="1">
-        <v>6023980</v>
+        <v>6066323</v>
       </c>
       <c r="D123" s="5">
-        <v>766998.1</v>
+        <v>471264.32</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>4</v>
@@ -3591,13 +3573,13 @@
         <v>8</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C124" s="1">
-        <v>6023980</v>
+        <v>6066323</v>
       </c>
       <c r="D124" s="5">
-        <v>1992999.81</v>
+        <v>351477.76277212001</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>4</v>
@@ -3611,13 +3593,13 @@
         <v>8</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="C125" s="1">
-        <v>6023980</v>
+        <v>6066323</v>
       </c>
       <c r="D125" s="5">
-        <v>525999.63</v>
+        <v>66066923.393727899</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>4</v>
@@ -3631,13 +3613,13 @@
         <v>8</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="C126" s="1">
-        <v>6023980</v>
+        <v>6066323</v>
       </c>
       <c r="D126" s="5">
-        <v>2708999.63</v>
+        <v>579364.12614367995</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>4</v>
@@ -3654,10 +3636,10 @@
         <v>129</v>
       </c>
       <c r="C127" s="1">
-        <v>6023980</v>
+        <v>6066323</v>
       </c>
       <c r="D127" s="5">
-        <v>4832999.8099999996</v>
+        <v>148023.0137525</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>4</v>
@@ -3674,10 +3656,10 @@
         <v>130</v>
       </c>
       <c r="C128" s="1">
-        <v>6023980</v>
+        <v>6066323</v>
       </c>
       <c r="D128" s="5">
-        <v>6283996.4900000002</v>
+        <v>460723.01</v>
       </c>
       <c r="E128" s="1" t="s">
         <v>4</v>
@@ -3694,10 +3676,10 @@
         <v>131</v>
       </c>
       <c r="C129" s="1">
-        <v>6023980</v>
+        <v>6066323</v>
       </c>
       <c r="D129" s="5">
-        <v>4877997.57</v>
+        <v>5042999.8130000001</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>4</v>
@@ -3714,10 +3696,10 @@
         <v>132</v>
       </c>
       <c r="C130" s="1">
-        <v>6023980</v>
+        <v>6066323</v>
       </c>
       <c r="D130" s="5">
-        <v>1077999.48</v>
+        <v>2511973.91</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>4</v>
@@ -3734,15 +3716,75 @@
         <v>133</v>
       </c>
       <c r="C131" s="1">
-        <v>6023980</v>
+        <v>6066323</v>
       </c>
       <c r="D131" s="5">
-        <v>1873999.63</v>
+        <v>1063999.8130000001</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F131" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6">
+      <c r="A132" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C132" s="1">
+        <v>6066323</v>
+      </c>
+      <c r="D132" s="5">
+        <v>691995.62899999996</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F132" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6">
+      <c r="A133" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C133" s="1">
+        <v>6066323</v>
+      </c>
+      <c r="D133" s="5">
+        <v>195994.098</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F133" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6">
+      <c r="A134" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C134" s="1">
+        <v>6066323</v>
+      </c>
+      <c r="D134" s="5">
+        <v>186997.68299999999</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F134" s="1" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>